<commit_message>
updating documentation for latest CAB changes
</commit_message>
<xml_diff>
--- a/PIT3/Schema Publication Changelog.xlsx
+++ b/PIT3/Schema Publication Changelog.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owalsh01\IdeaProjects\paye-employers-documentation\src\main\resources\PIT3\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA0D42A-0216-4A09-83D6-3CF7217EE1BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="7425" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14070" windowHeight="7425" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v0.10" sheetId="1" r:id="rId1"/>
@@ -22,15 +23,15 @@
   </definedNames>
   <calcPr calcId="171027"/>
   <customWorkbookViews>
+    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="445">
   <si>
     <t>Document</t>
   </si>
@@ -3201,12 +3202,15 @@
       <t>to be a date and not a datetime</t>
     </r>
   </si>
+  <si>
+    <t>Updated endpoints</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3330,13 +3334,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4094,6 +4091,77 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4139,8 +4207,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -4163,66 +4261,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4244,11 +4282,92 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4256,148 +4375,26 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4428,7 +4425,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -4769,7 +4766,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4802,12 +4799,12 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="130" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="104"/>
-      <c r="C2" s="104"/>
-      <c r="D2" s="105"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="132"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4830,12 +4827,12 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="104"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="105"/>
+      <c r="B4" s="131"/>
+      <c r="C4" s="131"/>
+      <c r="D4" s="132"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -4875,10 +4872,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="106" t="s">
+      <c r="A7" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="109">
+      <c r="B7" s="136">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -4892,8 +4889,8 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="107"/>
-      <c r="B8" s="110"/>
+      <c r="A8" s="134"/>
+      <c r="B8" s="137"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -4905,8 +4902,8 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="107"/>
-      <c r="B9" s="110"/>
+      <c r="A9" s="134"/>
+      <c r="B9" s="137"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -4918,8 +4915,8 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="107"/>
-      <c r="B10" s="110"/>
+      <c r="A10" s="134"/>
+      <c r="B10" s="137"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -4931,8 +4928,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="107"/>
-      <c r="B11" s="110"/>
+      <c r="A11" s="134"/>
+      <c r="B11" s="137"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -4944,8 +4941,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="108"/>
-      <c r="B12" s="111"/>
+      <c r="A12" s="135"/>
+      <c r="B12" s="138"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -4957,10 +4954,10 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="114" t="s">
+      <c r="A13" s="141" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="109">
+      <c r="B13" s="136">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -4974,8 +4971,8 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="115"/>
-      <c r="B14" s="111"/>
+      <c r="A14" s="142"/>
+      <c r="B14" s="138"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -5021,12 +5018,12 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="103" t="s">
+      <c r="A17" s="130" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="104"/>
-      <c r="C17" s="104"/>
-      <c r="D17" s="105"/>
+      <c r="B17" s="131"/>
+      <c r="C17" s="131"/>
+      <c r="D17" s="132"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -5066,21 +5063,21 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="103" t="s">
+      <c r="A20" s="130" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="104"/>
-      <c r="C20" s="104"/>
-      <c r="D20" s="105"/>
+      <c r="B20" s="131"/>
+      <c r="C20" s="131"/>
+      <c r="D20" s="132"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="116" t="s">
+      <c r="A21" s="143" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="113">
+      <c r="B21" s="140">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -5094,8 +5091,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="117"/>
-      <c r="B22" s="111"/>
+      <c r="A22" s="144"/>
+      <c r="B22" s="138"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -5118,18 +5115,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="103" t="s">
+      <c r="A24" s="130" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="104"/>
-      <c r="C24" s="104"/>
-      <c r="D24" s="105"/>
+      <c r="B24" s="131"/>
+      <c r="C24" s="131"/>
+      <c r="D24" s="132"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="112" t="s">
+      <c r="A25" s="139" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="113">
+      <c r="B25" s="140">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -5143,8 +5140,8 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="107"/>
-      <c r="B26" s="110"/>
+      <c r="A26" s="134"/>
+      <c r="B26" s="137"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -5156,8 +5153,8 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="107"/>
-      <c r="B27" s="110"/>
+      <c r="A27" s="134"/>
+      <c r="B27" s="137"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -5169,8 +5166,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="107"/>
-      <c r="B28" s="110"/>
+      <c r="A28" s="134"/>
+      <c r="B28" s="137"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -5182,8 +5179,8 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="107"/>
-      <c r="B29" s="110"/>
+      <c r="A29" s="134"/>
+      <c r="B29" s="137"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -5195,8 +5192,8 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="107"/>
-      <c r="B30" s="110"/>
+      <c r="A30" s="134"/>
+      <c r="B30" s="137"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -5208,8 +5205,8 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="107"/>
-      <c r="B31" s="110"/>
+      <c r="A31" s="134"/>
+      <c r="B31" s="137"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -5221,8 +5218,8 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="108"/>
-      <c r="B32" s="111"/>
+      <c r="A32" s="135"/>
+      <c r="B32" s="138"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -5346,12 +5343,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="103" t="s">
+      <c r="A41" s="130" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="104"/>
-      <c r="C41" s="104"/>
-      <c r="D41" s="105"/>
+      <c r="B41" s="131"/>
+      <c r="C41" s="131"/>
+      <c r="D41" s="132"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -5411,7 +5408,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5421,7 +5418,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -5449,7 +5446,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:XFC79"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -5531,10 +5528,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="133" t="s">
+      <c r="A7" s="145" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="132" t="s">
+      <c r="B7" s="146" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5545,8 +5542,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="133"/>
-      <c r="B8" s="132"/>
+      <c r="A8" s="145"/>
+      <c r="B8" s="146"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5555,8 +5552,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="133"/>
-      <c r="B9" s="132"/>
+      <c r="A9" s="145"/>
+      <c r="B9" s="146"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5565,8 +5562,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="133"/>
-      <c r="B10" s="132"/>
+      <c r="A10" s="145"/>
+      <c r="B10" s="146"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5575,8 +5572,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="133"/>
-      <c r="B11" s="132"/>
+      <c r="A11" s="145"/>
+      <c r="B11" s="146"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5585,8 +5582,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="133"/>
-      <c r="B12" s="132"/>
+      <c r="A12" s="145"/>
+      <c r="B12" s="146"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5595,10 +5592,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="135" t="s">
+      <c r="A13" s="148" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="132" t="s">
+      <c r="B13" s="146" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5609,8 +5606,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="135"/>
-      <c r="B14" s="132"/>
+      <c r="A14" s="148"/>
+      <c r="B14" s="146"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5619,8 +5616,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="135"/>
-      <c r="B15" s="132"/>
+      <c r="A15" s="148"/>
+      <c r="B15" s="146"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5629,10 +5626,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="118" t="s">
+      <c r="A16" s="149" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="127" t="s">
+      <c r="B16" s="150" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5643,8 +5640,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="118"/>
-      <c r="B17" s="127"/>
+      <c r="A17" s="149"/>
+      <c r="B17" s="150"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5653,8 +5650,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="118"/>
-      <c r="B18" s="127"/>
+      <c r="A18" s="149"/>
+      <c r="B18" s="150"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5663,8 +5660,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="118"/>
-      <c r="B19" s="127"/>
+      <c r="A19" s="149"/>
+      <c r="B19" s="150"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5673,8 +5670,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="118"/>
-      <c r="B20" s="127"/>
+      <c r="A20" s="149"/>
+      <c r="B20" s="150"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5683,8 +5680,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="118"/>
-      <c r="B21" s="127"/>
+      <c r="A21" s="149"/>
+      <c r="B21" s="150"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5693,8 +5690,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="118"/>
-      <c r="B22" s="127"/>
+      <c r="A22" s="149"/>
+      <c r="B22" s="150"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5703,8 +5700,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="118"/>
-      <c r="B23" s="127"/>
+      <c r="A23" s="149"/>
+      <c r="B23" s="150"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5713,26 +5710,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="118"/>
-      <c r="B24" s="127"/>
-      <c r="C24" s="118" t="s">
+      <c r="A24" s="149"/>
+      <c r="B24" s="150"/>
+      <c r="C24" s="149" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="119" t="s">
+      <c r="D24" s="156" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="118"/>
-      <c r="B25" s="127"/>
-      <c r="C25" s="118"/>
-      <c r="D25" s="119"/>
+      <c r="A25" s="149"/>
+      <c r="B25" s="150"/>
+      <c r="C25" s="149"/>
+      <c r="D25" s="156"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="133" t="s">
+      <c r="A26" s="145" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="132" t="s">
+      <c r="B26" s="146" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5743,8 +5740,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="133"/>
-      <c r="B27" s="132"/>
+      <c r="A27" s="145"/>
+      <c r="B27" s="146"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5771,28 +5768,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="134" t="s">
+      <c r="A30" s="147" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="132" t="s">
+      <c r="B30" s="146" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="118" t="s">
+      <c r="C30" s="149" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="122" t="s">
+      <c r="D30" s="159" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="134"/>
-      <c r="B31" s="132"/>
-      <c r="C31" s="118"/>
-      <c r="D31" s="122"/>
+      <c r="A31" s="147"/>
+      <c r="B31" s="146"/>
+      <c r="C31" s="149"/>
+      <c r="D31" s="159"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="134"/>
-      <c r="B32" s="132"/>
+      <c r="A32" s="147"/>
+      <c r="B32" s="146"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5801,8 +5798,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="134"/>
-      <c r="B33" s="132"/>
+      <c r="A33" s="147"/>
+      <c r="B33" s="146"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5811,8 +5808,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="134"/>
-      <c r="B34" s="132"/>
+      <c r="A34" s="147"/>
+      <c r="B34" s="146"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5821,8 +5818,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="134"/>
-      <c r="B35" s="132"/>
+      <c r="A35" s="147"/>
+      <c r="B35" s="146"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5831,8 +5828,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="134"/>
-      <c r="B36" s="132"/>
+      <c r="A36" s="147"/>
+      <c r="B36" s="146"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5841,26 +5838,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="134"/>
-      <c r="B37" s="132"/>
-      <c r="C37" s="123" t="s">
+      <c r="A37" s="147"/>
+      <c r="B37" s="146"/>
+      <c r="C37" s="160" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="125" t="s">
+      <c r="D37" s="162" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="134"/>
-      <c r="B38" s="132"/>
-      <c r="C38" s="124"/>
-      <c r="D38" s="125"/>
+      <c r="A38" s="147"/>
+      <c r="B38" s="146"/>
+      <c r="C38" s="161"/>
+      <c r="D38" s="162"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="133" t="s">
+      <c r="A39" s="145" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="132" t="s">
+      <c r="B39" s="146" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -5871,8 +5868,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="133"/>
-      <c r="B40" s="132"/>
+      <c r="A40" s="145"/>
+      <c r="B40" s="146"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -5899,10 +5896,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="134" t="s">
+      <c r="A43" s="147" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="132" t="s">
+      <c r="B43" s="146" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -5911,8 +5908,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="134"/>
-      <c r="B44" s="132"/>
+      <c r="A44" s="147"/>
+      <c r="B44" s="146"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -5921,10 +5918,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="129" t="s">
+      <c r="A45" s="153" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="132" t="s">
+      <c r="B45" s="146" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -5933,8 +5930,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="130"/>
-      <c r="B46" s="132"/>
+      <c r="A46" s="154"/>
+      <c r="B46" s="146"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -5943,8 +5940,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="130"/>
-      <c r="B47" s="132"/>
+      <c r="A47" s="154"/>
+      <c r="B47" s="146"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -5953,8 +5950,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="131"/>
-      <c r="B48" s="132"/>
+      <c r="A48" s="155"/>
+      <c r="B48" s="146"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -5963,10 +5960,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="127" t="s">
+      <c r="A49" s="150" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="127" t="s">
+      <c r="B49" s="150" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -10070,8 +10067,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="127"/>
-      <c r="B50" s="127"/>
+      <c r="A50" s="150"/>
+      <c r="B50" s="150"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -14175,8 +14172,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="127"/>
-      <c r="B51" s="127"/>
+      <c r="A51" s="150"/>
+      <c r="B51" s="150"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -18280,8 +18277,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="127"/>
-      <c r="B52" s="127"/>
+      <c r="A52" s="150"/>
+      <c r="B52" s="150"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -22385,12 +22382,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="127"/>
-      <c r="B53" s="127"/>
-      <c r="C53" s="121" t="s">
+      <c r="A53" s="150"/>
+      <c r="B53" s="150"/>
+      <c r="C53" s="158" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="122" t="s">
+      <c r="D53" s="159" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26490,10 +26487,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="127"/>
-      <c r="B54" s="127"/>
-      <c r="C54" s="121"/>
-      <c r="D54" s="122"/>
+      <c r="A54" s="150"/>
+      <c r="B54" s="150"/>
+      <c r="C54" s="158"/>
+      <c r="D54" s="159"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30611,10 +30608,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="126" t="s">
+      <c r="A57" s="151" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="127" t="s">
+      <c r="B57" s="150" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30625,8 +30622,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="126"/>
-      <c r="B58" s="127"/>
+      <c r="A58" s="151"/>
+      <c r="B58" s="150"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30635,8 +30632,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="126"/>
-      <c r="B59" s="127"/>
+      <c r="A59" s="151"/>
+      <c r="B59" s="150"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30645,8 +30642,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="126"/>
-      <c r="B60" s="127"/>
+      <c r="A60" s="151"/>
+      <c r="B60" s="150"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30655,8 +30652,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="126"/>
-      <c r="B61" s="127"/>
+      <c r="A61" s="151"/>
+      <c r="B61" s="150"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30665,8 +30662,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="126"/>
-      <c r="B62" s="127"/>
+      <c r="A62" s="151"/>
+      <c r="B62" s="150"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30675,8 +30672,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="126"/>
-      <c r="B63" s="127"/>
+      <c r="A63" s="151"/>
+      <c r="B63" s="150"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30685,16 +30682,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="126"/>
-      <c r="B64" s="127"/>
+      <c r="A64" s="151"/>
+      <c r="B64" s="150"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="126"/>
-      <c r="B65" s="127"/>
+      <c r="A65" s="151"/>
+      <c r="B65" s="150"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30703,16 +30700,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="126"/>
-      <c r="B66" s="127"/>
+      <c r="A66" s="151"/>
+      <c r="B66" s="150"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="126"/>
-      <c r="B67" s="127"/>
+      <c r="A67" s="151"/>
+      <c r="B67" s="150"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30721,8 +30718,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="126"/>
-      <c r="B68" s="127"/>
+      <c r="A68" s="151"/>
+      <c r="B68" s="150"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30731,8 +30728,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="126"/>
-      <c r="B69" s="127"/>
+      <c r="A69" s="151"/>
+      <c r="B69" s="150"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30741,8 +30738,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="126"/>
-      <c r="B70" s="127"/>
+      <c r="A70" s="151"/>
+      <c r="B70" s="150"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30751,8 +30748,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="126"/>
-      <c r="B71" s="127"/>
+      <c r="A71" s="151"/>
+      <c r="B71" s="150"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30761,8 +30758,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="126"/>
-      <c r="B72" s="127"/>
+      <c r="A72" s="151"/>
+      <c r="B72" s="150"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30771,16 +30768,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="126"/>
-      <c r="B73" s="127"/>
+      <c r="A73" s="151"/>
+      <c r="B73" s="150"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="126"/>
-      <c r="B74" s="127"/>
+      <c r="A74" s="151"/>
+      <c r="B74" s="150"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30789,18 +30786,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="126"/>
-      <c r="B75" s="127"/>
-      <c r="C75" s="120"/>
-      <c r="D75" s="128" t="s">
+      <c r="A75" s="151"/>
+      <c r="B75" s="150"/>
+      <c r="C75" s="157"/>
+      <c r="D75" s="152" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="126"/>
-      <c r="B76" s="127"/>
-      <c r="C76" s="120"/>
-      <c r="D76" s="128"/>
+      <c r="A76" s="151"/>
+      <c r="B76" s="150"/>
+      <c r="C76" s="157"/>
+      <c r="D76" s="152"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
@@ -30824,8 +30821,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -30834,13 +30831,29 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -30855,22 +30868,6 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -30878,7 +30875,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -30924,10 +30921,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="133" t="s">
+      <c r="A4" s="145" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="132" t="s">
+      <c r="B4" s="146" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -30938,133 +30935,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="133"/>
-      <c r="B5" s="132"/>
-      <c r="C5" s="143" t="s">
+      <c r="A5" s="145"/>
+      <c r="B5" s="146"/>
+      <c r="C5" s="172" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="142" t="s">
+      <c r="D5" s="171" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="133"/>
-      <c r="B6" s="132"/>
-      <c r="C6" s="143"/>
-      <c r="D6" s="142"/>
+      <c r="A6" s="145"/>
+      <c r="B6" s="146"/>
+      <c r="C6" s="172"/>
+      <c r="D6" s="171"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="133"/>
-      <c r="B7" s="132"/>
+      <c r="A7" s="145"/>
+      <c r="B7" s="146"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="133"/>
-      <c r="B8" s="132"/>
+      <c r="A8" s="145"/>
+      <c r="B8" s="146"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="133"/>
-      <c r="B9" s="132"/>
+      <c r="A9" s="145"/>
+      <c r="B9" s="146"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="135" t="s">
+      <c r="A10" s="148" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="132" t="s">
+      <c r="B10" s="146" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="145"/>
-      <c r="D10" s="142" t="s">
+      <c r="C10" s="170"/>
+      <c r="D10" s="171" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="135"/>
-      <c r="B11" s="132"/>
-      <c r="C11" s="145"/>
-      <c r="D11" s="142"/>
+      <c r="A11" s="148"/>
+      <c r="B11" s="146"/>
+      <c r="C11" s="170"/>
+      <c r="D11" s="171"/>
     </row>
     <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="135"/>
-      <c r="B12" s="132"/>
-      <c r="C12" s="145"/>
-      <c r="D12" s="142"/>
+      <c r="A12" s="148"/>
+      <c r="B12" s="146"/>
+      <c r="C12" s="170"/>
+      <c r="D12" s="171"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="118" t="s">
+      <c r="A13" s="149" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="127" t="s">
+      <c r="B13" s="150" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="144"/>
-      <c r="D13" s="142" t="s">
+      <c r="C13" s="173"/>
+      <c r="D13" s="171" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="118"/>
-      <c r="B14" s="127"/>
-      <c r="C14" s="144"/>
-      <c r="D14" s="142"/>
+      <c r="A14" s="149"/>
+      <c r="B14" s="150"/>
+      <c r="C14" s="173"/>
+      <c r="D14" s="171"/>
     </row>
     <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="118"/>
-      <c r="B15" s="127"/>
-      <c r="C15" s="144"/>
+      <c r="A15" s="149"/>
+      <c r="B15" s="150"/>
+      <c r="C15" s="173"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="118"/>
-      <c r="B16" s="127"/>
-      <c r="C16" s="144"/>
+      <c r="A16" s="149"/>
+      <c r="B16" s="150"/>
+      <c r="C16" s="173"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="118"/>
-      <c r="B17" s="127"/>
-      <c r="C17" s="144"/>
+      <c r="A17" s="149"/>
+      <c r="B17" s="150"/>
+      <c r="C17" s="173"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="118"/>
-      <c r="B18" s="127"/>
-      <c r="C18" s="144"/>
+      <c r="A18" s="149"/>
+      <c r="B18" s="150"/>
+      <c r="C18" s="173"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="118"/>
-      <c r="B19" s="127"/>
-      <c r="C19" s="144"/>
+      <c r="A19" s="149"/>
+      <c r="B19" s="150"/>
+      <c r="C19" s="173"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="118"/>
-      <c r="B20" s="127"/>
-      <c r="C20" s="144"/>
+      <c r="A20" s="149"/>
+      <c r="B20" s="150"/>
+      <c r="C20" s="173"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="118"/>
-      <c r="B21" s="127"/>
-      <c r="C21" s="144"/>
+      <c r="A21" s="149"/>
+      <c r="B21" s="150"/>
+      <c r="C21" s="173"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="118"/>
-      <c r="B22" s="127"/>
-      <c r="C22" s="144"/>
+      <c r="A22" s="149"/>
+      <c r="B22" s="150"/>
+      <c r="C22" s="173"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="118"/>
-      <c r="B23" s="127"/>
-      <c r="C23" s="144"/>
+      <c r="A23" s="149"/>
+      <c r="B23" s="150"/>
+      <c r="C23" s="173"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -31162,10 +31159,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="136" t="s">
+      <c r="A32" s="174" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="139" t="s">
+      <c r="B32" s="177" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -31176,26 +31173,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="137"/>
-      <c r="B33" s="140"/>
+      <c r="A33" s="175"/>
+      <c r="B33" s="178"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="137"/>
-      <c r="B34" s="140"/>
+      <c r="A34" s="175"/>
+      <c r="B34" s="178"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="137"/>
-      <c r="B35" s="140"/>
+      <c r="A35" s="175"/>
+      <c r="B35" s="178"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="138"/>
-      <c r="B36" s="141"/>
+      <c r="A36" s="176"/>
+      <c r="B36" s="179"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -31224,10 +31221,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="134" t="s">
+      <c r="A39" s="147" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="132" t="s">
+      <c r="B39" s="146" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -31238,8 +31235,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="134"/>
-      <c r="B40" s="132"/>
+      <c r="A40" s="147"/>
+      <c r="B40" s="146"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -31248,84 +31245,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="133" t="s">
+      <c r="A41" s="145" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="132" t="s">
+      <c r="B41" s="146" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="145" t="s">
+      <c r="C41" s="170" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="118" t="s">
+      <c r="D41" s="149" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="133"/>
-      <c r="B42" s="132"/>
-      <c r="C42" s="145"/>
-      <c r="D42" s="118"/>
+      <c r="A42" s="145"/>
+      <c r="B42" s="146"/>
+      <c r="C42" s="170"/>
+      <c r="D42" s="149"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="133"/>
-      <c r="B43" s="132"/>
-      <c r="C43" s="145" t="s">
+      <c r="A43" s="145"/>
+      <c r="B43" s="146"/>
+      <c r="C43" s="170" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="128" t="s">
+      <c r="D43" s="152" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="133"/>
-      <c r="B44" s="132"/>
-      <c r="C44" s="145"/>
-      <c r="D44" s="128"/>
+      <c r="A44" s="145"/>
+      <c r="B44" s="146"/>
+      <c r="C44" s="170"/>
+      <c r="D44" s="152"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="126" t="s">
+      <c r="A45" s="151" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="127" t="s">
+      <c r="B45" s="150" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="149"/>
+      <c r="C45" s="166"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="126"/>
-      <c r="B46" s="127"/>
-      <c r="C46" s="150"/>
-      <c r="D46" s="146" t="s">
+      <c r="A46" s="151"/>
+      <c r="B46" s="150"/>
+      <c r="C46" s="167"/>
+      <c r="D46" s="163" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="126"/>
-      <c r="B47" s="127"/>
-      <c r="C47" s="150"/>
-      <c r="D47" s="147"/>
+      <c r="A47" s="151"/>
+      <c r="B47" s="150"/>
+      <c r="C47" s="167"/>
+      <c r="D47" s="164"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="126"/>
-      <c r="B48" s="127"/>
-      <c r="C48" s="151"/>
-      <c r="D48" s="147"/>
+      <c r="A48" s="151"/>
+      <c r="B48" s="150"/>
+      <c r="C48" s="168"/>
+      <c r="D48" s="164"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="126"/>
-      <c r="B49" s="127"/>
-      <c r="C49" s="121"/>
-      <c r="D49" s="147"/>
+      <c r="A49" s="151"/>
+      <c r="B49" s="150"/>
+      <c r="C49" s="158"/>
+      <c r="D49" s="164"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="126"/>
-      <c r="B50" s="127"/>
-      <c r="C50" s="121"/>
-      <c r="D50" s="148"/>
+      <c r="A50" s="151"/>
+      <c r="B50" s="150"/>
+      <c r="C50" s="158"/>
+      <c r="D50" s="165"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -31348,10 +31345,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="127" t="s">
+      <c r="A53" s="150" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="127" t="s">
+      <c r="B53" s="150" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -31362,8 +31359,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="127"/>
-      <c r="B54" s="127"/>
+      <c r="A54" s="150"/>
+      <c r="B54" s="150"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -31372,8 +31369,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="127"/>
-      <c r="B55" s="127"/>
+      <c r="A55" s="150"/>
+      <c r="B55" s="150"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -31382,9 +31379,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="127"/>
-      <c r="B56" s="127"/>
-      <c r="C56" s="152" t="s">
+      <c r="A56" s="150"/>
+      <c r="B56" s="150"/>
+      <c r="C56" s="169" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -31392,16 +31389,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="127"/>
-      <c r="B57" s="127"/>
-      <c r="C57" s="152"/>
+      <c r="A57" s="150"/>
+      <c r="B57" s="150"/>
+      <c r="C57" s="169"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="127"/>
-      <c r="B58" s="127"/>
+      <c r="A58" s="150"/>
+      <c r="B58" s="150"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -31410,8 +31407,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="127"/>
-      <c r="B59" s="127"/>
+      <c r="A59" s="150"/>
+      <c r="B59" s="150"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -31420,9 +31417,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="127"/>
-      <c r="B60" s="127"/>
-      <c r="C60" s="152" t="s">
+      <c r="A60" s="150"/>
+      <c r="B60" s="150"/>
+      <c r="C60" s="169" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31430,25 +31427,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="127"/>
-      <c r="B61" s="127"/>
-      <c r="C61" s="152"/>
+      <c r="A61" s="150"/>
+      <c r="B61" s="150"/>
+      <c r="C61" s="169"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="127"/>
-      <c r="B62" s="127"/>
-      <c r="C62" s="152"/>
+      <c r="A62" s="150"/>
+      <c r="B62" s="150"/>
+      <c r="C62" s="169"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="127"/>
-      <c r="B63" s="127"/>
-      <c r="C63" s="145" t="s">
+      <c r="A63" s="150"/>
+      <c r="B63" s="150"/>
+      <c r="C63" s="170" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -31456,30 +31453,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="127"/>
-      <c r="B64" s="127"/>
-      <c r="C64" s="145"/>
-      <c r="D64" s="128" t="s">
+      <c r="A64" s="150"/>
+      <c r="B64" s="150"/>
+      <c r="C64" s="170"/>
+      <c r="D64" s="152" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="127"/>
-      <c r="B65" s="127"/>
-      <c r="C65" s="145"/>
-      <c r="D65" s="128"/>
+      <c r="A65" s="150"/>
+      <c r="B65" s="150"/>
+      <c r="C65" s="170"/>
+      <c r="D65" s="152"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="127"/>
-      <c r="B66" s="127"/>
-      <c r="C66" s="145"/>
-      <c r="D66" s="128"/>
+      <c r="A66" s="150"/>
+      <c r="B66" s="150"/>
+      <c r="C66" s="170"/>
+      <c r="D66" s="152"/>
     </row>
     <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="127"/>
-      <c r="B67" s="127"/>
-      <c r="C67" s="145"/>
-      <c r="D67" s="128"/>
+      <c r="A67" s="150"/>
+      <c r="B67" s="150"/>
+      <c r="C67" s="170"/>
+      <c r="D67" s="152"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
@@ -31535,6 +31532,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
@@ -31551,23 +31565,6 @@
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C63:C67"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31575,11 +31572,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D165"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B8"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31605,30 +31602,30 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="160" t="s">
+      <c r="A2" s="103" t="s">
         <v>433</v>
       </c>
-      <c r="B2" s="160"/>
-      <c r="C2" s="160"/>
-      <c r="D2" s="161"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="104"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="206" t="s">
+      <c r="A3" s="182" t="s">
         <v>434</v>
       </c>
-      <c r="B3" s="158" t="s">
+      <c r="B3" s="180" t="s">
         <v>435</v>
       </c>
       <c r="C3" s="101" t="s">
         <v>436</v>
       </c>
-      <c r="D3" s="162" t="s">
+      <c r="D3" s="105" t="s">
         <v>437</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="207"/>
-      <c r="B4" s="159"/>
+      <c r="A4" s="183"/>
+      <c r="B4" s="181"/>
       <c r="C4" s="100" t="s">
         <v>438</v>
       </c>
@@ -31637,18 +31634,18 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="160" t="s">
+      <c r="A5" s="103" t="s">
         <v>336</v>
       </c>
-      <c r="B5" s="160"/>
-      <c r="C5" s="160"/>
-      <c r="D5" s="161"/>
+      <c r="B5" s="103"/>
+      <c r="C5" s="103"/>
+      <c r="D5" s="104"/>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="155" t="s">
+      <c r="A6" s="199" t="s">
         <v>337</v>
       </c>
-      <c r="B6" s="156" t="s">
+      <c r="B6" s="200" t="s">
         <v>432</v>
       </c>
       <c r="C6" s="100" t="s">
@@ -31659,57 +31656,57 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="155"/>
-      <c r="B7" s="156"/>
+      <c r="A7" s="199"/>
+      <c r="B7" s="200"/>
       <c r="C7" s="100" t="s">
         <v>342</v>
       </c>
-      <c r="D7" s="163" t="s">
+      <c r="D7" s="106" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="155"/>
-      <c r="B8" s="156"/>
+      <c r="A8" s="199"/>
+      <c r="B8" s="200"/>
       <c r="C8" s="100" t="s">
         <v>338</v>
       </c>
-      <c r="D8" s="163" t="s">
+      <c r="D8" s="106" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="160" t="s">
+      <c r="A9" s="103" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="160"/>
-      <c r="C9" s="160"/>
-      <c r="D9" s="161"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="103"/>
+      <c r="D9" s="104"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="164" t="s">
+      <c r="A10" s="195" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="165" t="s">
+      <c r="B10" s="196" t="s">
         <v>432</v>
       </c>
-      <c r="C10" s="163"/>
-      <c r="D10" s="163" t="s">
+      <c r="C10" s="106"/>
+      <c r="D10" s="106" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="164"/>
-      <c r="B11" s="165"/>
+      <c r="A11" s="195"/>
+      <c r="B11" s="196"/>
       <c r="C11" s="70" t="s">
         <v>234</v>
       </c>
-      <c r="D11" s="166" t="s">
+      <c r="D11" s="107" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="167" t="s">
+      <c r="A12" s="108" t="s">
         <v>74</v>
       </c>
       <c r="B12" s="70" t="s">
@@ -31718,12 +31715,12 @@
       <c r="C12" s="70" t="s">
         <v>234</v>
       </c>
-      <c r="D12" s="168" t="s">
+      <c r="D12" s="109" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="167" t="s">
+      <c r="A13" s="108" t="s">
         <v>253</v>
       </c>
       <c r="B13" s="70" t="s">
@@ -31732,12 +31729,12 @@
       <c r="C13" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="168" t="s">
+      <c r="D13" s="109" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="167" t="s">
+      <c r="A14" s="108" t="s">
         <v>372</v>
       </c>
       <c r="B14" s="70" t="s">
@@ -31746,339 +31743,339 @@
       <c r="C14" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="168" t="s">
+      <c r="D14" s="109" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="167" t="s">
+      <c r="A15" s="108" t="s">
         <v>402</v>
       </c>
       <c r="B15" s="70" t="s">
         <v>432</v>
       </c>
       <c r="C15" s="70"/>
-      <c r="D15" s="168" t="s">
+      <c r="D15" s="109" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="164" t="s">
+      <c r="A16" s="195" t="s">
         <v>270</v>
       </c>
-      <c r="B16" s="165" t="s">
+      <c r="B16" s="196" t="s">
         <v>432</v>
       </c>
-      <c r="C16" s="163"/>
+      <c r="C16" s="106"/>
       <c r="D16" s="80" t="s">
         <v>441</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="164"/>
-      <c r="B17" s="165"/>
-      <c r="C17" s="163"/>
-      <c r="D17" s="163" t="s">
+      <c r="A17" s="195"/>
+      <c r="B17" s="196"/>
+      <c r="C17" s="106"/>
+      <c r="D17" s="106" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="164"/>
-      <c r="B18" s="165"/>
-      <c r="C18" s="169" t="s">
+      <c r="A18" s="195"/>
+      <c r="B18" s="196"/>
+      <c r="C18" s="110" t="s">
         <v>320</v>
       </c>
-      <c r="D18" s="163" t="s">
+      <c r="D18" s="106" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="164"/>
-      <c r="B19" s="165"/>
-      <c r="C19" s="170" t="s">
+      <c r="A19" s="195"/>
+      <c r="B19" s="196"/>
+      <c r="C19" s="111" t="s">
         <v>399</v>
       </c>
-      <c r="D19" s="171" t="s">
+      <c r="D19" s="112" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="167" t="s">
+      <c r="A20" s="108" t="s">
         <v>285</v>
       </c>
       <c r="B20" s="70" t="s">
         <v>432</v>
       </c>
-      <c r="C20" s="170" t="s">
+      <c r="C20" s="111" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="163"/>
+      <c r="D20" s="106"/>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="172" t="s">
+      <c r="A21" s="201" t="s">
         <v>165</v>
       </c>
-      <c r="B21" s="173" t="s">
+      <c r="B21" s="186" t="s">
         <v>432</v>
       </c>
-      <c r="C21" s="163"/>
-      <c r="D21" s="174" t="s">
+      <c r="C21" s="106"/>
+      <c r="D21" s="113" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="175"/>
-      <c r="B22" s="176"/>
-      <c r="C22" s="170" t="s">
+      <c r="A22" s="202"/>
+      <c r="B22" s="191"/>
+      <c r="C22" s="111" t="s">
         <v>356</v>
       </c>
-      <c r="D22" s="163" t="s">
+      <c r="D22" s="106" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="175"/>
-      <c r="B23" s="176"/>
-      <c r="C23" s="170" t="s">
+      <c r="A23" s="202"/>
+      <c r="B23" s="191"/>
+      <c r="C23" s="111" t="s">
         <v>354</v>
       </c>
-      <c r="D23" s="163" t="s">
+      <c r="D23" s="106" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="175"/>
-      <c r="B24" s="176"/>
-      <c r="C24" s="177" t="s">
+      <c r="A24" s="202"/>
+      <c r="B24" s="191"/>
+      <c r="C24" s="114" t="s">
         <v>362</v>
       </c>
-      <c r="D24" s="171" t="s">
+      <c r="D24" s="112" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="175"/>
-      <c r="B25" s="176"/>
-      <c r="C25" s="170" t="s">
+      <c r="A25" s="202"/>
+      <c r="B25" s="191"/>
+      <c r="C25" s="111" t="s">
         <v>354</v>
       </c>
-      <c r="D25" s="171" t="s">
+      <c r="D25" s="112" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="175"/>
-      <c r="B26" s="176"/>
-      <c r="C26" s="170" t="s">
+      <c r="A26" s="202"/>
+      <c r="B26" s="191"/>
+      <c r="C26" s="111" t="s">
         <v>366</v>
       </c>
-      <c r="D26" s="171" t="s">
+      <c r="D26" s="112" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="178"/>
-      <c r="B27" s="179"/>
-      <c r="C27" s="170" t="s">
+      <c r="A27" s="203"/>
+      <c r="B27" s="187"/>
+      <c r="C27" s="111" t="s">
         <v>354</v>
       </c>
-      <c r="D27" s="171" t="s">
+      <c r="D27" s="112" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="180" t="s">
+      <c r="A28" s="115" t="s">
         <v>326</v>
       </c>
       <c r="B28" s="70" t="s">
         <v>432</v>
       </c>
-      <c r="C28" s="170" t="s">
+      <c r="C28" s="111" t="s">
         <v>327</v>
       </c>
-      <c r="D28" s="171" t="s">
+      <c r="D28" s="112" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="180" t="s">
+      <c r="A29" s="115" t="s">
         <v>346</v>
       </c>
       <c r="B29" s="70" t="s">
         <v>432</v>
       </c>
-      <c r="C29" s="170" t="s">
+      <c r="C29" s="111" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="171"/>
+      <c r="D29" s="112"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="181" t="s">
+      <c r="A30" s="197" t="s">
         <v>364</v>
       </c>
-      <c r="B30" s="173" t="s">
+      <c r="B30" s="186" t="s">
         <v>432</v>
       </c>
-      <c r="C30" s="170" t="s">
+      <c r="C30" s="111" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="171"/>
+      <c r="D30" s="112"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="182"/>
-      <c r="B31" s="179"/>
-      <c r="C31" s="170" t="s">
+      <c r="A31" s="204"/>
+      <c r="B31" s="187"/>
+      <c r="C31" s="111" t="s">
         <v>399</v>
       </c>
-      <c r="D31" s="171" t="s">
+      <c r="D31" s="112" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="160" t="s">
+      <c r="A32" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="160"/>
-      <c r="C32" s="160"/>
-      <c r="D32" s="160"/>
+      <c r="B32" s="103"/>
+      <c r="C32" s="103"/>
+      <c r="D32" s="103"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="181" t="s">
+      <c r="A33" s="197" t="s">
         <v>236</v>
       </c>
-      <c r="B33" s="173" t="s">
+      <c r="B33" s="186" t="s">
         <v>432</v>
       </c>
-      <c r="C33" s="163"/>
-      <c r="D33" s="163" t="s">
+      <c r="C33" s="106"/>
+      <c r="D33" s="106" t="s">
         <v>442</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="183"/>
-      <c r="B34" s="176"/>
-      <c r="C34" s="163"/>
-      <c r="D34" s="163" t="s">
+      <c r="A34" s="198"/>
+      <c r="B34" s="191"/>
+      <c r="C34" s="106"/>
+      <c r="D34" s="106" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="183"/>
-      <c r="B35" s="176"/>
-      <c r="C35" s="163"/>
-      <c r="D35" s="163" t="s">
+      <c r="A35" s="198"/>
+      <c r="B35" s="191"/>
+      <c r="C35" s="106"/>
+      <c r="D35" s="106" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="183"/>
-      <c r="B36" s="176"/>
-      <c r="C36" s="163" t="s">
+      <c r="A36" s="198"/>
+      <c r="B36" s="191"/>
+      <c r="C36" s="106" t="s">
         <v>295</v>
       </c>
-      <c r="D36" s="163" t="s">
+      <c r="D36" s="106" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="183"/>
-      <c r="B37" s="176"/>
-      <c r="C37" s="163" t="s">
+      <c r="A37" s="198"/>
+      <c r="B37" s="191"/>
+      <c r="C37" s="106" t="s">
         <v>323</v>
       </c>
-      <c r="D37" s="171" t="s">
+      <c r="D37" s="112" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="182"/>
-      <c r="B38" s="179"/>
-      <c r="C38" s="163" t="s">
+      <c r="A38" s="204"/>
+      <c r="B38" s="187"/>
+      <c r="C38" s="106" t="s">
         <v>368</v>
       </c>
-      <c r="D38" s="171" t="s">
+      <c r="D38" s="112" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="184" t="s">
+      <c r="A39" s="192" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="173" t="s">
+      <c r="B39" s="186" t="s">
         <v>432</v>
       </c>
-      <c r="C39" s="163" t="s">
+      <c r="C39" s="106" t="s">
         <v>298</v>
       </c>
-      <c r="D39" s="171" t="s">
+      <c r="D39" s="112" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="185"/>
-      <c r="B40" s="176"/>
-      <c r="C40" s="163"/>
-      <c r="D40" s="163" t="s">
+      <c r="A40" s="193"/>
+      <c r="B40" s="191"/>
+      <c r="C40" s="106"/>
+      <c r="D40" s="106" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="185"/>
-      <c r="B41" s="176"/>
-      <c r="C41" s="186" t="s">
+      <c r="A41" s="193"/>
+      <c r="B41" s="191"/>
+      <c r="C41" s="116" t="s">
         <v>324</v>
       </c>
-      <c r="D41" s="171" t="s">
+      <c r="D41" s="112" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="185"/>
-      <c r="B42" s="176"/>
-      <c r="C42" s="186" t="s">
+      <c r="A42" s="193"/>
+      <c r="B42" s="191"/>
+      <c r="C42" s="116" t="s">
         <v>354</v>
       </c>
-      <c r="D42" s="171" t="s">
+      <c r="D42" s="112" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="185"/>
-      <c r="B43" s="176"/>
-      <c r="C43" s="186" t="s">
+      <c r="A43" s="193"/>
+      <c r="B43" s="191"/>
+      <c r="C43" s="116" t="s">
         <v>362</v>
       </c>
-      <c r="D43" s="171" t="s">
+      <c r="D43" s="112" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="185"/>
-      <c r="B44" s="176"/>
-      <c r="C44" s="186" t="s">
+      <c r="A44" s="193"/>
+      <c r="B44" s="191"/>
+      <c r="C44" s="116" t="s">
         <v>366</v>
       </c>
-      <c r="D44" s="171" t="s">
+      <c r="D44" s="112" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="185"/>
-      <c r="B45" s="176"/>
-      <c r="C45" s="186" t="s">
+      <c r="A45" s="193"/>
+      <c r="B45" s="191"/>
+      <c r="C45" s="116" t="s">
         <v>376</v>
       </c>
-      <c r="D45" s="187" t="s">
+      <c r="D45" s="117" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="188"/>
-      <c r="B46" s="179"/>
-      <c r="C46" s="167" t="s">
+      <c r="A46" s="194"/>
+      <c r="B46" s="187"/>
+      <c r="C46" s="108" t="s">
         <v>354</v>
       </c>
-      <c r="D46" s="171" t="s">
+      <c r="D46" s="112" t="s">
         <v>400</v>
       </c>
     </row>
@@ -32086,10 +32083,10 @@
       <c r="A47" s="189" t="s">
         <v>222</v>
       </c>
-      <c r="B47" s="173" t="s">
+      <c r="B47" s="186" t="s">
         <v>432</v>
       </c>
-      <c r="C47" s="153" t="s">
+      <c r="C47" s="206" t="s">
         <v>238</v>
       </c>
       <c r="D47" s="96" t="s">
@@ -32098,1239 +32095,1265 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="190"/>
-      <c r="B48" s="176"/>
-      <c r="C48" s="154"/>
-      <c r="D48" s="171" t="s">
+      <c r="B48" s="191"/>
+      <c r="C48" s="207"/>
+      <c r="D48" s="112" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="190"/>
-      <c r="B49" s="176"/>
-      <c r="C49" s="157" t="s">
+      <c r="B49" s="191"/>
+      <c r="C49" s="188" t="s">
         <v>239</v>
       </c>
-      <c r="D49" s="163" t="s">
+      <c r="D49" s="106" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="190"/>
-      <c r="B50" s="176"/>
-      <c r="C50" s="157"/>
-      <c r="D50" s="191" t="s">
+      <c r="B50" s="191"/>
+      <c r="C50" s="188"/>
+      <c r="D50" s="118" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="190"/>
-      <c r="B51" s="176"/>
-      <c r="C51" s="170" t="s">
+      <c r="B51" s="191"/>
+      <c r="C51" s="111" t="s">
         <v>302</v>
       </c>
-      <c r="D51" s="163" t="s">
+      <c r="D51" s="106" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="190"/>
-      <c r="B52" s="176"/>
-      <c r="C52" s="170">
+      <c r="B52" s="191"/>
+      <c r="C52" s="111">
         <v>2.1</v>
       </c>
-      <c r="D52" s="163" t="s">
+      <c r="D52" s="106" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="190"/>
-      <c r="B53" s="176"/>
-      <c r="C53" s="170" t="s">
+      <c r="B53" s="191"/>
+      <c r="C53" s="111" t="s">
         <v>238</v>
       </c>
-      <c r="D53" s="163" t="s">
+      <c r="D53" s="106" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="190"/>
-      <c r="B54" s="176"/>
-      <c r="C54" s="170" t="s">
+      <c r="B54" s="191"/>
+      <c r="C54" s="111" t="s">
         <v>238</v>
       </c>
-      <c r="D54" s="187" t="s">
+      <c r="D54" s="117" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="190"/>
-      <c r="B55" s="176"/>
-      <c r="C55" s="170" t="s">
+      <c r="B55" s="191"/>
+      <c r="C55" s="111" t="s">
         <v>238</v>
       </c>
-      <c r="D55" s="171" t="s">
+      <c r="D55" s="112" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="190"/>
-      <c r="B56" s="176"/>
-      <c r="C56" s="192" t="s">
+      <c r="B56" s="191"/>
+      <c r="C56" s="119" t="s">
         <v>373</v>
       </c>
-      <c r="D56" s="193" t="s">
+      <c r="D56" s="120" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="190"/>
-      <c r="B57" s="176"/>
-      <c r="C57" s="170">
+      <c r="B57" s="191"/>
+      <c r="C57" s="111">
         <v>2.1</v>
       </c>
-      <c r="D57" s="163" t="s">
+      <c r="D57" s="106" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="190"/>
-      <c r="B58" s="176"/>
-      <c r="C58" s="170" t="s">
+      <c r="B58" s="191"/>
+      <c r="C58" s="111" t="s">
         <v>238</v>
       </c>
-      <c r="D58" s="163" t="s">
+      <c r="D58" s="106" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="190"/>
-      <c r="B59" s="176"/>
-      <c r="C59" s="170" t="s">
+      <c r="B59" s="191"/>
+      <c r="C59" s="111" t="s">
         <v>238</v>
       </c>
-      <c r="D59" s="163" t="s">
+      <c r="D59" s="106" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="184" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="190"/>
+      <c r="B60" s="191"/>
+      <c r="C60" s="111">
+        <v>2.1</v>
+      </c>
+      <c r="D60" s="106" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="192" t="s">
         <v>291</v>
       </c>
-      <c r="B60" s="173" t="s">
+      <c r="B61" s="186" t="s">
         <v>432</v>
       </c>
-      <c r="C60" s="163" t="s">
+      <c r="C61" s="106" t="s">
         <v>292</v>
       </c>
-      <c r="D60" s="163" t="s">
+      <c r="D61" s="106" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="185"/>
-      <c r="B61" s="176"/>
-      <c r="C61" s="191" t="s">
+    <row r="62" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62" s="193"/>
+      <c r="B62" s="191"/>
+      <c r="C62" s="118" t="s">
         <v>276</v>
       </c>
-      <c r="D61" s="163" t="s">
+      <c r="D62" s="106" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="188"/>
-      <c r="B62" s="179"/>
-      <c r="C62" s="163" t="s">
+    <row r="63" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="194"/>
+      <c r="B63" s="187"/>
+      <c r="C63" s="106" t="s">
         <v>345</v>
       </c>
-      <c r="D62" s="163" t="s">
+      <c r="D63" s="106" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="181" t="s">
+    <row r="64" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="197" t="s">
         <v>365</v>
       </c>
-      <c r="B63" s="173" t="s">
+      <c r="B64" s="186" t="s">
         <v>432</v>
       </c>
-      <c r="C63" s="170" t="s">
+      <c r="C64" s="111" t="s">
         <v>30</v>
       </c>
-      <c r="D63" s="163"/>
-    </row>
-    <row r="64" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="183"/>
-      <c r="B64" s="176"/>
-      <c r="C64" s="170" t="s">
+      <c r="D64" s="106"/>
+    </row>
+    <row r="65" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="198"/>
+      <c r="B65" s="191"/>
+      <c r="C65" s="111" t="s">
         <v>373</v>
       </c>
-      <c r="D64" s="163" t="s">
+      <c r="D65" s="106" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="183"/>
-      <c r="B65" s="176"/>
-      <c r="C65" s="170">
+    <row r="66" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="198"/>
+      <c r="B66" s="191"/>
+      <c r="C66" s="111">
         <v>2.1</v>
       </c>
-      <c r="D65" s="163" t="s">
+      <c r="D66" s="106" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="183"/>
-      <c r="B66" s="176"/>
-      <c r="C66" s="170" t="s">
+    <row r="67" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="198"/>
+      <c r="B67" s="191"/>
+      <c r="C67" s="111" t="s">
         <v>239</v>
       </c>
-      <c r="D66" s="163" t="s">
+      <c r="D67" s="106" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="183"/>
-      <c r="B67" s="176"/>
-      <c r="C67" s="170" t="s">
+    <row r="68" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="198"/>
+      <c r="B68" s="191"/>
+      <c r="C68" s="111" t="s">
         <v>238</v>
       </c>
-      <c r="D67" s="163" t="s">
+      <c r="D68" s="106" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="160" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="B68" s="160"/>
-      <c r="C68" s="160"/>
-      <c r="D68" s="161"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="167" t="s">
+      <c r="B69" s="103"/>
+      <c r="C69" s="103"/>
+      <c r="D69" s="104"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="108" t="s">
         <v>378</v>
       </c>
-      <c r="B69" s="170" t="s">
+      <c r="B70" s="111" t="s">
         <v>432</v>
       </c>
-      <c r="C69" s="170" t="s">
+      <c r="C70" s="111" t="s">
         <v>379</v>
       </c>
-      <c r="D69" s="171"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="189" t="s">
+      <c r="D70" s="112"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="189" t="s">
         <v>256</v>
       </c>
-      <c r="B70" s="173" t="s">
+      <c r="B71" s="186" t="s">
         <v>432</v>
       </c>
-      <c r="C70" s="163"/>
-      <c r="D70" s="80" t="s">
+      <c r="C71" s="106"/>
+      <c r="D71" s="80" t="s">
         <v>441</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="190"/>
-      <c r="B71" s="176"/>
-      <c r="C71" s="163"/>
-      <c r="D71" s="163" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="190"/>
-      <c r="B72" s="176"/>
-      <c r="C72" s="163"/>
-      <c r="D72" s="171" t="s">
-        <v>382</v>
+      <c r="B72" s="191"/>
+      <c r="C72" s="106"/>
+      <c r="D72" s="106" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="190"/>
-      <c r="B73" s="176"/>
-      <c r="C73" s="163" t="s">
-        <v>419</v>
-      </c>
-      <c r="D73" s="171" t="s">
-        <v>420</v>
+      <c r="B73" s="191"/>
+      <c r="C73" s="106"/>
+      <c r="D73" s="112" t="s">
+        <v>382</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="190"/>
-      <c r="B74" s="176"/>
-      <c r="C74" s="163" t="s">
+      <c r="B74" s="191"/>
+      <c r="C74" s="106" t="s">
+        <v>419</v>
+      </c>
+      <c r="D74" s="112" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="190"/>
+      <c r="B75" s="191"/>
+      <c r="C75" s="106" t="s">
         <v>424</v>
       </c>
-      <c r="D74" s="171" t="s">
+      <c r="D75" s="112" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="164" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="195" t="s">
         <v>329</v>
       </c>
-      <c r="B75" s="165" t="s">
+      <c r="B76" s="196" t="s">
         <v>432</v>
       </c>
-      <c r="C75" s="80" t="s">
+      <c r="C76" s="80" t="s">
         <v>330</v>
       </c>
-      <c r="D75" s="171" t="s">
+      <c r="D76" s="112" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="164"/>
-      <c r="B76" s="165"/>
-      <c r="C76" s="163" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="195"/>
+      <c r="B77" s="196"/>
+      <c r="C77" s="106" t="s">
         <v>406</v>
       </c>
-      <c r="D76" s="163" t="s">
+      <c r="D77" s="106" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A77" s="164"/>
-      <c r="B77" s="165"/>
-      <c r="C77" s="194" t="s">
+    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="195"/>
+      <c r="B78" s="196"/>
+      <c r="C78" s="121" t="s">
         <v>409</v>
       </c>
-      <c r="D77" s="181" t="s">
+      <c r="D78" s="197" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="164"/>
-      <c r="B78" s="165"/>
-      <c r="C78" s="194" t="s">
+    <row r="79" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="195"/>
+      <c r="B79" s="196"/>
+      <c r="C79" s="121" t="s">
         <v>410</v>
       </c>
-      <c r="D78" s="183"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="164"/>
-      <c r="B79" s="165"/>
-      <c r="C79" s="194" t="s">
+      <c r="D79" s="198"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="195"/>
+      <c r="B80" s="196"/>
+      <c r="C80" s="121" t="s">
         <v>411</v>
       </c>
-      <c r="D79" s="183"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="164"/>
-      <c r="B80" s="165"/>
-      <c r="C80" s="194" t="s">
+      <c r="D80" s="198"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="195"/>
+      <c r="B81" s="196"/>
+      <c r="C81" s="121" t="s">
         <v>412</v>
       </c>
-      <c r="D80" s="182"/>
-    </row>
-    <row r="81" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="167" t="s">
+      <c r="D81" s="204"/>
+    </row>
+    <row r="82" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="108" t="s">
         <v>242</v>
       </c>
-      <c r="B81" s="170" t="s">
+      <c r="B82" s="111" t="s">
         <v>432</v>
       </c>
-      <c r="C81" s="70" t="s">
+      <c r="C82" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="D81" s="168" t="s">
+      <c r="D82" s="109" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="184" t="s">
+    <row r="83" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="192" t="s">
         <v>32</v>
       </c>
-      <c r="B82" s="173" t="s">
+      <c r="B83" s="186" t="s">
         <v>432</v>
       </c>
-      <c r="C82" s="163" t="s">
+      <c r="C83" s="106" t="s">
         <v>263</v>
       </c>
-      <c r="D82" s="163" t="s">
+      <c r="D83" s="106" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="185"/>
-      <c r="B83" s="176"/>
-      <c r="C83" s="163" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="193"/>
+      <c r="B84" s="191"/>
+      <c r="C84" s="106" t="s">
         <v>265</v>
       </c>
-      <c r="D83" s="163" t="s">
+      <c r="D84" s="106" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="185"/>
-      <c r="B84" s="176"/>
-      <c r="C84" s="163" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="193"/>
+      <c r="B85" s="191"/>
+      <c r="C85" s="106" t="s">
         <v>264</v>
       </c>
-      <c r="D84" s="163" t="s">
+      <c r="D85" s="106" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="185"/>
-      <c r="B85" s="176"/>
-      <c r="C85" s="171" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="193"/>
+      <c r="B86" s="191"/>
+      <c r="C86" s="112" t="s">
         <v>272</v>
       </c>
-      <c r="D85" s="171" t="s">
+      <c r="D86" s="112" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="185"/>
-      <c r="B86" s="176"/>
-      <c r="C86" s="163" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="193"/>
+      <c r="B87" s="191"/>
+      <c r="C87" s="106" t="s">
         <v>277</v>
       </c>
-      <c r="D86" s="163" t="s">
+      <c r="D87" s="106" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="185"/>
-      <c r="B87" s="176"/>
-      <c r="C87" s="163" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="193"/>
+      <c r="B88" s="191"/>
+      <c r="C88" s="106" t="s">
         <v>278</v>
       </c>
-      <c r="D87" s="163" t="s">
+      <c r="D88" s="106" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="185"/>
-      <c r="B88" s="176"/>
-      <c r="C88" s="171" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="193"/>
+      <c r="B89" s="191"/>
+      <c r="C89" s="112" t="s">
         <v>283</v>
       </c>
-      <c r="D88" s="171" t="s">
+      <c r="D89" s="112" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="185"/>
-      <c r="B89" s="176"/>
-      <c r="C89" s="171" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="193"/>
+      <c r="B90" s="191"/>
+      <c r="C90" s="112" t="s">
         <v>297</v>
       </c>
-      <c r="D89" s="171" t="s">
+      <c r="D90" s="112" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="185"/>
-      <c r="B90" s="176"/>
-      <c r="C90" s="171" t="s">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="193"/>
+      <c r="B91" s="191"/>
+      <c r="C91" s="112" t="s">
         <v>284</v>
       </c>
-      <c r="D90" s="171" t="s">
+      <c r="D91" s="112" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A91" s="185"/>
-      <c r="B91" s="176"/>
-      <c r="C91" s="195" t="s">
+    <row r="92" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="193"/>
+      <c r="B92" s="191"/>
+      <c r="C92" s="122" t="s">
         <v>243</v>
       </c>
-      <c r="D91" s="168" t="s">
+      <c r="D92" s="109" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A92" s="185"/>
-      <c r="B92" s="176"/>
-      <c r="C92" s="186" t="s">
+    <row r="93" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A93" s="193"/>
+      <c r="B93" s="191"/>
+      <c r="C93" s="116" t="s">
         <v>306</v>
       </c>
-      <c r="D92" s="171" t="s">
+      <c r="D93" s="112" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="185"/>
-      <c r="B93" s="176"/>
-      <c r="C93" s="163" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="193"/>
+      <c r="B94" s="191"/>
+      <c r="C94" s="106" t="s">
         <v>307</v>
       </c>
-      <c r="D93" s="163" t="s">
+      <c r="D94" s="106" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="185"/>
-      <c r="B94" s="176"/>
-      <c r="C94" s="171" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="193"/>
+      <c r="B95" s="191"/>
+      <c r="C95" s="112" t="s">
         <v>308</v>
       </c>
-      <c r="D94" s="171" t="s">
+      <c r="D95" s="112" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="185"/>
-      <c r="B95" s="176"/>
-      <c r="C95" s="171" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="193"/>
+      <c r="B96" s="191"/>
+      <c r="C96" s="112" t="s">
         <v>310</v>
       </c>
-      <c r="D95" s="171" t="s">
+      <c r="D96" s="112" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="185"/>
-      <c r="B96" s="176"/>
-      <c r="C96" s="171" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="193"/>
+      <c r="B97" s="191"/>
+      <c r="C97" s="112" t="s">
         <v>263</v>
       </c>
-      <c r="D96" s="171" t="s">
+      <c r="D97" s="112" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="185"/>
-      <c r="B97" s="176"/>
-      <c r="C97" s="163" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="193"/>
+      <c r="B98" s="191"/>
+      <c r="C98" s="106" t="s">
         <v>313</v>
       </c>
-      <c r="D97" s="163" t="s">
+      <c r="D98" s="106" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="185"/>
-      <c r="B98" s="176"/>
-      <c r="C98" s="171" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="193"/>
+      <c r="B99" s="191"/>
+      <c r="C99" s="112" t="s">
         <v>278</v>
       </c>
-      <c r="D98" s="171" t="s">
+      <c r="D99" s="112" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="185"/>
-      <c r="B99" s="176"/>
-      <c r="C99" s="171" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="193"/>
+      <c r="B100" s="191"/>
+      <c r="C100" s="112" t="s">
         <v>314</v>
       </c>
-      <c r="D99" s="171" t="s">
+      <c r="D100" s="112" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A100" s="185"/>
-      <c r="B100" s="176"/>
-      <c r="C100" s="163"/>
-      <c r="D100" s="97" t="s">
+    <row r="101" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A101" s="193"/>
+      <c r="B101" s="191"/>
+      <c r="C101" s="106"/>
+      <c r="D101" s="97" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="185"/>
-      <c r="B101" s="176"/>
-      <c r="C101" s="171" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="193"/>
+      <c r="B102" s="191"/>
+      <c r="C102" s="112" t="s">
         <v>317</v>
       </c>
-      <c r="D101" s="171" t="s">
+      <c r="D102" s="112" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="185"/>
-      <c r="B102" s="176"/>
-      <c r="C102" s="171" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="193"/>
+      <c r="B103" s="191"/>
+      <c r="C103" s="112" t="s">
         <v>263</v>
       </c>
-      <c r="D102" s="171" t="s">
+      <c r="D103" s="112" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="185"/>
-      <c r="B103" s="176"/>
-      <c r="C103" s="171" t="s">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="193"/>
+      <c r="B104" s="191"/>
+      <c r="C104" s="112" t="s">
         <v>334</v>
       </c>
-      <c r="D103" s="171" t="s">
+      <c r="D104" s="112" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="185"/>
-      <c r="B104" s="176"/>
-      <c r="C104" s="171" t="s">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="193"/>
+      <c r="B105" s="191"/>
+      <c r="C105" s="112" t="s">
         <v>335</v>
       </c>
-      <c r="D104" s="171" t="s">
+      <c r="D105" s="112" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="185"/>
-      <c r="B105" s="176"/>
-      <c r="C105" s="171" t="s">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="193"/>
+      <c r="B106" s="191"/>
+      <c r="C106" s="112" t="s">
         <v>319</v>
       </c>
-      <c r="D105" s="171" t="s">
+      <c r="D106" s="112" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="185"/>
-      <c r="B106" s="176"/>
-      <c r="C106" s="187" t="s">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="193"/>
+      <c r="B107" s="191"/>
+      <c r="C107" s="117" t="s">
         <v>340</v>
       </c>
-      <c r="D106" s="187" t="s">
+      <c r="D107" s="117" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="185"/>
-      <c r="B107" s="176"/>
-      <c r="C107" s="171" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="193"/>
+      <c r="B108" s="191"/>
+      <c r="C108" s="112" t="s">
         <v>333</v>
       </c>
-      <c r="D107" s="171" t="s">
+      <c r="D108" s="112" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="185"/>
-      <c r="B108" s="176"/>
-      <c r="C108" s="171" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="193"/>
+      <c r="B109" s="191"/>
+      <c r="C109" s="112" t="s">
         <v>348</v>
       </c>
-      <c r="D108" s="171" t="s">
+      <c r="D109" s="112" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="185"/>
-      <c r="B109" s="176"/>
-      <c r="C109" s="101" t="s">
+    <row r="110" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A110" s="193"/>
+      <c r="B110" s="191"/>
+      <c r="C110" s="101" t="s">
         <v>351</v>
       </c>
-      <c r="D109" s="196" t="s">
+      <c r="D110" s="123" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="185"/>
-      <c r="B110" s="176"/>
-      <c r="C110" s="171" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="193"/>
+      <c r="B111" s="191"/>
+      <c r="C111" s="112" t="s">
         <v>352</v>
       </c>
-      <c r="D110" s="171" t="s">
+      <c r="D111" s="112" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="185"/>
-      <c r="B111" s="176"/>
-      <c r="C111" s="171" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="193"/>
+      <c r="B112" s="191"/>
+      <c r="C112" s="112" t="s">
         <v>353</v>
       </c>
-      <c r="D111" s="171" t="s">
+      <c r="D112" s="112" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="185"/>
-      <c r="B112" s="176"/>
-      <c r="C112" s="171" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="193"/>
+      <c r="B113" s="191"/>
+      <c r="C113" s="112" t="s">
         <v>359</v>
       </c>
-      <c r="D112" s="171" t="s">
+      <c r="D113" s="112" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="185"/>
-      <c r="B113" s="176"/>
-      <c r="C113" s="171" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="193"/>
+      <c r="B114" s="191"/>
+      <c r="C114" s="112" t="s">
         <v>361</v>
       </c>
-      <c r="D113" s="171" t="s">
+      <c r="D114" s="112" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="185"/>
-      <c r="B114" s="176"/>
-      <c r="C114" s="171" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="193"/>
+      <c r="B115" s="191"/>
+      <c r="C115" s="112" t="s">
         <v>367</v>
       </c>
-      <c r="D114" s="171" t="s">
+      <c r="D115" s="112" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="185"/>
-      <c r="B115" s="176"/>
-      <c r="C115" s="171" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="193"/>
+      <c r="B116" s="191"/>
+      <c r="C116" s="112" t="s">
         <v>359</v>
       </c>
-      <c r="D115" s="171" t="s">
+      <c r="D116" s="112" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="185"/>
-      <c r="B116" s="176"/>
-      <c r="C116" s="187" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="193"/>
+      <c r="B117" s="191"/>
+      <c r="C117" s="117" t="s">
         <v>380</v>
       </c>
-      <c r="D116" s="187" t="s">
+      <c r="D117" s="117" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="185"/>
-      <c r="B117" s="176"/>
-      <c r="C117" s="163" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="193"/>
+      <c r="B118" s="191"/>
+      <c r="C118" s="106" t="s">
         <v>384</v>
       </c>
-      <c r="D117" s="163" t="s">
+      <c r="D118" s="106" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="185"/>
-      <c r="B118" s="176"/>
-      <c r="C118" s="163" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="193"/>
+      <c r="B119" s="191"/>
+      <c r="C119" s="106" t="s">
         <v>387</v>
       </c>
-      <c r="D118" s="163" t="s">
+      <c r="D119" s="106" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="185"/>
-      <c r="B119" s="176"/>
-      <c r="C119" s="163" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="193"/>
+      <c r="B120" s="191"/>
+      <c r="C120" s="106" t="s">
         <v>388</v>
       </c>
-      <c r="D119" s="163" t="s">
+      <c r="D120" s="106" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="185"/>
-      <c r="B120" s="176"/>
-      <c r="C120" s="163" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="193"/>
+      <c r="B121" s="191"/>
+      <c r="C121" s="106" t="s">
         <v>389</v>
       </c>
-      <c r="D120" s="163" t="s">
+      <c r="D121" s="106" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="185"/>
-      <c r="B121" s="176"/>
-      <c r="C121" s="163" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="193"/>
+      <c r="B122" s="191"/>
+      <c r="C122" s="106" t="s">
         <v>390</v>
       </c>
-      <c r="D121" s="163" t="s">
+      <c r="D122" s="106" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="185"/>
-      <c r="B122" s="176"/>
-      <c r="C122" s="163" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="193"/>
+      <c r="B123" s="191"/>
+      <c r="C123" s="106" t="s">
         <v>391</v>
       </c>
-      <c r="D122" s="163" t="s">
+      <c r="D123" s="106" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="185"/>
-      <c r="B123" s="176"/>
-      <c r="C123" s="163" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="193"/>
+      <c r="B124" s="191"/>
+      <c r="C124" s="106" t="s">
         <v>394</v>
       </c>
-      <c r="D123" s="163" t="s">
+      <c r="D124" s="106" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="185"/>
-      <c r="B124" s="176"/>
-      <c r="C124" s="163" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="193"/>
+      <c r="B125" s="191"/>
+      <c r="C125" s="106" t="s">
         <v>404</v>
       </c>
-      <c r="D124" s="163" t="s">
+      <c r="D125" s="106" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="185"/>
-      <c r="B125" s="176"/>
-      <c r="C125" s="163" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="193"/>
+      <c r="B126" s="191"/>
+      <c r="C126" s="106" t="s">
         <v>405</v>
       </c>
-      <c r="D125" s="163" t="s">
+      <c r="D126" s="106" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="185"/>
-      <c r="B126" s="176"/>
-      <c r="C126" s="163" t="s">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="193"/>
+      <c r="B127" s="191"/>
+      <c r="C127" s="106" t="s">
         <v>422</v>
       </c>
-      <c r="D126" s="163" t="s">
+      <c r="D127" s="106" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="185"/>
-      <c r="B127" s="176"/>
-      <c r="C127" s="163" t="s">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="193"/>
+      <c r="B128" s="191"/>
+      <c r="C128" s="106" t="s">
         <v>423</v>
       </c>
-      <c r="D127" s="163" t="s">
+      <c r="D128" s="106" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="188"/>
-      <c r="B128" s="179"/>
-      <c r="C128" s="163" t="s">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="194"/>
+      <c r="B129" s="187"/>
+      <c r="C129" s="106" t="s">
         <v>426</v>
       </c>
-      <c r="D128" s="163" t="s">
+      <c r="D129" s="106" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="197" t="s">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="124" t="s">
         <v>416</v>
-      </c>
-      <c r="B129" s="70" t="s">
-        <v>432</v>
-      </c>
-      <c r="C129" s="163" t="s">
-        <v>30</v>
-      </c>
-      <c r="D129" s="171" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="167" t="s">
-        <v>304</v>
       </c>
       <c r="B130" s="70" t="s">
         <v>432</v>
       </c>
-      <c r="C130" s="163" t="s">
+      <c r="C130" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="D130" s="171" t="s">
+      <c r="D130" s="112" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="167" t="s">
-        <v>305</v>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="108" t="s">
+        <v>304</v>
       </c>
       <c r="B131" s="70" t="s">
         <v>432</v>
       </c>
-      <c r="C131" s="163" t="s">
+      <c r="C131" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="D131" s="171" t="s">
+      <c r="D131" s="112" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="160" t="s">
+    <row r="132" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="108" t="s">
+        <v>305</v>
+      </c>
+      <c r="B132" s="70" t="s">
+        <v>432</v>
+      </c>
+      <c r="C132" s="106" t="s">
+        <v>30</v>
+      </c>
+      <c r="D132" s="112" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="B132" s="160"/>
-      <c r="C132" s="160"/>
-      <c r="D132" s="161"/>
-    </row>
-    <row r="133" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="189" t="s">
+      <c r="B133" s="103"/>
+      <c r="C133" s="103"/>
+      <c r="D133" s="104"/>
+    </row>
+    <row r="134" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="189" t="s">
         <v>84</v>
       </c>
-      <c r="B133" s="173" t="s">
+      <c r="B134" s="186" t="s">
         <v>432</v>
       </c>
-      <c r="C133" s="163"/>
-      <c r="D133" s="80" t="s">
+      <c r="C134" s="106"/>
+      <c r="D134" s="80" t="s">
         <v>441</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="190"/>
-      <c r="B134" s="176"/>
-      <c r="C134" s="70" t="s">
-        <v>245</v>
-      </c>
-      <c r="D134" s="163" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="190"/>
-      <c r="B135" s="176"/>
-      <c r="C135" s="70">
-        <v>10.1</v>
-      </c>
-      <c r="D135" s="163" t="s">
-        <v>267</v>
+      <c r="B135" s="191"/>
+      <c r="C135" s="70" t="s">
+        <v>245</v>
+      </c>
+      <c r="D135" s="106" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="190"/>
-      <c r="B136" s="176"/>
+      <c r="B136" s="191"/>
       <c r="C136" s="70">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="D136" s="163" t="s">
+        <v>10.1</v>
+      </c>
+      <c r="D136" s="106" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="190"/>
-      <c r="B137" s="176"/>
-      <c r="C137" s="98" t="s">
-        <v>288</v>
-      </c>
-      <c r="D137" s="95" t="s">
-        <v>289</v>
+      <c r="B137" s="191"/>
+      <c r="C137" s="70">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D137" s="106" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="190"/>
-      <c r="B138" s="176"/>
+      <c r="B138" s="191"/>
       <c r="C138" s="98" t="s">
-        <v>370</v>
+        <v>288</v>
       </c>
       <c r="D138" s="95" t="s">
-        <v>371</v>
+        <v>289</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="190"/>
-      <c r="B139" s="176"/>
+      <c r="B139" s="191"/>
       <c r="C139" s="98" t="s">
-        <v>117</v>
+        <v>370</v>
       </c>
       <c r="D139" s="95" t="s">
-        <v>415</v>
+        <v>371</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="190"/>
-      <c r="B140" s="176"/>
+      <c r="B140" s="191"/>
       <c r="C140" s="98" t="s">
+        <v>117</v>
+      </c>
+      <c r="D140" s="95" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="190"/>
+      <c r="B141" s="191"/>
+      <c r="C141" s="98" t="s">
         <v>417</v>
       </c>
-      <c r="D140" s="95" t="s">
+      <c r="D141" s="95" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="198"/>
-      <c r="B141" s="179"/>
-      <c r="C141" s="98" t="s">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="205"/>
+      <c r="B142" s="187"/>
+      <c r="C142" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="D141" s="95" t="s">
+      <c r="D142" s="95" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="173" t="s">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="186" t="s">
         <v>246</v>
       </c>
-      <c r="B142" s="173" t="s">
+      <c r="B143" s="186" t="s">
         <v>432</v>
       </c>
-      <c r="C142" s="98"/>
-      <c r="D142" s="199" t="s">
+      <c r="C143" s="98"/>
+      <c r="D143" s="125" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="176"/>
-      <c r="B143" s="176"/>
-      <c r="C143" s="200" t="s">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="191"/>
+      <c r="B144" s="191"/>
+      <c r="C144" s="126" t="s">
         <v>428</v>
       </c>
-      <c r="D143" s="102" t="s">
+      <c r="D144" s="102" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="168" t="s">
+    <row r="145" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="109" t="s">
         <v>257</v>
       </c>
-      <c r="B144" s="70" t="s">
+      <c r="B145" s="70" t="s">
         <v>432</v>
       </c>
-      <c r="C144" s="70" t="s">
+      <c r="C145" s="70" t="s">
         <v>249</v>
       </c>
-      <c r="D144" s="171" t="s">
+      <c r="D145" s="112" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="201" t="s">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="127" t="s">
         <v>247</v>
       </c>
-      <c r="B145" s="160"/>
-      <c r="C145" s="202"/>
-      <c r="D145" s="202"/>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="167" t="s">
+      <c r="B146" s="103"/>
+      <c r="C146" s="128"/>
+      <c r="D146" s="128"/>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="108" t="s">
         <v>248</v>
       </c>
-      <c r="B146" s="70" t="s">
+      <c r="B147" s="70" t="s">
         <v>432</v>
       </c>
-      <c r="C146" s="203" t="s">
+      <c r="C147" s="129" t="s">
         <v>260</v>
       </c>
-      <c r="D146" s="163" t="s">
+      <c r="D147" s="106" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="189" t="s">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="189" t="s">
         <v>280</v>
       </c>
-      <c r="B147" s="173" t="s">
+      <c r="B148" s="186" t="s">
         <v>432</v>
       </c>
-      <c r="C147" s="95" t="s">
+      <c r="C148" s="95" t="s">
         <v>290</v>
       </c>
-      <c r="D147" s="163" t="s">
+      <c r="D148" s="106" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="190"/>
-      <c r="B148" s="176"/>
-      <c r="C148" s="163" t="s">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="190"/>
+      <c r="B149" s="191"/>
+      <c r="C149" s="106" t="s">
         <v>300</v>
       </c>
-      <c r="D148" s="171" t="s">
+      <c r="D149" s="112" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A149" s="190"/>
-      <c r="B149" s="176"/>
-      <c r="C149" s="203" t="s">
+    <row r="150" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A150" s="190"/>
+      <c r="B150" s="191"/>
+      <c r="C150" s="129" t="s">
         <v>281</v>
       </c>
-      <c r="D149" s="163" t="s">
+      <c r="D150" s="106" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="198"/>
-      <c r="B150" s="179"/>
-      <c r="C150" s="203" t="s">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="205"/>
+      <c r="B151" s="187"/>
+      <c r="C151" s="129" t="s">
         <v>21</v>
       </c>
-      <c r="D150" s="163" t="s">
+      <c r="D151" s="106" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="202" t="s">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="128" t="s">
         <v>56</v>
       </c>
-      <c r="B151" s="202"/>
-      <c r="C151" s="202"/>
-      <c r="D151" s="202"/>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="189" t="s">
+      <c r="B152" s="128"/>
+      <c r="C152" s="128"/>
+      <c r="D152" s="128"/>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="189" t="s">
         <v>58</v>
       </c>
-      <c r="B152" s="173" t="s">
+      <c r="B153" s="186" t="s">
         <v>266</v>
       </c>
-      <c r="C152" s="203" t="s">
+      <c r="C153" s="129" t="s">
         <v>260</v>
       </c>
-      <c r="D152" s="163" t="s">
+      <c r="D153" s="106" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="190"/>
-      <c r="B153" s="176"/>
-      <c r="C153" s="203" t="s">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="190"/>
+      <c r="B154" s="191"/>
+      <c r="C154" s="129" t="s">
         <v>260</v>
       </c>
-      <c r="D153" s="163" t="s">
+      <c r="D154" s="106" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="198"/>
-      <c r="B154" s="179"/>
-      <c r="C154" s="163"/>
-      <c r="D154" s="163" t="s">
+    <row r="155" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="205"/>
+      <c r="B155" s="187"/>
+      <c r="C155" s="106"/>
+      <c r="D155" s="106" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="155" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A155" s="204" t="s">
+    <row r="156" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A156" s="184" t="s">
         <v>59</v>
       </c>
-      <c r="B155" s="173" t="s">
+      <c r="B156" s="186" t="s">
         <v>266</v>
       </c>
-      <c r="C155" s="191" t="s">
+      <c r="C156" s="118" t="s">
         <v>259</v>
       </c>
-      <c r="D155" s="163" t="s">
+      <c r="D156" s="106" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="205"/>
-      <c r="B156" s="179"/>
-      <c r="C156" s="191"/>
-      <c r="D156" s="163" t="s">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="185"/>
+      <c r="B157" s="187"/>
+      <c r="C157" s="118"/>
+      <c r="D157" s="106" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A157" s="204" t="s">
+    <row r="158" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A158" s="184" t="s">
         <v>286</v>
       </c>
-      <c r="B157" s="173" t="s">
+      <c r="B158" s="186" t="s">
         <v>266</v>
       </c>
-      <c r="C157" s="191"/>
-      <c r="D157" s="191" t="s">
+      <c r="C158" s="118"/>
+      <c r="D158" s="118" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="205"/>
-      <c r="B158" s="179"/>
-      <c r="C158" s="163"/>
-      <c r="D158" s="163" t="s">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="185"/>
+      <c r="B159" s="187"/>
+      <c r="C159" s="106"/>
+      <c r="D159" s="106" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A159" s="204" t="s">
+    <row r="160" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A160" s="184" t="s">
         <v>60</v>
       </c>
-      <c r="B159" s="173" t="s">
+      <c r="B160" s="186" t="s">
         <v>266</v>
       </c>
-      <c r="C159" s="191" t="s">
+      <c r="C160" s="118" t="s">
         <v>259</v>
       </c>
-      <c r="D159" s="163" t="s">
+      <c r="D160" s="106" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="205"/>
-      <c r="B160" s="179"/>
-      <c r="C160" s="163"/>
-      <c r="D160" s="163" t="s">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="185"/>
+      <c r="B161" s="187"/>
+      <c r="C161" s="106"/>
+      <c r="D161" s="106" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="202" t="s">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="128" t="s">
         <v>268</v>
       </c>
-      <c r="B161" s="202"/>
-      <c r="C161" s="202"/>
-      <c r="D161" s="202"/>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="163"/>
-      <c r="B162" s="70" t="s">
+      <c r="B162" s="128"/>
+      <c r="C162" s="128"/>
+      <c r="D162" s="128"/>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="106"/>
+      <c r="B163" s="70" t="s">
         <v>432</v>
       </c>
-      <c r="C162" s="163" t="s">
+      <c r="C163" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="D162" s="171" t="s">
+      <c r="D163" s="112" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="202" t="s">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="128" t="s">
         <v>274</v>
       </c>
-      <c r="B163" s="202"/>
-      <c r="C163" s="202"/>
-      <c r="D163" s="202"/>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="163"/>
-      <c r="B164" s="70" t="s">
+      <c r="B164" s="128"/>
+      <c r="C164" s="128"/>
+      <c r="D164" s="128"/>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="106"/>
+      <c r="B165" s="70" t="s">
         <v>432</v>
       </c>
-      <c r="C164" s="163" t="s">
+      <c r="C165" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="D164" s="171" t="s">
+      <c r="D165" s="112" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="163"/>
-      <c r="B165" s="70"/>
-      <c r="C165" s="163" t="s">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="106"/>
+      <c r="B166" s="70"/>
+      <c r="C166" s="106" t="s">
         <v>396</v>
       </c>
-      <c r="D165" s="171" t="s">
+      <c r="D166" s="112" t="s">
         <v>397</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="D78:D81"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="A153:A155"/>
+    <mergeCell ref="B153:B155"/>
+    <mergeCell ref="A134:A142"/>
+    <mergeCell ref="B134:B142"/>
+    <mergeCell ref="A148:A151"/>
+    <mergeCell ref="B148:B151"/>
+    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="A39:A46"/>
+    <mergeCell ref="B39:B46"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="A143:A144"/>
+    <mergeCell ref="B143:B144"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="A71:A75"/>
+    <mergeCell ref="B71:B75"/>
+    <mergeCell ref="A83:A129"/>
+    <mergeCell ref="B83:B129"/>
+    <mergeCell ref="A47:A60"/>
+    <mergeCell ref="B47:B60"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="A76:A81"/>
+    <mergeCell ref="B76:B81"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="B64:B68"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A159:A160"/>
-    <mergeCell ref="B159:B160"/>
-    <mergeCell ref="A155:A156"/>
-    <mergeCell ref="B155:B156"/>
-    <mergeCell ref="A157:A158"/>
-    <mergeCell ref="B157:B158"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="A70:A74"/>
-    <mergeCell ref="B70:B74"/>
-    <mergeCell ref="A82:A128"/>
-    <mergeCell ref="B82:B128"/>
-    <mergeCell ref="A47:A59"/>
-    <mergeCell ref="B47:B59"/>
-    <mergeCell ref="A60:A62"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="A75:A80"/>
-    <mergeCell ref="B75:B80"/>
-    <mergeCell ref="A63:A67"/>
-    <mergeCell ref="B63:B67"/>
+    <mergeCell ref="A160:A161"/>
+    <mergeCell ref="B160:B161"/>
+    <mergeCell ref="A156:A157"/>
+    <mergeCell ref="B156:B157"/>
+    <mergeCell ref="A158:A159"/>
+    <mergeCell ref="B158:B159"/>
     <mergeCell ref="A6:A8"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="B10:B11"/>
@@ -33339,22 +33362,6 @@
     <mergeCell ref="B21:B27"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A16:A19"/>
-    <mergeCell ref="D77:D80"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="A152:A154"/>
-    <mergeCell ref="B152:B154"/>
-    <mergeCell ref="A133:A141"/>
-    <mergeCell ref="B133:B141"/>
-    <mergeCell ref="A147:A150"/>
-    <mergeCell ref="B147:B150"/>
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="B33:B38"/>
-    <mergeCell ref="A39:A46"/>
-    <mergeCell ref="B39:B46"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="A142:A143"/>
-    <mergeCell ref="B142:B143"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Line Item Correction Rules line 8, updated
</commit_message>
<xml_diff>
--- a/PIT3/Schema Publication Changelog.xlsx
+++ b/PIT3/Schema Publication Changelog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitLab\DOCUMENTATION\src\main\resources\PIT3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sconnor0\IdeaProjects\paye-employers-documentation\src\main\resources\PIT3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A192E86F-31BC-47E1-B6C7-7B2B6DA9754E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9187238-0F22-47FF-A5FE-16CD1C403587}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v0.10" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
+    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
     <customWorkbookView name="O'Brien, Ciaran - Personal View" guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="751" activeSheetId="2"/>
-    <customWorkbookView name="Arnold, Eve - Personal View" guid="{057DBB0B-BBF6-4A94-8406-46C99A7DC1D6}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1276" windowHeight="758" activeSheetId="2"/>
-    <customWorkbookView name="Walsh, David P - Personal View" guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1436" windowHeight="675" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="485">
   <si>
     <t>Document</t>
   </si>
@@ -3328,6 +3328,12 @@
   </si>
   <si>
     <t>PIT Current Version Features</t>
+  </si>
+  <si>
+    <t>Item line number 8</t>
+  </si>
+  <si>
+    <t>Context Updated</t>
   </si>
 </sst>
 </file>
@@ -3942,7 +3948,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="220">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -4307,7 +4313,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4316,6 +4321,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4362,8 +4374,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -4386,66 +4428,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4467,16 +4449,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4488,17 +4500,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4509,6 +4524,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4518,30 +4539,23 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4946,12 +4960,12 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="144" t="s">
+      <c r="A2" s="146" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="145"/>
-      <c r="C2" s="145"/>
-      <c r="D2" s="146"/>
+      <c r="B2" s="147"/>
+      <c r="C2" s="147"/>
+      <c r="D2" s="148"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -4974,12 +4988,12 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="144" t="s">
+      <c r="A4" s="146" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="145"/>
-      <c r="C4" s="145"/>
-      <c r="D4" s="146"/>
+      <c r="B4" s="147"/>
+      <c r="C4" s="147"/>
+      <c r="D4" s="148"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -5019,10 +5033,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="147" t="s">
+      <c r="A7" s="149" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="150">
+      <c r="B7" s="152">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -5036,8 +5050,8 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="148"/>
-      <c r="B8" s="151"/>
+      <c r="A8" s="150"/>
+      <c r="B8" s="153"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -5049,8 +5063,8 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="148"/>
-      <c r="B9" s="151"/>
+      <c r="A9" s="150"/>
+      <c r="B9" s="153"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -5062,8 +5076,8 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="148"/>
-      <c r="B10" s="151"/>
+      <c r="A10" s="150"/>
+      <c r="B10" s="153"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -5075,8 +5089,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="148"/>
-      <c r="B11" s="151"/>
+      <c r="A11" s="150"/>
+      <c r="B11" s="153"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -5088,8 +5102,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="149"/>
-      <c r="B12" s="152"/>
+      <c r="A12" s="151"/>
+      <c r="B12" s="154"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -5101,10 +5115,10 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="155" t="s">
+      <c r="A13" s="157" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="150">
+      <c r="B13" s="152">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -5118,8 +5132,8 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="156"/>
-      <c r="B14" s="152"/>
+      <c r="A14" s="158"/>
+      <c r="B14" s="154"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -5165,12 +5179,12 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="144" t="s">
+      <c r="A17" s="146" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="145"/>
-      <c r="C17" s="145"/>
-      <c r="D17" s="146"/>
+      <c r="B17" s="147"/>
+      <c r="C17" s="147"/>
+      <c r="D17" s="148"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -5210,21 +5224,21 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="144" t="s">
+      <c r="A20" s="146" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="145"/>
-      <c r="C20" s="145"/>
-      <c r="D20" s="146"/>
+      <c r="B20" s="147"/>
+      <c r="C20" s="147"/>
+      <c r="D20" s="148"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="157" t="s">
+      <c r="A21" s="159" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="154">
+      <c r="B21" s="156">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -5238,8 +5252,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="158"/>
-      <c r="B22" s="152"/>
+      <c r="A22" s="160"/>
+      <c r="B22" s="154"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -5262,18 +5276,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="144" t="s">
+      <c r="A24" s="146" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="145"/>
-      <c r="C24" s="145"/>
-      <c r="D24" s="146"/>
+      <c r="B24" s="147"/>
+      <c r="C24" s="147"/>
+      <c r="D24" s="148"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="153" t="s">
+      <c r="A25" s="155" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="154">
+      <c r="B25" s="156">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -5287,8 +5301,8 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="148"/>
-      <c r="B26" s="151"/>
+      <c r="A26" s="150"/>
+      <c r="B26" s="153"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -5300,8 +5314,8 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="148"/>
-      <c r="B27" s="151"/>
+      <c r="A27" s="150"/>
+      <c r="B27" s="153"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -5313,8 +5327,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="148"/>
-      <c r="B28" s="151"/>
+      <c r="A28" s="150"/>
+      <c r="B28" s="153"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -5326,8 +5340,8 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="148"/>
-      <c r="B29" s="151"/>
+      <c r="A29" s="150"/>
+      <c r="B29" s="153"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -5339,8 +5353,8 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="148"/>
-      <c r="B30" s="151"/>
+      <c r="A30" s="150"/>
+      <c r="B30" s="153"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -5352,8 +5366,8 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="148"/>
-      <c r="B31" s="151"/>
+      <c r="A31" s="150"/>
+      <c r="B31" s="153"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -5365,8 +5379,8 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="149"/>
-      <c r="B32" s="152"/>
+      <c r="A32" s="151"/>
+      <c r="B32" s="154"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -5490,12 +5504,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="144" t="s">
+      <c r="A41" s="146" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="145"/>
-      <c r="C41" s="145"/>
-      <c r="D41" s="146"/>
+      <c r="B41" s="147"/>
+      <c r="C41" s="147"/>
+      <c r="D41" s="148"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -5555,7 +5569,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5565,7 +5579,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}" topLeftCell="B1">
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="B1">
       <selection activeCell="C15" sqref="C15:D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -5675,10 +5689,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="174" t="s">
+      <c r="A7" s="161" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="173" t="s">
+      <c r="B7" s="162" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5689,8 +5703,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="174"/>
-      <c r="B8" s="173"/>
+      <c r="A8" s="161"/>
+      <c r="B8" s="162"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5699,8 +5713,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="174"/>
-      <c r="B9" s="173"/>
+      <c r="A9" s="161"/>
+      <c r="B9" s="162"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5709,8 +5723,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="174"/>
-      <c r="B10" s="173"/>
+      <c r="A10" s="161"/>
+      <c r="B10" s="162"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5719,8 +5733,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="174"/>
-      <c r="B11" s="173"/>
+      <c r="A11" s="161"/>
+      <c r="B11" s="162"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5729,8 +5743,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="174"/>
-      <c r="B12" s="173"/>
+      <c r="A12" s="161"/>
+      <c r="B12" s="162"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5739,10 +5753,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="176" t="s">
+      <c r="A13" s="164" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="173" t="s">
+      <c r="B13" s="162" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5753,8 +5767,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="176"/>
-      <c r="B14" s="173"/>
+      <c r="A14" s="164"/>
+      <c r="B14" s="162"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5763,8 +5777,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="176"/>
-      <c r="B15" s="173"/>
+      <c r="A15" s="164"/>
+      <c r="B15" s="162"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5773,10 +5787,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="159" t="s">
+      <c r="A16" s="165" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="168" t="s">
+      <c r="B16" s="166" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5787,8 +5801,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="159"/>
-      <c r="B17" s="168"/>
+      <c r="A17" s="165"/>
+      <c r="B17" s="166"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5797,8 +5811,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="159"/>
-      <c r="B18" s="168"/>
+      <c r="A18" s="165"/>
+      <c r="B18" s="166"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5807,8 +5821,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="159"/>
-      <c r="B19" s="168"/>
+      <c r="A19" s="165"/>
+      <c r="B19" s="166"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5817,8 +5831,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="159"/>
-      <c r="B20" s="168"/>
+      <c r="A20" s="165"/>
+      <c r="B20" s="166"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5827,8 +5841,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="159"/>
-      <c r="B21" s="168"/>
+      <c r="A21" s="165"/>
+      <c r="B21" s="166"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5837,8 +5851,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="159"/>
-      <c r="B22" s="168"/>
+      <c r="A22" s="165"/>
+      <c r="B22" s="166"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5847,8 +5861,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="159"/>
-      <c r="B23" s="168"/>
+      <c r="A23" s="165"/>
+      <c r="B23" s="166"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5857,26 +5871,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="159"/>
-      <c r="B24" s="168"/>
-      <c r="C24" s="159" t="s">
+      <c r="A24" s="165"/>
+      <c r="B24" s="166"/>
+      <c r="C24" s="165" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="160" t="s">
+      <c r="D24" s="172" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="159"/>
-      <c r="B25" s="168"/>
-      <c r="C25" s="159"/>
-      <c r="D25" s="160"/>
+      <c r="A25" s="165"/>
+      <c r="B25" s="166"/>
+      <c r="C25" s="165"/>
+      <c r="D25" s="172"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="174" t="s">
+      <c r="A26" s="161" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="173" t="s">
+      <c r="B26" s="162" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5887,8 +5901,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="174"/>
-      <c r="B27" s="173"/>
+      <c r="A27" s="161"/>
+      <c r="B27" s="162"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5915,28 +5929,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="175" t="s">
+      <c r="A30" s="163" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="173" t="s">
+      <c r="B30" s="162" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="159" t="s">
+      <c r="C30" s="165" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="163" t="s">
+      <c r="D30" s="175" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="175"/>
-      <c r="B31" s="173"/>
-      <c r="C31" s="159"/>
-      <c r="D31" s="163"/>
+      <c r="A31" s="163"/>
+      <c r="B31" s="162"/>
+      <c r="C31" s="165"/>
+      <c r="D31" s="175"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="175"/>
-      <c r="B32" s="173"/>
+      <c r="A32" s="163"/>
+      <c r="B32" s="162"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -5945,8 +5959,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="175"/>
-      <c r="B33" s="173"/>
+      <c r="A33" s="163"/>
+      <c r="B33" s="162"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -5955,8 +5969,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="175"/>
-      <c r="B34" s="173"/>
+      <c r="A34" s="163"/>
+      <c r="B34" s="162"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -5965,8 +5979,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="175"/>
-      <c r="B35" s="173"/>
+      <c r="A35" s="163"/>
+      <c r="B35" s="162"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -5975,8 +5989,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="175"/>
-      <c r="B36" s="173"/>
+      <c r="A36" s="163"/>
+      <c r="B36" s="162"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -5985,26 +5999,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="175"/>
-      <c r="B37" s="173"/>
-      <c r="C37" s="164" t="s">
+      <c r="A37" s="163"/>
+      <c r="B37" s="162"/>
+      <c r="C37" s="176" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="166" t="s">
+      <c r="D37" s="178" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="175"/>
-      <c r="B38" s="173"/>
-      <c r="C38" s="165"/>
-      <c r="D38" s="166"/>
+      <c r="A38" s="163"/>
+      <c r="B38" s="162"/>
+      <c r="C38" s="177"/>
+      <c r="D38" s="178"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="174" t="s">
+      <c r="A39" s="161" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="173" t="s">
+      <c r="B39" s="162" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -6015,8 +6029,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="174"/>
-      <c r="B40" s="173"/>
+      <c r="A40" s="161"/>
+      <c r="B40" s="162"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -6043,10 +6057,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="175" t="s">
+      <c r="A43" s="163" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="173" t="s">
+      <c r="B43" s="162" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -6055,8 +6069,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="175"/>
-      <c r="B44" s="173"/>
+      <c r="A44" s="163"/>
+      <c r="B44" s="162"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -6065,10 +6079,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="170" t="s">
+      <c r="A45" s="169" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="173" t="s">
+      <c r="B45" s="162" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -6077,8 +6091,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="171"/>
-      <c r="B46" s="173"/>
+      <c r="A46" s="170"/>
+      <c r="B46" s="162"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -6087,8 +6101,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="171"/>
-      <c r="B47" s="173"/>
+      <c r="A47" s="170"/>
+      <c r="B47" s="162"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -6097,8 +6111,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="172"/>
-      <c r="B48" s="173"/>
+      <c r="A48" s="171"/>
+      <c r="B48" s="162"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -6107,10 +6121,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="168" t="s">
+      <c r="A49" s="166" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="168" t="s">
+      <c r="B49" s="166" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -10214,8 +10228,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="168"/>
-      <c r="B50" s="168"/>
+      <c r="A50" s="166"/>
+      <c r="B50" s="166"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -14319,8 +14333,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="168"/>
-      <c r="B51" s="168"/>
+      <c r="A51" s="166"/>
+      <c r="B51" s="166"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -18424,8 +18438,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="168"/>
-      <c r="B52" s="168"/>
+      <c r="A52" s="166"/>
+      <c r="B52" s="166"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -22529,12 +22543,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="168"/>
-      <c r="B53" s="168"/>
-      <c r="C53" s="162" t="s">
+      <c r="A53" s="166"/>
+      <c r="B53" s="166"/>
+      <c r="C53" s="174" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="163" t="s">
+      <c r="D53" s="175" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26634,10 +26648,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="168"/>
-      <c r="B54" s="168"/>
-      <c r="C54" s="162"/>
-      <c r="D54" s="163"/>
+      <c r="A54" s="166"/>
+      <c r="B54" s="166"/>
+      <c r="C54" s="174"/>
+      <c r="D54" s="175"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30758,7 +30772,7 @@
       <c r="A57" s="167" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="168" t="s">
+      <c r="B57" s="166" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30770,7 +30784,7 @@
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="167"/>
-      <c r="B58" s="168"/>
+      <c r="B58" s="166"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30780,7 +30794,7 @@
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
       <c r="A59" s="167"/>
-      <c r="B59" s="168"/>
+      <c r="B59" s="166"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30790,7 +30804,7 @@
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="167"/>
-      <c r="B60" s="168"/>
+      <c r="B60" s="166"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30800,7 +30814,7 @@
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
       <c r="A61" s="167"/>
-      <c r="B61" s="168"/>
+      <c r="B61" s="166"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30810,7 +30824,7 @@
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
       <c r="A62" s="167"/>
-      <c r="B62" s="168"/>
+      <c r="B62" s="166"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30820,7 +30834,7 @@
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
       <c r="A63" s="167"/>
-      <c r="B63" s="168"/>
+      <c r="B63" s="166"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30830,7 +30844,7 @@
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
       <c r="A64" s="167"/>
-      <c r="B64" s="168"/>
+      <c r="B64" s="166"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
@@ -30838,7 +30852,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="167"/>
-      <c r="B65" s="168"/>
+      <c r="B65" s="166"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30848,7 +30862,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="167"/>
-      <c r="B66" s="168"/>
+      <c r="B66" s="166"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
@@ -30856,7 +30870,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="167"/>
-      <c r="B67" s="168"/>
+      <c r="B67" s="166"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30866,7 +30880,7 @@
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="167"/>
-      <c r="B68" s="168"/>
+      <c r="B68" s="166"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30876,7 +30890,7 @@
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="167"/>
-      <c r="B69" s="168"/>
+      <c r="B69" s="166"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30886,7 +30900,7 @@
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="167"/>
-      <c r="B70" s="168"/>
+      <c r="B70" s="166"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30896,7 +30910,7 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="167"/>
-      <c r="B71" s="168"/>
+      <c r="B71" s="166"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30906,7 +30920,7 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="167"/>
-      <c r="B72" s="168"/>
+      <c r="B72" s="166"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30916,7 +30930,7 @@
     </row>
     <row r="73" spans="1:4" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="167"/>
-      <c r="B73" s="168"/>
+      <c r="B73" s="166"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
@@ -30924,7 +30938,7 @@
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="167"/>
-      <c r="B74" s="168"/>
+      <c r="B74" s="166"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -30934,17 +30948,17 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="167"/>
-      <c r="B75" s="168"/>
-      <c r="C75" s="161"/>
-      <c r="D75" s="169" t="s">
+      <c r="B75" s="166"/>
+      <c r="C75" s="173"/>
+      <c r="D75" s="168" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="7.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="167"/>
-      <c r="B76" s="168"/>
-      <c r="C76" s="161"/>
-      <c r="D76" s="169"/>
+      <c r="B76" s="166"/>
+      <c r="C76" s="173"/>
+      <c r="D76" s="168"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
@@ -30968,8 +30982,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
-      <selection activeCell="D20" sqref="D20"/>
+    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
+      <selection activeCell="A7" sqref="A7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -30978,13 +30992,29 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{99CEABDF-88F7-4121-AD5F-66FD045725EC}">
-      <selection activeCell="A7" sqref="A7"/>
+    <customSheetView guid="{3ECA9ADB-6C26-4D30-9FA0-625C82AEEE29}" topLeftCell="A13">
+      <selection activeCell="D20" sqref="D20"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="30">
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="A57:A76"/>
+    <mergeCell ref="B57:B76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:A54"/>
+    <mergeCell ref="B49:B54"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="A43:A44"/>
@@ -30999,22 +31029,6 @@
     <mergeCell ref="B16:B25"/>
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A57:A76"/>
-    <mergeCell ref="B57:B76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:A54"/>
-    <mergeCell ref="B49:B54"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
@@ -31068,10 +31082,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="174" t="s">
+      <c r="A4" s="161" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="173" t="s">
+      <c r="B4" s="162" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -31082,133 +31096,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="174"/>
-      <c r="B5" s="173"/>
-      <c r="C5" s="184" t="s">
+      <c r="A5" s="161"/>
+      <c r="B5" s="162"/>
+      <c r="C5" s="188" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="183" t="s">
+      <c r="D5" s="187" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="174"/>
-      <c r="B6" s="173"/>
-      <c r="C6" s="184"/>
-      <c r="D6" s="183"/>
+      <c r="A6" s="161"/>
+      <c r="B6" s="162"/>
+      <c r="C6" s="188"/>
+      <c r="D6" s="187"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="174"/>
-      <c r="B7" s="173"/>
+      <c r="A7" s="161"/>
+      <c r="B7" s="162"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="174"/>
-      <c r="B8" s="173"/>
+      <c r="A8" s="161"/>
+      <c r="B8" s="162"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="174"/>
-      <c r="B9" s="173"/>
+      <c r="A9" s="161"/>
+      <c r="B9" s="162"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="176" t="s">
+      <c r="A10" s="164" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="173" t="s">
+      <c r="B10" s="162" t="s">
         <v>185</v>
       </c>
       <c r="C10" s="186"/>
-      <c r="D10" s="183" t="s">
+      <c r="D10" s="187" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="176"/>
-      <c r="B11" s="173"/>
+      <c r="A11" s="164"/>
+      <c r="B11" s="162"/>
       <c r="C11" s="186"/>
-      <c r="D11" s="183"/>
+      <c r="D11" s="187"/>
     </row>
     <row r="12" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="176"/>
-      <c r="B12" s="173"/>
+      <c r="A12" s="164"/>
+      <c r="B12" s="162"/>
       <c r="C12" s="186"/>
-      <c r="D12" s="183"/>
+      <c r="D12" s="187"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="159" t="s">
+      <c r="A13" s="165" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="168" t="s">
+      <c r="B13" s="166" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="185"/>
-      <c r="D13" s="183" t="s">
+      <c r="C13" s="189"/>
+      <c r="D13" s="187" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="159"/>
-      <c r="B14" s="168"/>
-      <c r="C14" s="185"/>
-      <c r="D14" s="183"/>
+      <c r="A14" s="165"/>
+      <c r="B14" s="166"/>
+      <c r="C14" s="189"/>
+      <c r="D14" s="187"/>
     </row>
     <row r="15" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="159"/>
-      <c r="B15" s="168"/>
-      <c r="C15" s="185"/>
+      <c r="A15" s="165"/>
+      <c r="B15" s="166"/>
+      <c r="C15" s="189"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="159"/>
-      <c r="B16" s="168"/>
-      <c r="C16" s="185"/>
+      <c r="A16" s="165"/>
+      <c r="B16" s="166"/>
+      <c r="C16" s="189"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="159"/>
-      <c r="B17" s="168"/>
-      <c r="C17" s="185"/>
+      <c r="A17" s="165"/>
+      <c r="B17" s="166"/>
+      <c r="C17" s="189"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="159"/>
-      <c r="B18" s="168"/>
-      <c r="C18" s="185"/>
+      <c r="A18" s="165"/>
+      <c r="B18" s="166"/>
+      <c r="C18" s="189"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="159"/>
-      <c r="B19" s="168"/>
-      <c r="C19" s="185"/>
+      <c r="A19" s="165"/>
+      <c r="B19" s="166"/>
+      <c r="C19" s="189"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="159"/>
-      <c r="B20" s="168"/>
-      <c r="C20" s="185"/>
+      <c r="A20" s="165"/>
+      <c r="B20" s="166"/>
+      <c r="C20" s="189"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="159"/>
-      <c r="B21" s="168"/>
-      <c r="C21" s="185"/>
+      <c r="A21" s="165"/>
+      <c r="B21" s="166"/>
+      <c r="C21" s="189"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="159"/>
-      <c r="B22" s="168"/>
-      <c r="C22" s="185"/>
+      <c r="A22" s="165"/>
+      <c r="B22" s="166"/>
+      <c r="C22" s="189"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="159"/>
-      <c r="B23" s="168"/>
-      <c r="C23" s="185"/>
+      <c r="A23" s="165"/>
+      <c r="B23" s="166"/>
+      <c r="C23" s="189"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -31306,10 +31320,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="177" t="s">
+      <c r="A32" s="190" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="180" t="s">
+      <c r="B32" s="193" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -31320,26 +31334,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="178"/>
-      <c r="B33" s="181"/>
+      <c r="A33" s="191"/>
+      <c r="B33" s="194"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="178"/>
-      <c r="B34" s="181"/>
+      <c r="A34" s="191"/>
+      <c r="B34" s="194"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="178"/>
-      <c r="B35" s="181"/>
+      <c r="A35" s="191"/>
+      <c r="B35" s="194"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="179"/>
-      <c r="B36" s="182"/>
+      <c r="A36" s="192"/>
+      <c r="B36" s="195"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -31368,10 +31382,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="175" t="s">
+      <c r="A39" s="163" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="173" t="s">
+      <c r="B39" s="162" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -31382,8 +31396,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="175"/>
-      <c r="B40" s="173"/>
+      <c r="A40" s="163"/>
+      <c r="B40" s="162"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -31392,84 +31406,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="174" t="s">
+      <c r="A41" s="161" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="173" t="s">
+      <c r="B41" s="162" t="s">
         <v>185</v>
       </c>
       <c r="C41" s="186" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="159" t="s">
+      <c r="D41" s="165" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="174"/>
-      <c r="B42" s="173"/>
+      <c r="A42" s="161"/>
+      <c r="B42" s="162"/>
       <c r="C42" s="186"/>
-      <c r="D42" s="159"/>
+      <c r="D42" s="165"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="174"/>
-      <c r="B43" s="173"/>
+      <c r="A43" s="161"/>
+      <c r="B43" s="162"/>
       <c r="C43" s="186" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="169" t="s">
+      <c r="D43" s="168" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="174"/>
-      <c r="B44" s="173"/>
+      <c r="A44" s="161"/>
+      <c r="B44" s="162"/>
       <c r="C44" s="186"/>
-      <c r="D44" s="169"/>
+      <c r="D44" s="168"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="167" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="168" t="s">
+      <c r="B45" s="166" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="190"/>
+      <c r="C45" s="182"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="167"/>
-      <c r="B46" s="168"/>
-      <c r="C46" s="191"/>
-      <c r="D46" s="187" t="s">
+      <c r="B46" s="166"/>
+      <c r="C46" s="183"/>
+      <c r="D46" s="179" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="167"/>
-      <c r="B47" s="168"/>
-      <c r="C47" s="191"/>
-      <c r="D47" s="188"/>
+      <c r="B47" s="166"/>
+      <c r="C47" s="183"/>
+      <c r="D47" s="180"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="167"/>
-      <c r="B48" s="168"/>
-      <c r="C48" s="192"/>
-      <c r="D48" s="188"/>
+      <c r="B48" s="166"/>
+      <c r="C48" s="184"/>
+      <c r="D48" s="180"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="167"/>
-      <c r="B49" s="168"/>
-      <c r="C49" s="162"/>
-      <c r="D49" s="188"/>
+      <c r="B49" s="166"/>
+      <c r="C49" s="174"/>
+      <c r="D49" s="180"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="167"/>
-      <c r="B50" s="168"/>
-      <c r="C50" s="162"/>
-      <c r="D50" s="189"/>
+      <c r="B50" s="166"/>
+      <c r="C50" s="174"/>
+      <c r="D50" s="181"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -31492,10 +31506,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="168" t="s">
+      <c r="A53" s="166" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="168" t="s">
+      <c r="B53" s="166" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -31506,8 +31520,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="168"/>
-      <c r="B54" s="168"/>
+      <c r="A54" s="166"/>
+      <c r="B54" s="166"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -31516,8 +31530,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="168"/>
-      <c r="B55" s="168"/>
+      <c r="A55" s="166"/>
+      <c r="B55" s="166"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -31526,9 +31540,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="168"/>
-      <c r="B56" s="168"/>
-      <c r="C56" s="193" t="s">
+      <c r="A56" s="166"/>
+      <c r="B56" s="166"/>
+      <c r="C56" s="185" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -31536,16 +31550,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="168"/>
-      <c r="B57" s="168"/>
-      <c r="C57" s="193"/>
+      <c r="A57" s="166"/>
+      <c r="B57" s="166"/>
+      <c r="C57" s="185"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="168"/>
-      <c r="B58" s="168"/>
+      <c r="A58" s="166"/>
+      <c r="B58" s="166"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -31554,8 +31568,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="168"/>
-      <c r="B59" s="168"/>
+      <c r="A59" s="166"/>
+      <c r="B59" s="166"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -31564,9 +31578,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="168"/>
-      <c r="B60" s="168"/>
-      <c r="C60" s="193" t="s">
+      <c r="A60" s="166"/>
+      <c r="B60" s="166"/>
+      <c r="C60" s="185" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31574,24 +31588,24 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="168"/>
-      <c r="B61" s="168"/>
-      <c r="C61" s="193"/>
+      <c r="A61" s="166"/>
+      <c r="B61" s="166"/>
+      <c r="C61" s="185"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="168"/>
-      <c r="B62" s="168"/>
-      <c r="C62" s="193"/>
+      <c r="A62" s="166"/>
+      <c r="B62" s="166"/>
+      <c r="C62" s="185"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="168"/>
-      <c r="B63" s="168"/>
+      <c r="A63" s="166"/>
+      <c r="B63" s="166"/>
       <c r="C63" s="186" t="s">
         <v>206</v>
       </c>
@@ -31600,30 +31614,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="168"/>
-      <c r="B64" s="168"/>
+      <c r="A64" s="166"/>
+      <c r="B64" s="166"/>
       <c r="C64" s="186"/>
-      <c r="D64" s="169" t="s">
+      <c r="D64" s="168" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="168"/>
-      <c r="B65" s="168"/>
+      <c r="A65" s="166"/>
+      <c r="B65" s="166"/>
       <c r="C65" s="186"/>
-      <c r="D65" s="169"/>
+      <c r="D65" s="168"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="168"/>
-      <c r="B66" s="168"/>
+      <c r="A66" s="166"/>
+      <c r="B66" s="166"/>
       <c r="C66" s="186"/>
-      <c r="D66" s="169"/>
+      <c r="D66" s="168"/>
     </row>
     <row r="67" spans="1:4" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="168"/>
-      <c r="B67" s="168"/>
+      <c r="A67" s="166"/>
+      <c r="B67" s="166"/>
       <c r="C67" s="186"/>
-      <c r="D67" s="169"/>
+      <c r="D67" s="168"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
@@ -31679,6 +31693,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A13:A23"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C13:C23"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
     <mergeCell ref="D64:D67"/>
     <mergeCell ref="D41:D42"/>
     <mergeCell ref="D46:D50"/>
@@ -31695,23 +31726,6 @@
     <mergeCell ref="B45:B50"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="C63:C67"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C13:C23"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="A32:A36"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="A13:A23"/>
-    <mergeCell ref="B13:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31720,10 +31734,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D202"/>
+  <dimension ref="A1:D203"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A8"/>
+    <sheetView tabSelected="1" topLeftCell="A156" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B174" sqref="B174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31757,10 +31771,10 @@
       <c r="D2" s="104"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="211" t="s">
+      <c r="A3" s="196" t="s">
         <v>434</v>
       </c>
-      <c r="B3" s="211" t="s">
+      <c r="B3" s="196" t="s">
         <v>435</v>
       </c>
       <c r="C3" s="101" t="s">
@@ -31771,8 +31785,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="211"/>
-      <c r="B4" s="211"/>
+      <c r="A4" s="196"/>
+      <c r="B4" s="196"/>
       <c r="C4" s="100" t="s">
         <v>438</v>
       </c>
@@ -31781,16 +31795,16 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="219" t="s">
+      <c r="A5" s="145" t="s">
         <v>482</v>
       </c>
-      <c r="B5" s="219" t="s">
+      <c r="B5" s="145" t="s">
         <v>432</v>
       </c>
-      <c r="C5" s="217" t="s">
+      <c r="C5" s="143" t="s">
         <v>480</v>
       </c>
-      <c r="D5" s="218" t="s">
+      <c r="D5" s="144" t="s">
         <v>250</v>
       </c>
     </row>
@@ -31803,10 +31817,10 @@
       <c r="D6" s="127"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="196" t="s">
+      <c r="A7" s="197" t="s">
         <v>248</v>
       </c>
-      <c r="B7" s="198" t="s">
+      <c r="B7" s="200" t="s">
         <v>432</v>
       </c>
       <c r="C7" s="128" t="s">
@@ -31817,8 +31831,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="201"/>
-      <c r="B8" s="200"/>
+      <c r="A8" s="199"/>
+      <c r="B8" s="202"/>
       <c r="C8" s="128" t="s">
         <v>451</v>
       </c>
@@ -31827,10 +31841,10 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="196" t="s">
+      <c r="A9" s="197" t="s">
         <v>280</v>
       </c>
-      <c r="B9" s="198" t="s">
+      <c r="B9" s="200" t="s">
         <v>432</v>
       </c>
       <c r="C9" s="95" t="s">
@@ -31841,8 +31855,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="197"/>
-      <c r="B10" s="199"/>
+      <c r="A10" s="198"/>
+      <c r="B10" s="201"/>
       <c r="C10" s="106" t="s">
         <v>300</v>
       </c>
@@ -31851,8 +31865,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="197"/>
-      <c r="B11" s="199"/>
+      <c r="A11" s="198"/>
+      <c r="B11" s="201"/>
       <c r="C11" s="128" t="s">
         <v>281</v>
       </c>
@@ -31861,8 +31875,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="197"/>
-      <c r="B12" s="199"/>
+      <c r="A12" s="198"/>
+      <c r="B12" s="201"/>
       <c r="C12" s="128" t="s">
         <v>21</v>
       </c>
@@ -31871,8 +31885,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="201"/>
-      <c r="B13" s="200"/>
+      <c r="A13" s="199"/>
+      <c r="B13" s="202"/>
       <c r="C13" s="128" t="s">
         <v>449</v>
       </c>
@@ -31895,10 +31909,10 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="196" t="s">
+      <c r="A15" s="197" t="s">
         <v>454</v>
       </c>
-      <c r="B15" s="198" t="s">
+      <c r="B15" s="200" t="s">
         <v>432</v>
       </c>
       <c r="C15" s="128" t="s">
@@ -31909,8 +31923,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="201"/>
-      <c r="B16" s="200"/>
+      <c r="A16" s="199"/>
+      <c r="B16" s="202"/>
       <c r="C16" s="128"/>
       <c r="D16" s="106" t="s">
         <v>479</v>
@@ -31925,10 +31939,10 @@
       <c r="D17" s="104"/>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="210" t="s">
+      <c r="A18" s="215" t="s">
         <v>337</v>
       </c>
-      <c r="B18" s="211" t="s">
+      <c r="B18" s="196" t="s">
         <v>432</v>
       </c>
       <c r="C18" s="100" t="s">
@@ -31939,8 +31953,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="210"/>
-      <c r="B19" s="211"/>
+      <c r="A19" s="215"/>
+      <c r="B19" s="196"/>
       <c r="C19" s="100" t="s">
         <v>342</v>
       </c>
@@ -31949,8 +31963,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="210"/>
-      <c r="B20" s="211"/>
+      <c r="A20" s="215"/>
+      <c r="B20" s="196"/>
       <c r="C20" s="100" t="s">
         <v>338</v>
       </c>
@@ -31967,10 +31981,10 @@
       <c r="D21" s="104"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="196" t="s">
+      <c r="A22" s="197" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="198" t="s">
+      <c r="B22" s="200" t="s">
         <v>432</v>
       </c>
       <c r="C22" s="106"/>
@@ -31979,8 +31993,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="197"/>
-      <c r="B23" s="199"/>
+      <c r="A23" s="198"/>
+      <c r="B23" s="201"/>
       <c r="C23" s="70" t="s">
         <v>234</v>
       </c>
@@ -31989,9 +32003,9 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="197"/>
-      <c r="B24" s="199"/>
-      <c r="C24" s="143" t="s">
+      <c r="A24" s="198"/>
+      <c r="B24" s="201"/>
+      <c r="C24" s="142" t="s">
         <v>445</v>
       </c>
       <c r="D24" s="107" t="s">
@@ -31999,9 +32013,9 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="197"/>
-      <c r="B25" s="199"/>
-      <c r="C25" s="142" t="s">
+      <c r="A25" s="198"/>
+      <c r="B25" s="201"/>
+      <c r="C25" s="141" t="s">
         <v>480</v>
       </c>
       <c r="D25" s="136" t="s">
@@ -32009,10 +32023,10 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="196" t="s">
+      <c r="A26" s="197" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="198" t="s">
+      <c r="B26" s="200" t="s">
         <v>432</v>
       </c>
       <c r="C26" s="70" t="s">
@@ -32023,8 +32037,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="197"/>
-      <c r="B27" s="199"/>
+      <c r="A27" s="198"/>
+      <c r="B27" s="201"/>
       <c r="C27" s="131" t="s">
         <v>467</v>
       </c>
@@ -32033,8 +32047,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="201"/>
-      <c r="B28" s="200"/>
+      <c r="A28" s="199"/>
+      <c r="B28" s="202"/>
       <c r="C28" s="137" t="s">
         <v>457</v>
       </c>
@@ -32083,7 +32097,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="213" t="s">
+      <c r="A32" s="211" t="s">
         <v>270</v>
       </c>
       <c r="B32" s="212" t="s">
@@ -32095,7 +32109,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="213"/>
+      <c r="A33" s="211"/>
       <c r="B33" s="212"/>
       <c r="C33" s="106"/>
       <c r="D33" s="106" t="s">
@@ -32103,7 +32117,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="213"/>
+      <c r="A34" s="211"/>
       <c r="B34" s="212"/>
       <c r="C34" s="110" t="s">
         <v>320</v>
@@ -32113,7 +32127,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="213"/>
+      <c r="A35" s="211"/>
       <c r="B35" s="212"/>
       <c r="C35" s="111" t="s">
         <v>399</v>
@@ -32135,10 +32149,10 @@
       <c r="D36" s="106"/>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="214" t="s">
+      <c r="A37" s="203" t="s">
         <v>165</v>
       </c>
-      <c r="B37" s="198" t="s">
+      <c r="B37" s="200" t="s">
         <v>432</v>
       </c>
       <c r="C37" s="106"/>
@@ -32147,8 +32161,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="215"/>
-      <c r="B38" s="199"/>
+      <c r="A38" s="204"/>
+      <c r="B38" s="201"/>
       <c r="C38" s="111" t="s">
         <v>356</v>
       </c>
@@ -32157,8 +32171,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="215"/>
-      <c r="B39" s="199"/>
+      <c r="A39" s="204"/>
+      <c r="B39" s="201"/>
       <c r="C39" s="111" t="s">
         <v>354</v>
       </c>
@@ -32167,8 +32181,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="215"/>
-      <c r="B40" s="199"/>
+      <c r="A40" s="204"/>
+      <c r="B40" s="201"/>
       <c r="C40" s="114" t="s">
         <v>362</v>
       </c>
@@ -32177,8 +32191,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="215"/>
-      <c r="B41" s="199"/>
+      <c r="A41" s="204"/>
+      <c r="B41" s="201"/>
       <c r="C41" s="111" t="s">
         <v>354</v>
       </c>
@@ -32187,8 +32201,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="215"/>
-      <c r="B42" s="199"/>
+      <c r="A42" s="204"/>
+      <c r="B42" s="201"/>
       <c r="C42" s="111" t="s">
         <v>366</v>
       </c>
@@ -32197,8 +32211,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="215"/>
-      <c r="B43" s="199"/>
+      <c r="A43" s="204"/>
+      <c r="B43" s="201"/>
       <c r="C43" s="111" t="s">
         <v>354</v>
       </c>
@@ -32207,8 +32221,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="215"/>
-      <c r="B44" s="199"/>
+      <c r="A44" s="204"/>
+      <c r="B44" s="201"/>
       <c r="C44" s="130" t="s">
         <v>461</v>
       </c>
@@ -32217,8 +32231,8 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="215"/>
-      <c r="B45" s="199"/>
+      <c r="A45" s="204"/>
+      <c r="B45" s="201"/>
       <c r="C45" s="130" t="s">
         <v>456</v>
       </c>
@@ -32227,8 +32241,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="215"/>
-      <c r="B46" s="199"/>
+      <c r="A46" s="204"/>
+      <c r="B46" s="201"/>
       <c r="C46" s="130" t="s">
         <v>354</v>
       </c>
@@ -32237,8 +32251,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="215"/>
-      <c r="B47" s="199"/>
+      <c r="A47" s="204"/>
+      <c r="B47" s="201"/>
       <c r="C47" s="130" t="s">
         <v>456</v>
       </c>
@@ -32247,9 +32261,9 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="215"/>
-      <c r="B48" s="199"/>
-      <c r="C48" s="141" t="s">
+      <c r="A48" s="204"/>
+      <c r="B48" s="201"/>
+      <c r="C48" s="140" t="s">
         <v>354</v>
       </c>
       <c r="D48" s="136" t="s">
@@ -32257,9 +32271,9 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="215"/>
-      <c r="B49" s="199"/>
-      <c r="C49" s="141" t="s">
+      <c r="A49" s="204"/>
+      <c r="B49" s="201"/>
+      <c r="C49" s="140" t="s">
         <v>480</v>
       </c>
       <c r="D49" s="136" t="s">
@@ -32293,10 +32307,10 @@
       <c r="D51" s="112"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="202" t="s">
+      <c r="A52" s="205" t="s">
         <v>364</v>
       </c>
-      <c r="B52" s="198" t="s">
+      <c r="B52" s="200" t="s">
         <v>432</v>
       </c>
       <c r="C52" s="111" t="s">
@@ -32305,8 +32319,8 @@
       <c r="D52" s="112"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="203"/>
-      <c r="B53" s="200"/>
+      <c r="A53" s="218"/>
+      <c r="B53" s="202"/>
       <c r="C53" s="111" t="s">
         <v>399</v>
       </c>
@@ -32323,10 +32337,10 @@
       <c r="D54" s="103"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="202" t="s">
+      <c r="A55" s="205" t="s">
         <v>236</v>
       </c>
-      <c r="B55" s="198" t="s">
+      <c r="B55" s="200" t="s">
         <v>432</v>
       </c>
       <c r="C55" s="106"/>
@@ -32335,24 +32349,24 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="204"/>
-      <c r="B56" s="199"/>
+      <c r="A56" s="206"/>
+      <c r="B56" s="201"/>
       <c r="C56" s="106"/>
       <c r="D56" s="106" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="204"/>
-      <c r="B57" s="199"/>
+      <c r="A57" s="206"/>
+      <c r="B57" s="201"/>
       <c r="C57" s="106"/>
       <c r="D57" s="106" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="204"/>
-      <c r="B58" s="199"/>
+      <c r="A58" s="206"/>
+      <c r="B58" s="201"/>
       <c r="C58" s="106" t="s">
         <v>295</v>
       </c>
@@ -32361,8 +32375,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="204"/>
-      <c r="B59" s="199"/>
+      <c r="A59" s="206"/>
+      <c r="B59" s="201"/>
       <c r="C59" s="106" t="s">
         <v>323</v>
       </c>
@@ -32371,8 +32385,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="204"/>
-      <c r="B60" s="199"/>
+      <c r="A60" s="206"/>
+      <c r="B60" s="201"/>
       <c r="C60" s="106" t="s">
         <v>368</v>
       </c>
@@ -32381,8 +32395,8 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="204"/>
-      <c r="B61" s="199"/>
+      <c r="A61" s="206"/>
+      <c r="B61" s="201"/>
       <c r="C61" s="61" t="s">
         <v>472</v>
       </c>
@@ -32391,8 +32405,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="204"/>
-      <c r="B62" s="199"/>
+      <c r="A62" s="206"/>
+      <c r="B62" s="201"/>
       <c r="C62" s="58" t="s">
         <v>37</v>
       </c>
@@ -32401,8 +32415,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="204"/>
-      <c r="B63" s="199"/>
+      <c r="A63" s="206"/>
+      <c r="B63" s="201"/>
       <c r="C63" s="138" t="s">
         <v>354</v>
       </c>
@@ -32411,8 +32425,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="204"/>
-      <c r="B64" s="199"/>
+      <c r="A64" s="206"/>
+      <c r="B64" s="201"/>
       <c r="C64" s="138" t="s">
         <v>456</v>
       </c>
@@ -32421,8 +32435,8 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="204"/>
-      <c r="B65" s="199"/>
+      <c r="A65" s="206"/>
+      <c r="B65" s="201"/>
       <c r="C65" s="138" t="s">
         <v>480</v>
       </c>
@@ -32431,10 +32445,10 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="205" t="s">
+      <c r="A66" s="208" t="s">
         <v>27</v>
       </c>
-      <c r="B66" s="198" t="s">
+      <c r="B66" s="200" t="s">
         <v>432</v>
       </c>
       <c r="C66" s="106" t="s">
@@ -32445,16 +32459,16 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="206"/>
-      <c r="B67" s="199"/>
+      <c r="A67" s="209"/>
+      <c r="B67" s="201"/>
       <c r="C67" s="106"/>
       <c r="D67" s="106" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="206"/>
-      <c r="B68" s="199"/>
+      <c r="A68" s="209"/>
+      <c r="B68" s="201"/>
       <c r="C68" s="116" t="s">
         <v>324</v>
       </c>
@@ -32463,8 +32477,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="206"/>
-      <c r="B69" s="199"/>
+      <c r="A69" s="209"/>
+      <c r="B69" s="201"/>
       <c r="C69" s="116" t="s">
         <v>354</v>
       </c>
@@ -32473,8 +32487,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="206"/>
-      <c r="B70" s="199"/>
+      <c r="A70" s="209"/>
+      <c r="B70" s="201"/>
       <c r="C70" s="116" t="s">
         <v>362</v>
       </c>
@@ -32483,8 +32497,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="206"/>
-      <c r="B71" s="199"/>
+      <c r="A71" s="209"/>
+      <c r="B71" s="201"/>
       <c r="C71" s="116" t="s">
         <v>366</v>
       </c>
@@ -32493,8 +32507,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A72" s="206"/>
-      <c r="B72" s="199"/>
+      <c r="A72" s="209"/>
+      <c r="B72" s="201"/>
       <c r="C72" s="116" t="s">
         <v>376</v>
       </c>
@@ -32503,8 +32517,8 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="206"/>
-      <c r="B73" s="199"/>
+      <c r="A73" s="209"/>
+      <c r="B73" s="201"/>
       <c r="C73" s="108" t="s">
         <v>354</v>
       </c>
@@ -32513,8 +32527,8 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="206"/>
-      <c r="B74" s="199"/>
+      <c r="A74" s="209"/>
+      <c r="B74" s="201"/>
       <c r="C74" s="138" t="s">
         <v>461</v>
       </c>
@@ -32523,8 +32537,8 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="206"/>
-      <c r="B75" s="199"/>
+      <c r="A75" s="209"/>
+      <c r="B75" s="201"/>
       <c r="C75" s="138" t="s">
         <v>456</v>
       </c>
@@ -32533,8 +32547,8 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="206"/>
-      <c r="B76" s="199"/>
+      <c r="A76" s="209"/>
+      <c r="B76" s="201"/>
       <c r="C76" s="138" t="s">
         <v>354</v>
       </c>
@@ -32543,8 +32557,8 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="206"/>
-      <c r="B77" s="199"/>
+      <c r="A77" s="209"/>
+      <c r="B77" s="201"/>
       <c r="C77" s="138" t="s">
         <v>456</v>
       </c>
@@ -32553,8 +32567,8 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="206"/>
-      <c r="B78" s="199"/>
+      <c r="A78" s="209"/>
+      <c r="B78" s="201"/>
       <c r="C78" s="138" t="s">
         <v>368</v>
       </c>
@@ -32563,8 +32577,8 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="206"/>
-      <c r="B79" s="199"/>
+      <c r="A79" s="209"/>
+      <c r="B79" s="201"/>
       <c r="C79" s="138" t="s">
         <v>354</v>
       </c>
@@ -32573,8 +32587,8 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="207"/>
-      <c r="B80" s="200"/>
+      <c r="A80" s="210"/>
+      <c r="B80" s="202"/>
       <c r="C80" s="138" t="s">
         <v>480</v>
       </c>
@@ -32583,13 +32597,13 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="196" t="s">
+      <c r="A81" s="197" t="s">
         <v>222</v>
       </c>
-      <c r="B81" s="198" t="s">
+      <c r="B81" s="200" t="s">
         <v>432</v>
       </c>
-      <c r="C81" s="194" t="s">
+      <c r="C81" s="216" t="s">
         <v>238</v>
       </c>
       <c r="D81" s="96" t="s">
@@ -32597,17 +32611,17 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="197"/>
-      <c r="B82" s="199"/>
-      <c r="C82" s="195"/>
+      <c r="A82" s="198"/>
+      <c r="B82" s="201"/>
+      <c r="C82" s="217"/>
       <c r="D82" s="112" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="197"/>
-      <c r="B83" s="199"/>
-      <c r="C83" s="216" t="s">
+      <c r="A83" s="198"/>
+      <c r="B83" s="201"/>
+      <c r="C83" s="207" t="s">
         <v>239</v>
       </c>
       <c r="D83" s="106" t="s">
@@ -32615,16 +32629,16 @@
       </c>
     </row>
     <row r="84" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A84" s="197"/>
-      <c r="B84" s="199"/>
-      <c r="C84" s="216"/>
+      <c r="A84" s="198"/>
+      <c r="B84" s="201"/>
+      <c r="C84" s="207"/>
       <c r="D84" s="118" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="197"/>
-      <c r="B85" s="199"/>
+      <c r="A85" s="198"/>
+      <c r="B85" s="201"/>
       <c r="C85" s="111" t="s">
         <v>302</v>
       </c>
@@ -32633,8 +32647,8 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="197"/>
-      <c r="B86" s="199"/>
+      <c r="A86" s="198"/>
+      <c r="B86" s="201"/>
       <c r="C86" s="111">
         <v>2.1</v>
       </c>
@@ -32643,8 +32657,8 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="197"/>
-      <c r="B87" s="199"/>
+      <c r="A87" s="198"/>
+      <c r="B87" s="201"/>
       <c r="C87" s="111" t="s">
         <v>238</v>
       </c>
@@ -32653,8 +32667,8 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="197"/>
-      <c r="B88" s="199"/>
+      <c r="A88" s="198"/>
+      <c r="B88" s="201"/>
       <c r="C88" s="111" t="s">
         <v>238</v>
       </c>
@@ -32663,8 +32677,8 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="197"/>
-      <c r="B89" s="199"/>
+      <c r="A89" s="198"/>
+      <c r="B89" s="201"/>
       <c r="C89" s="111" t="s">
         <v>238</v>
       </c>
@@ -32673,8 +32687,8 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="197"/>
-      <c r="B90" s="199"/>
+      <c r="A90" s="198"/>
+      <c r="B90" s="201"/>
       <c r="C90" s="119" t="s">
         <v>373</v>
       </c>
@@ -32683,8 +32697,8 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="197"/>
-      <c r="B91" s="199"/>
+      <c r="A91" s="198"/>
+      <c r="B91" s="201"/>
       <c r="C91" s="111">
         <v>2.1</v>
       </c>
@@ -32693,8 +32707,8 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="197"/>
-      <c r="B92" s="199"/>
+      <c r="A92" s="198"/>
+      <c r="B92" s="201"/>
       <c r="C92" s="111" t="s">
         <v>238</v>
       </c>
@@ -32703,8 +32717,8 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="197"/>
-      <c r="B93" s="199"/>
+      <c r="A93" s="198"/>
+      <c r="B93" s="201"/>
       <c r="C93" s="111" t="s">
         <v>238</v>
       </c>
@@ -32713,8 +32727,8 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="197"/>
-      <c r="B94" s="199"/>
+      <c r="A94" s="198"/>
+      <c r="B94" s="201"/>
       <c r="C94" s="111">
         <v>2.1</v>
       </c>
@@ -32723,10 +32737,10 @@
       </c>
     </row>
     <row r="95" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="205" t="s">
+      <c r="A95" s="208" t="s">
         <v>291</v>
       </c>
-      <c r="B95" s="198" t="s">
+      <c r="B95" s="200" t="s">
         <v>432</v>
       </c>
       <c r="C95" s="106" t="s">
@@ -32737,8 +32751,8 @@
       </c>
     </row>
     <row r="96" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A96" s="206"/>
-      <c r="B96" s="199"/>
+      <c r="A96" s="209"/>
+      <c r="B96" s="201"/>
       <c r="C96" s="118" t="s">
         <v>276</v>
       </c>
@@ -32747,8 +32761,8 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="207"/>
-      <c r="B97" s="200"/>
+      <c r="A97" s="210"/>
+      <c r="B97" s="202"/>
       <c r="C97" s="106" t="s">
         <v>345</v>
       </c>
@@ -32757,10 +32771,10 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="202" t="s">
+      <c r="A98" s="205" t="s">
         <v>365</v>
       </c>
-      <c r="B98" s="198" t="s">
+      <c r="B98" s="200" t="s">
         <v>432</v>
       </c>
       <c r="C98" s="111" t="s">
@@ -32769,8 +32783,8 @@
       <c r="D98" s="106"/>
     </row>
     <row r="99" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="204"/>
-      <c r="B99" s="199"/>
+      <c r="A99" s="206"/>
+      <c r="B99" s="201"/>
       <c r="C99" s="111" t="s">
         <v>373</v>
       </c>
@@ -32779,8 +32793,8 @@
       </c>
     </row>
     <row r="100" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="204"/>
-      <c r="B100" s="199"/>
+      <c r="A100" s="206"/>
+      <c r="B100" s="201"/>
       <c r="C100" s="111">
         <v>2.1</v>
       </c>
@@ -32789,8 +32803,8 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="204"/>
-      <c r="B101" s="199"/>
+      <c r="A101" s="206"/>
+      <c r="B101" s="201"/>
       <c r="C101" s="111" t="s">
         <v>239</v>
       </c>
@@ -32799,8 +32813,8 @@
       </c>
     </row>
     <row r="102" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="204"/>
-      <c r="B102" s="199"/>
+      <c r="A102" s="206"/>
+      <c r="B102" s="201"/>
       <c r="C102" s="111" t="s">
         <v>238</v>
       </c>
@@ -32829,10 +32843,10 @@
       <c r="D104" s="112"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="196" t="s">
+      <c r="A105" s="197" t="s">
         <v>256</v>
       </c>
-      <c r="B105" s="198" t="s">
+      <c r="B105" s="200" t="s">
         <v>432</v>
       </c>
       <c r="C105" s="106"/>
@@ -32841,24 +32855,24 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="197"/>
-      <c r="B106" s="199"/>
+      <c r="A106" s="198"/>
+      <c r="B106" s="201"/>
       <c r="C106" s="106"/>
       <c r="D106" s="106" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="197"/>
-      <c r="B107" s="199"/>
+      <c r="A107" s="198"/>
+      <c r="B107" s="201"/>
       <c r="C107" s="106"/>
       <c r="D107" s="112" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="197"/>
-      <c r="B108" s="199"/>
+      <c r="A108" s="198"/>
+      <c r="B108" s="201"/>
       <c r="C108" s="106" t="s">
         <v>419</v>
       </c>
@@ -32867,8 +32881,8 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="197"/>
-      <c r="B109" s="199"/>
+      <c r="A109" s="198"/>
+      <c r="B109" s="201"/>
       <c r="C109" s="106" t="s">
         <v>424</v>
       </c>
@@ -32877,8 +32891,8 @@
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="197"/>
-      <c r="B110" s="199"/>
+      <c r="A110" s="198"/>
+      <c r="B110" s="201"/>
       <c r="C110" s="58" t="s">
         <v>474</v>
       </c>
@@ -32887,8 +32901,8 @@
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="197"/>
-      <c r="B111" s="199"/>
+      <c r="A111" s="198"/>
+      <c r="B111" s="201"/>
       <c r="C111" s="58" t="s">
         <v>480</v>
       </c>
@@ -32897,7 +32911,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="213" t="s">
+      <c r="A112" s="211" t="s">
         <v>329</v>
       </c>
       <c r="B112" s="212" t="s">
@@ -32911,7 +32925,7 @@
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="213"/>
+      <c r="A113" s="211"/>
       <c r="B113" s="212"/>
       <c r="C113" s="106" t="s">
         <v>406</v>
@@ -32921,41 +32935,41 @@
       </c>
     </row>
     <row r="114" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A114" s="213"/>
+      <c r="A114" s="211"/>
       <c r="B114" s="212"/>
       <c r="C114" s="121" t="s">
         <v>409</v>
       </c>
-      <c r="D114" s="202" t="s">
+      <c r="D114" s="205" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A115" s="213"/>
+      <c r="A115" s="211"/>
       <c r="B115" s="212"/>
       <c r="C115" s="121" t="s">
         <v>410</v>
       </c>
-      <c r="D115" s="204"/>
+      <c r="D115" s="206"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="213"/>
+      <c r="A116" s="211"/>
       <c r="B116" s="212"/>
       <c r="C116" s="121" t="s">
         <v>411</v>
       </c>
-      <c r="D116" s="204"/>
+      <c r="D116" s="206"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="213"/>
+      <c r="A117" s="211"/>
       <c r="B117" s="212"/>
       <c r="C117" s="121" t="s">
         <v>412</v>
       </c>
-      <c r="D117" s="204"/>
+      <c r="D117" s="206"/>
     </row>
     <row r="118" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="213"/>
+      <c r="A118" s="211"/>
       <c r="B118" s="212"/>
       <c r="C118" s="139" t="s">
         <v>475</v>
@@ -32979,10 +32993,10 @@
       </c>
     </row>
     <row r="120" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="205" t="s">
+      <c r="A120" s="208" t="s">
         <v>32</v>
       </c>
-      <c r="B120" s="198" t="s">
+      <c r="B120" s="200" t="s">
         <v>432</v>
       </c>
       <c r="C120" s="106" t="s">
@@ -32993,8 +33007,8 @@
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="206"/>
-      <c r="B121" s="199"/>
+      <c r="A121" s="209"/>
+      <c r="B121" s="201"/>
       <c r="C121" s="106" t="s">
         <v>265</v>
       </c>
@@ -33003,8 +33017,8 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="206"/>
-      <c r="B122" s="199"/>
+      <c r="A122" s="209"/>
+      <c r="B122" s="201"/>
       <c r="C122" s="106" t="s">
         <v>264</v>
       </c>
@@ -33013,8 +33027,8 @@
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="206"/>
-      <c r="B123" s="199"/>
+      <c r="A123" s="209"/>
+      <c r="B123" s="201"/>
       <c r="C123" s="112" t="s">
         <v>272</v>
       </c>
@@ -33023,8 +33037,8 @@
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="206"/>
-      <c r="B124" s="199"/>
+      <c r="A124" s="209"/>
+      <c r="B124" s="201"/>
       <c r="C124" s="106" t="s">
         <v>277</v>
       </c>
@@ -33033,8 +33047,8 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="206"/>
-      <c r="B125" s="199"/>
+      <c r="A125" s="209"/>
+      <c r="B125" s="201"/>
       <c r="C125" s="106" t="s">
         <v>278</v>
       </c>
@@ -33043,8 +33057,8 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="206"/>
-      <c r="B126" s="199"/>
+      <c r="A126" s="209"/>
+      <c r="B126" s="201"/>
       <c r="C126" s="112" t="s">
         <v>283</v>
       </c>
@@ -33053,8 +33067,8 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="206"/>
-      <c r="B127" s="199"/>
+      <c r="A127" s="209"/>
+      <c r="B127" s="201"/>
       <c r="C127" s="112" t="s">
         <v>297</v>
       </c>
@@ -33063,8 +33077,8 @@
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="206"/>
-      <c r="B128" s="199"/>
+      <c r="A128" s="209"/>
+      <c r="B128" s="201"/>
       <c r="C128" s="112" t="s">
         <v>284</v>
       </c>
@@ -33073,8 +33087,8 @@
       </c>
     </row>
     <row r="129" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A129" s="206"/>
-      <c r="B129" s="199"/>
+      <c r="A129" s="209"/>
+      <c r="B129" s="201"/>
       <c r="C129" s="122" t="s">
         <v>243</v>
       </c>
@@ -33083,8 +33097,8 @@
       </c>
     </row>
     <row r="130" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A130" s="206"/>
-      <c r="B130" s="199"/>
+      <c r="A130" s="209"/>
+      <c r="B130" s="201"/>
       <c r="C130" s="116" t="s">
         <v>306</v>
       </c>
@@ -33093,8 +33107,8 @@
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="206"/>
-      <c r="B131" s="199"/>
+      <c r="A131" s="209"/>
+      <c r="B131" s="201"/>
       <c r="C131" s="106" t="s">
         <v>307</v>
       </c>
@@ -33103,8 +33117,8 @@
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="206"/>
-      <c r="B132" s="199"/>
+      <c r="A132" s="209"/>
+      <c r="B132" s="201"/>
       <c r="C132" s="112" t="s">
         <v>308</v>
       </c>
@@ -33113,8 +33127,8 @@
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="206"/>
-      <c r="B133" s="199"/>
+      <c r="A133" s="209"/>
+      <c r="B133" s="201"/>
       <c r="C133" s="112" t="s">
         <v>310</v>
       </c>
@@ -33123,8 +33137,8 @@
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="206"/>
-      <c r="B134" s="199"/>
+      <c r="A134" s="209"/>
+      <c r="B134" s="201"/>
       <c r="C134" s="112" t="s">
         <v>263</v>
       </c>
@@ -33133,8 +33147,8 @@
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="206"/>
-      <c r="B135" s="199"/>
+      <c r="A135" s="209"/>
+      <c r="B135" s="201"/>
       <c r="C135" s="106" t="s">
         <v>313</v>
       </c>
@@ -33143,8 +33157,8 @@
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="206"/>
-      <c r="B136" s="199"/>
+      <c r="A136" s="209"/>
+      <c r="B136" s="201"/>
       <c r="C136" s="112" t="s">
         <v>278</v>
       </c>
@@ -33153,8 +33167,8 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="206"/>
-      <c r="B137" s="199"/>
+      <c r="A137" s="209"/>
+      <c r="B137" s="201"/>
       <c r="C137" s="112" t="s">
         <v>314</v>
       </c>
@@ -33163,16 +33177,16 @@
       </c>
     </row>
     <row r="138" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A138" s="206"/>
-      <c r="B138" s="199"/>
+      <c r="A138" s="209"/>
+      <c r="B138" s="201"/>
       <c r="C138" s="106"/>
       <c r="D138" s="97" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="206"/>
-      <c r="B139" s="199"/>
+      <c r="A139" s="209"/>
+      <c r="B139" s="201"/>
       <c r="C139" s="112" t="s">
         <v>317</v>
       </c>
@@ -33181,8 +33195,8 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="206"/>
-      <c r="B140" s="199"/>
+      <c r="A140" s="209"/>
+      <c r="B140" s="201"/>
       <c r="C140" s="112" t="s">
         <v>263</v>
       </c>
@@ -33191,8 +33205,8 @@
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="206"/>
-      <c r="B141" s="199"/>
+      <c r="A141" s="209"/>
+      <c r="B141" s="201"/>
       <c r="C141" s="112" t="s">
         <v>334</v>
       </c>
@@ -33201,8 +33215,8 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="206"/>
-      <c r="B142" s="199"/>
+      <c r="A142" s="209"/>
+      <c r="B142" s="201"/>
       <c r="C142" s="112" t="s">
         <v>335</v>
       </c>
@@ -33211,8 +33225,8 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="206"/>
-      <c r="B143" s="199"/>
+      <c r="A143" s="209"/>
+      <c r="B143" s="201"/>
       <c r="C143" s="112" t="s">
         <v>319</v>
       </c>
@@ -33221,8 +33235,8 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="206"/>
-      <c r="B144" s="199"/>
+      <c r="A144" s="209"/>
+      <c r="B144" s="201"/>
       <c r="C144" s="117" t="s">
         <v>340</v>
       </c>
@@ -33231,8 +33245,8 @@
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A145" s="206"/>
-      <c r="B145" s="199"/>
+      <c r="A145" s="209"/>
+      <c r="B145" s="201"/>
       <c r="C145" s="112" t="s">
         <v>333</v>
       </c>
@@ -33241,8 +33255,8 @@
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="206"/>
-      <c r="B146" s="199"/>
+      <c r="A146" s="209"/>
+      <c r="B146" s="201"/>
       <c r="C146" s="112" t="s">
         <v>348</v>
       </c>
@@ -33251,8 +33265,8 @@
       </c>
     </row>
     <row r="147" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A147" s="206"/>
-      <c r="B147" s="199"/>
+      <c r="A147" s="209"/>
+      <c r="B147" s="201"/>
       <c r="C147" s="101" t="s">
         <v>351</v>
       </c>
@@ -33261,8 +33275,8 @@
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="206"/>
-      <c r="B148" s="199"/>
+      <c r="A148" s="209"/>
+      <c r="B148" s="201"/>
       <c r="C148" s="112" t="s">
         <v>352</v>
       </c>
@@ -33271,8 +33285,8 @@
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="206"/>
-      <c r="B149" s="199"/>
+      <c r="A149" s="209"/>
+      <c r="B149" s="201"/>
       <c r="C149" s="112" t="s">
         <v>353</v>
       </c>
@@ -33281,8 +33295,8 @@
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="206"/>
-      <c r="B150" s="199"/>
+      <c r="A150" s="209"/>
+      <c r="B150" s="201"/>
       <c r="C150" s="112" t="s">
         <v>359</v>
       </c>
@@ -33291,8 +33305,8 @@
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="206"/>
-      <c r="B151" s="199"/>
+      <c r="A151" s="209"/>
+      <c r="B151" s="201"/>
       <c r="C151" s="112" t="s">
         <v>361</v>
       </c>
@@ -33301,8 +33315,8 @@
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="206"/>
-      <c r="B152" s="199"/>
+      <c r="A152" s="209"/>
+      <c r="B152" s="201"/>
       <c r="C152" s="112" t="s">
         <v>367</v>
       </c>
@@ -33311,8 +33325,8 @@
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="206"/>
-      <c r="B153" s="199"/>
+      <c r="A153" s="209"/>
+      <c r="B153" s="201"/>
       <c r="C153" s="112" t="s">
         <v>359</v>
       </c>
@@ -33321,8 +33335,8 @@
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="206"/>
-      <c r="B154" s="199"/>
+      <c r="A154" s="209"/>
+      <c r="B154" s="201"/>
       <c r="C154" s="117" t="s">
         <v>380</v>
       </c>
@@ -33331,8 +33345,8 @@
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="206"/>
-      <c r="B155" s="199"/>
+      <c r="A155" s="209"/>
+      <c r="B155" s="201"/>
       <c r="C155" s="106" t="s">
         <v>384</v>
       </c>
@@ -33341,8 +33355,8 @@
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="206"/>
-      <c r="B156" s="199"/>
+      <c r="A156" s="209"/>
+      <c r="B156" s="201"/>
       <c r="C156" s="106" t="s">
         <v>387</v>
       </c>
@@ -33351,8 +33365,8 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="206"/>
-      <c r="B157" s="199"/>
+      <c r="A157" s="209"/>
+      <c r="B157" s="201"/>
       <c r="C157" s="106" t="s">
         <v>388</v>
       </c>
@@ -33361,8 +33375,8 @@
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="206"/>
-      <c r="B158" s="199"/>
+      <c r="A158" s="209"/>
+      <c r="B158" s="201"/>
       <c r="C158" s="106" t="s">
         <v>389</v>
       </c>
@@ -33371,8 +33385,8 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="206"/>
-      <c r="B159" s="199"/>
+      <c r="A159" s="209"/>
+      <c r="B159" s="201"/>
       <c r="C159" s="106" t="s">
         <v>390</v>
       </c>
@@ -33381,8 +33395,8 @@
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="206"/>
-      <c r="B160" s="199"/>
+      <c r="A160" s="209"/>
+      <c r="B160" s="201"/>
       <c r="C160" s="106" t="s">
         <v>391</v>
       </c>
@@ -33391,8 +33405,8 @@
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="206"/>
-      <c r="B161" s="199"/>
+      <c r="A161" s="209"/>
+      <c r="B161" s="201"/>
       <c r="C161" s="106" t="s">
         <v>394</v>
       </c>
@@ -33401,8 +33415,8 @@
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="206"/>
-      <c r="B162" s="199"/>
+      <c r="A162" s="209"/>
+      <c r="B162" s="201"/>
       <c r="C162" s="106" t="s">
         <v>404</v>
       </c>
@@ -33411,8 +33425,8 @@
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="206"/>
-      <c r="B163" s="199"/>
+      <c r="A163" s="209"/>
+      <c r="B163" s="201"/>
       <c r="C163" s="106" t="s">
         <v>405</v>
       </c>
@@ -33421,8 +33435,8 @@
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="206"/>
-      <c r="B164" s="199"/>
+      <c r="A164" s="209"/>
+      <c r="B164" s="201"/>
       <c r="C164" s="106" t="s">
         <v>422</v>
       </c>
@@ -33431,8 +33445,8 @@
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="206"/>
-      <c r="B165" s="199"/>
+      <c r="A165" s="209"/>
+      <c r="B165" s="201"/>
       <c r="C165" s="106" t="s">
         <v>423</v>
       </c>
@@ -33441,8 +33455,8 @@
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="206"/>
-      <c r="B166" s="199"/>
+      <c r="A166" s="209"/>
+      <c r="B166" s="201"/>
       <c r="C166" s="106" t="s">
         <v>426</v>
       </c>
@@ -33451,8 +33465,8 @@
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="206"/>
-      <c r="B167" s="199"/>
+      <c r="A167" s="209"/>
+      <c r="B167" s="201"/>
       <c r="C167" s="58" t="s">
         <v>477</v>
       </c>
@@ -33461,8 +33475,8 @@
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="206"/>
-      <c r="B168" s="199"/>
+      <c r="A168" s="209"/>
+      <c r="B168" s="201"/>
       <c r="C168" s="106" t="s">
         <v>422</v>
       </c>
@@ -33471,8 +33485,8 @@
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="207"/>
-      <c r="B169" s="200"/>
+      <c r="A169" s="210"/>
+      <c r="B169" s="202"/>
       <c r="C169" s="106" t="s">
         <v>476</v>
       </c>
@@ -33481,10 +33495,10 @@
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="205" t="s">
+      <c r="A170" s="219" t="s">
         <v>416</v>
       </c>
-      <c r="B170" s="198" t="s">
+      <c r="B170" s="200" t="s">
         <v>432</v>
       </c>
       <c r="C170" s="106" t="s">
@@ -33495,32 +33509,28 @@
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="207"/>
-      <c r="B171" s="200"/>
-      <c r="C171" s="140" t="s">
+      <c r="A171" s="220"/>
+      <c r="B171" s="201"/>
+      <c r="C171" s="58" t="s">
         <v>478</v>
       </c>
-      <c r="D171" s="140" t="s">
+      <c r="D171" s="58" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="108" t="s">
+      <c r="A172" s="221"/>
+      <c r="B172" s="202"/>
+      <c r="C172" s="58" t="s">
+        <v>483</v>
+      </c>
+      <c r="D172" s="58" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="108" t="s">
         <v>304</v>
-      </c>
-      <c r="B172" s="70" t="s">
-        <v>432</v>
-      </c>
-      <c r="C172" s="106" t="s">
-        <v>30</v>
-      </c>
-      <c r="D172" s="112" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="108" t="s">
-        <v>305</v>
       </c>
       <c r="B173" s="70" t="s">
         <v>432</v>
@@ -33532,314 +33542,348 @@
         <v>269</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="103" t="s">
+    <row r="174" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="108" t="s">
+        <v>305</v>
+      </c>
+      <c r="B174" s="70" t="s">
+        <v>432</v>
+      </c>
+      <c r="C174" s="106" t="s">
+        <v>30</v>
+      </c>
+      <c r="D174" s="112" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="B174" s="103"/>
-      <c r="C174" s="103"/>
-      <c r="D174" s="104"/>
-    </row>
-    <row r="175" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A175" s="196" t="s">
+      <c r="B175" s="103"/>
+      <c r="C175" s="103"/>
+      <c r="D175" s="104"/>
+    </row>
+    <row r="176" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="197" t="s">
         <v>84</v>
       </c>
-      <c r="B175" s="198" t="s">
+      <c r="B176" s="200" t="s">
         <v>432</v>
       </c>
-      <c r="C175" s="106"/>
-      <c r="D175" s="80" t="s">
+      <c r="C176" s="106"/>
+      <c r="D176" s="80" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="197"/>
-      <c r="B176" s="199"/>
-      <c r="C176" s="70" t="s">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="198"/>
+      <c r="B177" s="201"/>
+      <c r="C177" s="70" t="s">
         <v>245</v>
       </c>
-      <c r="D176" s="106" t="s">
+      <c r="D177" s="106" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="197"/>
-      <c r="B177" s="199"/>
-      <c r="C177" s="70">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="198"/>
+      <c r="B178" s="201"/>
+      <c r="C178" s="70">
         <v>10.1</v>
-      </c>
-      <c r="D177" s="106" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="197"/>
-      <c r="B178" s="199"/>
-      <c r="C178" s="70">
-        <v>10.199999999999999</v>
       </c>
       <c r="D178" s="106" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="197"/>
-      <c r="B179" s="199"/>
-      <c r="C179" s="98" t="s">
+      <c r="A179" s="198"/>
+      <c r="B179" s="201"/>
+      <c r="C179" s="70">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="D179" s="106" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="198"/>
+      <c r="B180" s="201"/>
+      <c r="C180" s="98" t="s">
         <v>288</v>
       </c>
-      <c r="D179" s="95" t="s">
+      <c r="D180" s="95" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="197"/>
-      <c r="B180" s="199"/>
-      <c r="C180" s="98" t="s">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="198"/>
+      <c r="B181" s="201"/>
+      <c r="C181" s="98" t="s">
         <v>370</v>
       </c>
-      <c r="D180" s="95" t="s">
+      <c r="D181" s="95" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="197"/>
-      <c r="B181" s="199"/>
-      <c r="C181" s="98" t="s">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="198"/>
+      <c r="B182" s="201"/>
+      <c r="C182" s="98" t="s">
         <v>117</v>
       </c>
-      <c r="D181" s="95" t="s">
+      <c r="D182" s="95" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="197"/>
-      <c r="B182" s="199"/>
-      <c r="C182" s="98" t="s">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="198"/>
+      <c r="B183" s="201"/>
+      <c r="C183" s="98" t="s">
         <v>417</v>
       </c>
-      <c r="D182" s="95" t="s">
+      <c r="D183" s="95" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="197"/>
-      <c r="B183" s="199"/>
-      <c r="C183" s="98" t="s">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="198"/>
+      <c r="B184" s="201"/>
+      <c r="C184" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="D183" s="95" t="s">
+      <c r="D184" s="95" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="184" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A184" s="201"/>
-      <c r="B184" s="200"/>
-      <c r="C184" s="98" t="s">
+    <row r="185" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A185" s="199"/>
+      <c r="B185" s="202"/>
+      <c r="C185" s="98" t="s">
         <v>460</v>
       </c>
-      <c r="D184" s="135" t="s">
+      <c r="D185" s="135" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="196" t="s">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="197" t="s">
         <v>246</v>
       </c>
-      <c r="B185" s="198" t="s">
+      <c r="B186" s="200" t="s">
         <v>432</v>
       </c>
-      <c r="C185" s="98"/>
-      <c r="D185" s="124" t="s">
+      <c r="C186" s="98"/>
+      <c r="D186" s="124" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="197"/>
-      <c r="B186" s="199"/>
-      <c r="C186" s="125" t="s">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="198"/>
+      <c r="B187" s="201"/>
+      <c r="C187" s="125" t="s">
         <v>428</v>
       </c>
-      <c r="D186" s="102" t="s">
+      <c r="D187" s="102" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="187" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A187" s="109" t="s">
+    <row r="188" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="109" t="s">
         <v>257</v>
       </c>
-      <c r="B187" s="70" t="s">
+      <c r="B188" s="70" t="s">
         <v>432</v>
       </c>
-      <c r="C187" s="134" t="s">
+      <c r="C188" s="134" t="s">
         <v>249</v>
       </c>
-      <c r="D187" s="112" t="s">
+      <c r="D188" s="112" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="127" t="s">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="127" t="s">
         <v>56</v>
       </c>
-      <c r="B188" s="127"/>
-      <c r="C188" s="127"/>
-      <c r="D188" s="127"/>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="196" t="s">
+      <c r="B189" s="127"/>
+      <c r="C189" s="127"/>
+      <c r="D189" s="127"/>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" s="197" t="s">
         <v>58</v>
       </c>
-      <c r="B189" s="198" t="s">
+      <c r="B190" s="200" t="s">
         <v>266</v>
       </c>
-      <c r="C189" s="128" t="s">
-        <v>260</v>
-      </c>
-      <c r="D189" s="106" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="197"/>
-      <c r="B190" s="199"/>
       <c r="C190" s="128" t="s">
         <v>260</v>
       </c>
       <c r="D190" s="106" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="198"/>
+      <c r="B191" s="201"/>
+      <c r="C191" s="128" t="s">
+        <v>260</v>
+      </c>
+      <c r="D191" s="106" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A191" s="201"/>
-      <c r="B191" s="200"/>
-      <c r="C191" s="106"/>
-      <c r="D191" s="106" t="s">
+    <row r="192" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="199"/>
+      <c r="B192" s="202"/>
+      <c r="C192" s="106"/>
+      <c r="D192" s="106" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A192" s="208" t="s">
+    <row r="193" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A193" s="213" t="s">
         <v>59</v>
       </c>
-      <c r="B192" s="198" t="s">
+      <c r="B193" s="200" t="s">
         <v>266</v>
       </c>
-      <c r="C192" s="118" t="s">
+      <c r="C193" s="118" t="s">
         <v>259</v>
       </c>
-      <c r="D192" s="106" t="s">
+      <c r="D193" s="106" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A193" s="209"/>
-      <c r="B193" s="200"/>
-      <c r="C193" s="118"/>
-      <c r="D193" s="106" t="s">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="214"/>
+      <c r="B194" s="202"/>
+      <c r="C194" s="118"/>
+      <c r="D194" s="106" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A194" s="208" t="s">
+    <row r="195" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A195" s="213" t="s">
         <v>286</v>
       </c>
-      <c r="B194" s="198" t="s">
+      <c r="B195" s="200" t="s">
         <v>266</v>
       </c>
-      <c r="C194" s="118"/>
-      <c r="D194" s="118" t="s">
+      <c r="C195" s="118"/>
+      <c r="D195" s="118" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="209"/>
-      <c r="B195" s="200"/>
-      <c r="C195" s="106"/>
-      <c r="D195" s="106" t="s">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="214"/>
+      <c r="B196" s="202"/>
+      <c r="C196" s="106"/>
+      <c r="D196" s="106" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="196" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A196" s="208" t="s">
+    <row r="197" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A197" s="213" t="s">
         <v>60</v>
       </c>
-      <c r="B196" s="198" t="s">
+      <c r="B197" s="200" t="s">
         <v>266</v>
       </c>
-      <c r="C196" s="118" t="s">
+      <c r="C197" s="118" t="s">
         <v>259</v>
       </c>
-      <c r="D196" s="106" t="s">
+      <c r="D197" s="106" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="209"/>
-      <c r="B197" s="200"/>
-      <c r="C197" s="106"/>
-      <c r="D197" s="106" t="s">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="214"/>
+      <c r="B198" s="202"/>
+      <c r="C198" s="106"/>
+      <c r="D198" s="106" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="127" t="s">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" s="127" t="s">
         <v>268</v>
       </c>
-      <c r="B198" s="127"/>
-      <c r="C198" s="127"/>
-      <c r="D198" s="127"/>
-    </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="106"/>
-      <c r="B199" s="70" t="s">
+      <c r="B199" s="127"/>
+      <c r="C199" s="127"/>
+      <c r="D199" s="127"/>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="106"/>
+      <c r="B200" s="70" t="s">
         <v>432</v>
       </c>
-      <c r="C199" s="106" t="s">
+      <c r="C200" s="106" t="s">
         <v>30</v>
       </c>
-      <c r="D199" s="112" t="s">
+      <c r="D200" s="112" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="127" t="s">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" s="127" t="s">
         <v>274</v>
       </c>
-      <c r="B200" s="127"/>
-      <c r="C200" s="127"/>
-      <c r="D200" s="127"/>
-    </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="106"/>
-      <c r="B201" s="70" t="s">
-        <v>432</v>
-      </c>
-      <c r="C201" s="106" t="s">
-        <v>30</v>
-      </c>
-      <c r="D201" s="112" t="s">
-        <v>269</v>
-      </c>
+      <c r="B201" s="127"/>
+      <c r="C201" s="127"/>
+      <c r="D201" s="127"/>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="106"/>
-      <c r="B202" s="70"/>
+      <c r="B202" s="70" t="s">
+        <v>432</v>
+      </c>
       <c r="C202" s="106" t="s">
+        <v>30</v>
+      </c>
+      <c r="D202" s="112" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="106"/>
+      <c r="B203" s="70"/>
+      <c r="C203" s="106" t="s">
         <v>396</v>
       </c>
-      <c r="D202" s="112" t="s">
+      <c r="D203" s="112" t="s">
         <v>397</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="A37:A49"/>
-    <mergeCell ref="B37:B49"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A26:A28"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="A190:A192"/>
+    <mergeCell ref="B190:B192"/>
+    <mergeCell ref="A176:A185"/>
+    <mergeCell ref="B176:B185"/>
+    <mergeCell ref="A55:A65"/>
+    <mergeCell ref="B55:B65"/>
+    <mergeCell ref="A66:A80"/>
+    <mergeCell ref="B66:B80"/>
+    <mergeCell ref="A120:A169"/>
+    <mergeCell ref="B120:B169"/>
+    <mergeCell ref="A186:A187"/>
+    <mergeCell ref="B186:B187"/>
+    <mergeCell ref="B170:B172"/>
+    <mergeCell ref="A170:A172"/>
+    <mergeCell ref="A197:A198"/>
+    <mergeCell ref="B197:B198"/>
+    <mergeCell ref="A193:A194"/>
+    <mergeCell ref="B193:B194"/>
+    <mergeCell ref="A195:A196"/>
+    <mergeCell ref="B195:B196"/>
     <mergeCell ref="D114:D117"/>
     <mergeCell ref="C83:C84"/>
     <mergeCell ref="A81:A94"/>
@@ -33850,43 +33894,23 @@
     <mergeCell ref="B112:B118"/>
     <mergeCell ref="A98:A102"/>
     <mergeCell ref="B98:B102"/>
+    <mergeCell ref="A105:A111"/>
+    <mergeCell ref="B105:B111"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="A37:A49"/>
+    <mergeCell ref="B37:B49"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A196:A197"/>
-    <mergeCell ref="B196:B197"/>
-    <mergeCell ref="A192:A193"/>
-    <mergeCell ref="B192:B193"/>
-    <mergeCell ref="A194:A195"/>
-    <mergeCell ref="B194:B195"/>
     <mergeCell ref="A18:A20"/>
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A105:A111"/>
-    <mergeCell ref="B105:B111"/>
-    <mergeCell ref="A189:A191"/>
-    <mergeCell ref="B189:B191"/>
-    <mergeCell ref="A175:A184"/>
-    <mergeCell ref="B175:B184"/>
-    <mergeCell ref="A55:A65"/>
-    <mergeCell ref="B55:B65"/>
-    <mergeCell ref="A66:A80"/>
-    <mergeCell ref="B66:B80"/>
-    <mergeCell ref="A170:A171"/>
-    <mergeCell ref="B170:B171"/>
-    <mergeCell ref="A120:A169"/>
-    <mergeCell ref="B120:B169"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="A185:A186"/>
-    <mergeCell ref="B185:B186"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A26:A28"/>
-    <mergeCell ref="B26:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
pit3 and advance payment updates
</commit_message>
<xml_diff>
--- a/PIT3/Schema Publication Changelog.xlsx
+++ b/PIT3/Schema Publication Changelog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ademps03\IdeaProjects\paye-employers-documentation\src\main\resources\PIT3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwalsh06\IdeaProjects\paye-employers-documentation\src\main\resources\PIT3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E4BB29-0183-4945-9860-2FF88940E777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF27A87-3964-4BFA-B8C7-8B314C0A24B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v0.10" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="521">
   <si>
     <t>Document</t>
   </si>
@@ -3370,6 +3370,78 @@
   </si>
   <si>
     <t>added note re. upper limit</t>
+  </si>
+  <si>
+    <t>ERR Technical Support Documentation</t>
+  </si>
+  <si>
+    <t>Enhanced Reporting Requirements Overview</t>
+  </si>
+  <si>
+    <t>Enhanced Reporting Submission Request: Data Items</t>
+  </si>
+  <si>
+    <t>Enhanced Reporting Notification (ERN) Request: Data Items</t>
+  </si>
+  <si>
+    <t>Enhanced Reporting Request Monthly Report: Data Items</t>
+  </si>
+  <si>
+    <t>Enhanced Reporting Validation Rules</t>
+  </si>
+  <si>
+    <t>Enhanced Reporting Web Service Definition</t>
+  </si>
+  <si>
+    <t>Enhanced Reporting Schema</t>
+  </si>
+  <si>
+    <t>ERN Web Service Definition</t>
+  </si>
+  <si>
+    <t>ERN Schema</t>
+  </si>
+  <si>
+    <t>ERR Examples</t>
+  </si>
+  <si>
+    <t>Enhanced Reporting Requirements - Overview of Web Service Examples</t>
+  </si>
+  <si>
+    <t>Example 1: Full ERR Life Cycle</t>
+  </si>
+  <si>
+    <t>Example 2: Overpayment Correction</t>
+  </si>
+  <si>
+    <t>Example 3: Underpayment Correction</t>
+  </si>
+  <si>
+    <t>Example 4: Amendment of Incorrect ERR Submission</t>
+  </si>
+  <si>
+    <t>ERR Example Scenarios</t>
+  </si>
+  <si>
+    <t>ERR Screen Upload Examples</t>
+  </si>
+  <si>
+    <t>ERR File Upload CSV Conversion</t>
+  </si>
+  <si>
+    <t>Screen upload examples</t>
+  </si>
+  <si>
+    <t>ERR_Submission_Agent</t>
+  </si>
+  <si>
+    <t>XML and JSON samples added to illustrate how to include Agent TAIN when trying to submit file upload using an agent cert.</t>
+  </si>
+  <si>
+    <t>LookUpERN_Agent</t>
+  </si>
+  <si>
+    <t>XML and JSON samples added to illustrate how to include Agent TAIN when trying to do LookUpERN using an agent cert.</t>
   </si>
 </sst>
 </file>
@@ -3984,7 +4056,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="233">
+  <cellXfs count="237">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -4325,9 +4397,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4362,23 +4431,8 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4388,6 +4442,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4999,7 +5083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -5029,12 +5113,12 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="154" t="s">
+      <c r="A2" s="158" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="155"/>
-      <c r="C2" s="155"/>
-      <c r="D2" s="156"/>
+      <c r="B2" s="159"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="160"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -5057,12 +5141,12 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="154" t="s">
+      <c r="A4" s="158" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="155"/>
-      <c r="C4" s="155"/>
-      <c r="D4" s="156"/>
+      <c r="B4" s="159"/>
+      <c r="C4" s="159"/>
+      <c r="D4" s="160"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -5102,10 +5186,10 @@
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="157" t="s">
+      <c r="A7" s="161" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="160">
+      <c r="B7" s="164">
         <v>0.1</v>
       </c>
       <c r="C7" s="11" t="s">
@@ -5119,8 +5203,8 @@
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="158"/>
-      <c r="B8" s="161"/>
+      <c r="A8" s="162"/>
+      <c r="B8" s="165"/>
       <c r="C8" s="11" t="s">
         <v>5</v>
       </c>
@@ -5132,8 +5216,8 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="158"/>
-      <c r="B9" s="161"/>
+      <c r="A9" s="162"/>
+      <c r="B9" s="165"/>
       <c r="C9" s="11" t="s">
         <v>6</v>
       </c>
@@ -5145,8 +5229,8 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="158"/>
-      <c r="B10" s="161"/>
+      <c r="A10" s="162"/>
+      <c r="B10" s="165"/>
       <c r="C10" s="11" t="s">
         <v>61</v>
       </c>
@@ -5158,8 +5242,8 @@
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="158"/>
-      <c r="B11" s="161"/>
+      <c r="A11" s="162"/>
+      <c r="B11" s="165"/>
       <c r="C11" s="11" t="s">
         <v>73</v>
       </c>
@@ -5171,8 +5255,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="159"/>
-      <c r="B12" s="162"/>
+      <c r="A12" s="163"/>
+      <c r="B12" s="166"/>
       <c r="C12" s="11" t="s">
         <v>67</v>
       </c>
@@ -5184,10 +5268,10 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="165" t="s">
+      <c r="A13" s="169" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="160">
+      <c r="B13" s="164">
         <v>0.1</v>
       </c>
       <c r="C13" s="11" t="s">
@@ -5201,8 +5285,8 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="166"/>
-      <c r="B14" s="162"/>
+      <c r="A14" s="170"/>
+      <c r="B14" s="166"/>
       <c r="C14" s="11" t="s">
         <v>69</v>
       </c>
@@ -5248,12 +5332,12 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="154" t="s">
+      <c r="A17" s="158" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="155"/>
-      <c r="C17" s="155"/>
-      <c r="D17" s="156"/>
+      <c r="B17" s="159"/>
+      <c r="C17" s="159"/>
+      <c r="D17" s="160"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -5293,21 +5377,21 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="154" t="s">
+      <c r="A20" s="158" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="155"/>
-      <c r="C20" s="155"/>
-      <c r="D20" s="156"/>
+      <c r="B20" s="159"/>
+      <c r="C20" s="159"/>
+      <c r="D20" s="160"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="167" t="s">
+      <c r="A21" s="171" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="164">
+      <c r="B21" s="168">
         <v>0.1</v>
       </c>
       <c r="C21" s="11" t="s">
@@ -5321,8 +5405,8 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="168"/>
-      <c r="B22" s="162"/>
+      <c r="A22" s="172"/>
+      <c r="B22" s="166"/>
       <c r="C22" s="27" t="s">
         <v>37</v>
       </c>
@@ -5345,18 +5429,18 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="154" t="s">
+      <c r="A24" s="158" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="155"/>
-      <c r="C24" s="155"/>
-      <c r="D24" s="156"/>
+      <c r="B24" s="159"/>
+      <c r="C24" s="159"/>
+      <c r="D24" s="160"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="163" t="s">
+      <c r="A25" s="167" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="164">
+      <c r="B25" s="168">
         <v>0.1</v>
       </c>
       <c r="C25" s="8" t="s">
@@ -5370,8 +5454,8 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="158"/>
-      <c r="B26" s="161"/>
+      <c r="A26" s="162"/>
+      <c r="B26" s="165"/>
       <c r="C26" s="11" t="s">
         <v>71</v>
       </c>
@@ -5383,8 +5467,8 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="158"/>
-      <c r="B27" s="161"/>
+      <c r="A27" s="162"/>
+      <c r="B27" s="165"/>
       <c r="C27" s="11" t="s">
         <v>11</v>
       </c>
@@ -5396,8 +5480,8 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="158"/>
-      <c r="B28" s="161"/>
+      <c r="A28" s="162"/>
+      <c r="B28" s="165"/>
       <c r="C28" s="21" t="s">
         <v>72</v>
       </c>
@@ -5409,8 +5493,8 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="158"/>
-      <c r="B29" s="161"/>
+      <c r="A29" s="162"/>
+      <c r="B29" s="165"/>
       <c r="C29" s="11" t="s">
         <v>9</v>
       </c>
@@ -5422,8 +5506,8 @@
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="158"/>
-      <c r="B30" s="161"/>
+      <c r="A30" s="162"/>
+      <c r="B30" s="165"/>
       <c r="C30" s="11" t="s">
         <v>13</v>
       </c>
@@ -5435,8 +5519,8 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="158"/>
-      <c r="B31" s="161"/>
+      <c r="A31" s="162"/>
+      <c r="B31" s="165"/>
       <c r="C31" s="11" t="s">
         <v>15</v>
       </c>
@@ -5448,8 +5532,8 @@
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="159"/>
-      <c r="B32" s="162"/>
+      <c r="A32" s="163"/>
+      <c r="B32" s="166"/>
       <c r="C32" s="11" t="s">
         <v>17</v>
       </c>
@@ -5573,12 +5657,12 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="154" t="s">
+      <c r="A41" s="158" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="155"/>
-      <c r="C41" s="155"/>
-      <c r="D41" s="156"/>
+      <c r="B41" s="159"/>
+      <c r="C41" s="159"/>
+      <c r="D41" s="160"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -5679,7 +5763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:XFC79"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A88" workbookViewId="0">
       <selection activeCell="A30" sqref="A30:A38"/>
     </sheetView>
   </sheetViews>
@@ -5758,10 +5842,10 @@
       <c r="D6" s="44"/>
     </row>
     <row r="7" spans="1:4" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="184" t="s">
+      <c r="A7" s="188" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="183" t="s">
+      <c r="B7" s="187" t="s">
         <v>85</v>
       </c>
       <c r="C7" s="43" t="s">
@@ -5772,8 +5856,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="184"/>
-      <c r="B8" s="183"/>
+      <c r="A8" s="188"/>
+      <c r="B8" s="187"/>
       <c r="C8" s="38" t="s">
         <v>88</v>
       </c>
@@ -5782,8 +5866,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="184"/>
-      <c r="B9" s="183"/>
+      <c r="A9" s="188"/>
+      <c r="B9" s="187"/>
       <c r="C9" s="38" t="s">
         <v>89</v>
       </c>
@@ -5792,8 +5876,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="184"/>
-      <c r="B10" s="183"/>
+      <c r="A10" s="188"/>
+      <c r="B10" s="187"/>
       <c r="C10" s="38" t="s">
         <v>6</v>
       </c>
@@ -5802,8 +5886,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="184"/>
-      <c r="B11" s="183"/>
+      <c r="A11" s="188"/>
+      <c r="B11" s="187"/>
       <c r="C11" s="38" t="s">
         <v>93</v>
       </c>
@@ -5812,8 +5896,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="184"/>
-      <c r="B12" s="183"/>
+      <c r="A12" s="188"/>
+      <c r="B12" s="187"/>
       <c r="C12" s="38" t="s">
         <v>96</v>
       </c>
@@ -5822,10 +5906,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="186" t="s">
+      <c r="A13" s="190" t="s">
         <v>146</v>
       </c>
-      <c r="B13" s="183" t="s">
+      <c r="B13" s="187" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -5836,8 +5920,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="186"/>
-      <c r="B14" s="183"/>
+      <c r="A14" s="190"/>
+      <c r="B14" s="187"/>
       <c r="C14" s="38" t="s">
         <v>180</v>
       </c>
@@ -5846,8 +5930,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="186"/>
-      <c r="B15" s="183"/>
+      <c r="A15" s="190"/>
+      <c r="B15" s="187"/>
       <c r="C15" s="43" t="s">
         <v>182</v>
       </c>
@@ -5856,10 +5940,10 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="169" t="s">
+      <c r="A16" s="173" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="178" t="s">
+      <c r="B16" s="182" t="s">
         <v>85</v>
       </c>
       <c r="C16" s="59" t="s">
@@ -5870,8 +5954,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="169"/>
-      <c r="B17" s="178"/>
+      <c r="A17" s="173"/>
+      <c r="B17" s="182"/>
       <c r="C17" s="58" t="s">
         <v>148</v>
       </c>
@@ -5880,8 +5964,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="169"/>
-      <c r="B18" s="178"/>
+      <c r="A18" s="173"/>
+      <c r="B18" s="182"/>
       <c r="C18" s="58" t="s">
         <v>93</v>
       </c>
@@ -5890,8 +5974,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="169"/>
-      <c r="B19" s="178"/>
+      <c r="A19" s="173"/>
+      <c r="B19" s="182"/>
       <c r="C19" s="58" t="s">
         <v>151</v>
       </c>
@@ -5900,8 +5984,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="169"/>
-      <c r="B20" s="178"/>
+      <c r="A20" s="173"/>
+      <c r="B20" s="182"/>
       <c r="C20" s="58" t="s">
         <v>153</v>
       </c>
@@ -5910,8 +5994,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="169"/>
-      <c r="B21" s="178"/>
+      <c r="A21" s="173"/>
+      <c r="B21" s="182"/>
       <c r="C21" s="58" t="s">
         <v>155</v>
       </c>
@@ -5920,8 +6004,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="169"/>
-      <c r="B22" s="178"/>
+      <c r="A22" s="173"/>
+      <c r="B22" s="182"/>
       <c r="C22" s="58" t="s">
         <v>157</v>
       </c>
@@ -5930,8 +6014,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="169"/>
-      <c r="B23" s="178"/>
+      <c r="A23" s="173"/>
+      <c r="B23" s="182"/>
       <c r="C23" s="66" t="s">
         <v>159</v>
       </c>
@@ -5940,26 +6024,26 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="169"/>
-      <c r="B24" s="178"/>
-      <c r="C24" s="169" t="s">
+      <c r="A24" s="173"/>
+      <c r="B24" s="182"/>
+      <c r="C24" s="173" t="s">
         <v>161</v>
       </c>
-      <c r="D24" s="170" t="s">
+      <c r="D24" s="174" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="4.1500000000000004" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="169"/>
-      <c r="B25" s="178"/>
-      <c r="C25" s="169"/>
-      <c r="D25" s="170"/>
+      <c r="A25" s="173"/>
+      <c r="B25" s="182"/>
+      <c r="C25" s="173"/>
+      <c r="D25" s="174"/>
     </row>
     <row r="26" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="184" t="s">
+      <c r="A26" s="188" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="183" t="s">
+      <c r="B26" s="187" t="s">
         <v>85</v>
       </c>
       <c r="C26" s="38" t="s">
@@ -5970,8 +6054,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="184"/>
-      <c r="B27" s="183"/>
+      <c r="A27" s="188"/>
+      <c r="B27" s="187"/>
       <c r="C27" s="38"/>
       <c r="D27" s="41" t="s">
         <v>118</v>
@@ -5998,28 +6082,28 @@
       <c r="D29" s="39"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="185" t="s">
+      <c r="A30" s="189" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="183" t="s">
+      <c r="B30" s="187" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="169" t="s">
+      <c r="C30" s="173" t="s">
         <v>169</v>
       </c>
-      <c r="D30" s="173" t="s">
+      <c r="D30" s="177" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="185"/>
-      <c r="B31" s="183"/>
-      <c r="C31" s="169"/>
-      <c r="D31" s="173"/>
+      <c r="A31" s="189"/>
+      <c r="B31" s="187"/>
+      <c r="C31" s="173"/>
+      <c r="D31" s="177"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="185"/>
-      <c r="B32" s="183"/>
+      <c r="A32" s="189"/>
+      <c r="B32" s="187"/>
       <c r="C32" s="58" t="s">
         <v>167</v>
       </c>
@@ -6028,8 +6112,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="185"/>
-      <c r="B33" s="183"/>
+      <c r="A33" s="189"/>
+      <c r="B33" s="187"/>
       <c r="C33" s="58" t="s">
         <v>168</v>
       </c>
@@ -6038,8 +6122,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="185"/>
-      <c r="B34" s="183"/>
+      <c r="A34" s="189"/>
+      <c r="B34" s="187"/>
       <c r="C34" s="67" t="s">
         <v>170</v>
       </c>
@@ -6048,8 +6132,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="185"/>
-      <c r="B35" s="183"/>
+      <c r="A35" s="189"/>
+      <c r="B35" s="187"/>
       <c r="C35" s="58" t="s">
         <v>157</v>
       </c>
@@ -6058,8 +6142,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="185"/>
-      <c r="B36" s="183"/>
+      <c r="A36" s="189"/>
+      <c r="B36" s="187"/>
       <c r="C36" s="67" t="s">
         <v>159</v>
       </c>
@@ -6068,26 +6152,26 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="185"/>
-      <c r="B37" s="183"/>
-      <c r="C37" s="174" t="s">
+      <c r="A37" s="189"/>
+      <c r="B37" s="187"/>
+      <c r="C37" s="178" t="s">
         <v>161</v>
       </c>
-      <c r="D37" s="176" t="s">
+      <c r="D37" s="180" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="6.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="185"/>
-      <c r="B38" s="183"/>
-      <c r="C38" s="175"/>
-      <c r="D38" s="176"/>
+      <c r="A38" s="189"/>
+      <c r="B38" s="187"/>
+      <c r="C38" s="179"/>
+      <c r="D38" s="180"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="184" t="s">
+      <c r="A39" s="188" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="183" t="s">
+      <c r="B39" s="187" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="38" t="s">
@@ -6098,8 +6182,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="184"/>
-      <c r="B40" s="183"/>
+      <c r="A40" s="188"/>
+      <c r="B40" s="187"/>
       <c r="C40" s="38"/>
       <c r="D40" s="49" t="s">
         <v>98</v>
@@ -6126,10 +6210,10 @@
       <c r="D42" s="44"/>
     </row>
     <row r="43" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="185" t="s">
+      <c r="A43" s="189" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="183" t="s">
+      <c r="B43" s="187" t="s">
         <v>85</v>
       </c>
       <c r="C43" s="38"/>
@@ -6138,8 +6222,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="185"/>
-      <c r="B44" s="183"/>
+      <c r="A44" s="189"/>
+      <c r="B44" s="187"/>
       <c r="C44" s="38" t="s">
         <v>145</v>
       </c>
@@ -6148,10 +6232,10 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="180" t="s">
+      <c r="A45" s="184" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="183" t="s">
+      <c r="B45" s="187" t="s">
         <v>85</v>
       </c>
       <c r="C45" s="38"/>
@@ -6160,8 +6244,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="181"/>
-      <c r="B46" s="183"/>
+      <c r="A46" s="185"/>
+      <c r="B46" s="187"/>
       <c r="C46" s="38" t="s">
         <v>101</v>
       </c>
@@ -6170,8 +6254,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="181"/>
-      <c r="B47" s="183"/>
+      <c r="A47" s="185"/>
+      <c r="B47" s="187"/>
       <c r="C47" s="38" t="s">
         <v>99</v>
       </c>
@@ -6180,8 +6264,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="182"/>
-      <c r="B48" s="183"/>
+      <c r="A48" s="186"/>
+      <c r="B48" s="187"/>
       <c r="C48" s="38" t="s">
         <v>145</v>
       </c>
@@ -6190,10 +6274,10 @@
       </c>
     </row>
     <row r="49" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A49" s="178" t="s">
+      <c r="A49" s="182" t="s">
         <v>32</v>
       </c>
-      <c r="B49" s="178" t="s">
+      <c r="B49" s="182" t="s">
         <v>85</v>
       </c>
       <c r="C49" s="58"/>
@@ -10297,8 +10381,8 @@
       <c r="XFC49" s="42"/>
     </row>
     <row r="50" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="178"/>
-      <c r="B50" s="178"/>
+      <c r="A50" s="182"/>
+      <c r="B50" s="182"/>
       <c r="C50" s="59" t="s">
         <v>105</v>
       </c>
@@ -14402,8 +14486,8 @@
       <c r="XFC50" s="42"/>
     </row>
     <row r="51" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A51" s="178"/>
-      <c r="B51" s="178"/>
+      <c r="A51" s="182"/>
+      <c r="B51" s="182"/>
       <c r="C51" s="38" t="s">
         <v>107</v>
       </c>
@@ -18507,8 +18591,8 @@
       <c r="XFC51" s="42"/>
     </row>
     <row r="52" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A52" s="178"/>
-      <c r="B52" s="178"/>
+      <c r="A52" s="182"/>
+      <c r="B52" s="182"/>
       <c r="C52" s="58" t="s">
         <v>108</v>
       </c>
@@ -22612,12 +22696,12 @@
       <c r="XFC52" s="42"/>
     </row>
     <row r="53" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A53" s="178"/>
-      <c r="B53" s="178"/>
-      <c r="C53" s="172" t="s">
+      <c r="A53" s="182"/>
+      <c r="B53" s="182"/>
+      <c r="C53" s="176" t="s">
         <v>109</v>
       </c>
-      <c r="D53" s="173" t="s">
+      <c r="D53" s="177" t="s">
         <v>144</v>
       </c>
       <c r="G53" s="42"/>
@@ -26717,10 +26801,10 @@
       <c r="XFC53" s="42"/>
     </row>
     <row r="54" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="178"/>
-      <c r="B54" s="178"/>
-      <c r="C54" s="172"/>
-      <c r="D54" s="173"/>
+      <c r="A54" s="182"/>
+      <c r="B54" s="182"/>
+      <c r="C54" s="176"/>
+      <c r="D54" s="177"/>
       <c r="G54" s="42"/>
       <c r="K54" s="42"/>
       <c r="O54" s="42"/>
@@ -30838,10 +30922,10 @@
       </c>
     </row>
     <row r="57" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A57" s="177" t="s">
+      <c r="A57" s="181" t="s">
         <v>84</v>
       </c>
-      <c r="B57" s="178" t="s">
+      <c r="B57" s="182" t="s">
         <v>85</v>
       </c>
       <c r="C57" s="58" t="s">
@@ -30852,8 +30936,8 @@
       </c>
     </row>
     <row r="58" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="177"/>
-      <c r="B58" s="178"/>
+      <c r="A58" s="181"/>
+      <c r="B58" s="182"/>
       <c r="C58" s="61" t="s">
         <v>113</v>
       </c>
@@ -30862,8 +30946,8 @@
       </c>
     </row>
     <row r="59" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A59" s="177"/>
-      <c r="B59" s="178"/>
+      <c r="A59" s="181"/>
+      <c r="B59" s="182"/>
       <c r="C59" s="58" t="s">
         <v>114</v>
       </c>
@@ -30872,8 +30956,8 @@
       </c>
     </row>
     <row r="60" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="177"/>
-      <c r="B60" s="178"/>
+      <c r="A60" s="181"/>
+      <c r="B60" s="182"/>
       <c r="C60" s="58" t="s">
         <v>115</v>
       </c>
@@ -30882,8 +30966,8 @@
       </c>
     </row>
     <row r="61" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A61" s="177"/>
-      <c r="B61" s="178"/>
+      <c r="A61" s="181"/>
+      <c r="B61" s="182"/>
       <c r="C61" s="38" t="s">
         <v>145</v>
       </c>
@@ -30892,8 +30976,8 @@
       </c>
     </row>
     <row r="62" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A62" s="177"/>
-      <c r="B62" s="178"/>
+      <c r="A62" s="181"/>
+      <c r="B62" s="182"/>
       <c r="C62" s="58" t="s">
         <v>117</v>
       </c>
@@ -30902,8 +30986,8 @@
       </c>
     </row>
     <row r="63" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A63" s="177"/>
-      <c r="B63" s="178"/>
+      <c r="A63" s="181"/>
+      <c r="B63" s="182"/>
       <c r="C63" s="58" t="s">
         <v>117</v>
       </c>
@@ -30912,16 +30996,16 @@
       </c>
     </row>
     <row r="64" spans="1:1023 1027:2047 2051:3071 3075:4095 4099:5119 5123:6143 6147:7167 7171:8191 8195:9215 9219:10239 10243:11263 11267:12287 12291:13311 13315:14335 14339:15359 15363:16383" x14ac:dyDescent="0.25">
-      <c r="A64" s="177"/>
-      <c r="B64" s="178"/>
+      <c r="A64" s="181"/>
+      <c r="B64" s="182"/>
       <c r="C64" s="58"/>
       <c r="D64" s="47" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="177"/>
-      <c r="B65" s="178"/>
+      <c r="A65" s="181"/>
+      <c r="B65" s="182"/>
       <c r="C65" s="58" t="s">
         <v>120</v>
       </c>
@@ -30930,16 +31014,16 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="177"/>
-      <c r="B66" s="178"/>
+      <c r="A66" s="181"/>
+      <c r="B66" s="182"/>
       <c r="C66" s="58"/>
       <c r="D66" s="46" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="177"/>
-      <c r="B67" s="178"/>
+      <c r="A67" s="181"/>
+      <c r="B67" s="182"/>
       <c r="C67" s="58" t="s">
         <v>122</v>
       </c>
@@ -30948,8 +31032,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="177"/>
-      <c r="B68" s="178"/>
+      <c r="A68" s="181"/>
+      <c r="B68" s="182"/>
       <c r="C68" s="58" t="s">
         <v>123</v>
       </c>
@@ -30958,8 +31042,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="177"/>
-      <c r="B69" s="178"/>
+      <c r="A69" s="181"/>
+      <c r="B69" s="182"/>
       <c r="C69" s="61" t="s">
         <v>125</v>
       </c>
@@ -30968,8 +31052,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="177"/>
-      <c r="B70" s="178"/>
+      <c r="A70" s="181"/>
+      <c r="B70" s="182"/>
       <c r="C70" s="61" t="s">
         <v>126</v>
       </c>
@@ -30978,8 +31062,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="177"/>
-      <c r="B71" s="178"/>
+      <c r="A71" s="181"/>
+      <c r="B71" s="182"/>
       <c r="C71" s="58" t="s">
         <v>127</v>
       </c>
@@ -30988,8 +31072,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="177"/>
-      <c r="B72" s="178"/>
+      <c r="A72" s="181"/>
+      <c r="B72" s="182"/>
       <c r="C72" s="58" t="s">
         <v>128</v>
       </c>
@@ -30998,16 +31082,16 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="177"/>
-      <c r="B73" s="178"/>
+      <c r="A73" s="181"/>
+      <c r="B73" s="182"/>
       <c r="C73" s="58"/>
       <c r="D73" s="49" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="177"/>
-      <c r="B74" s="178"/>
+      <c r="A74" s="181"/>
+      <c r="B74" s="182"/>
       <c r="C74" s="58" t="s">
         <v>129</v>
       </c>
@@ -31016,18 +31100,18 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="177"/>
-      <c r="B75" s="178"/>
-      <c r="C75" s="171"/>
-      <c r="D75" s="179" t="s">
+      <c r="A75" s="181"/>
+      <c r="B75" s="182"/>
+      <c r="C75" s="175"/>
+      <c r="D75" s="183" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="177"/>
-      <c r="B76" s="178"/>
-      <c r="C76" s="171"/>
-      <c r="D76" s="179"/>
+      <c r="A76" s="181"/>
+      <c r="B76" s="182"/>
+      <c r="C76" s="175"/>
+      <c r="D76" s="183"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="39" t="s">
@@ -31108,7 +31192,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A32" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -31151,10 +31235,10 @@
       <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="184" t="s">
+      <c r="A4" s="188" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="183" t="s">
+      <c r="B4" s="187" t="s">
         <v>185</v>
       </c>
       <c r="C4" s="72" t="s">
@@ -31165,133 +31249,133 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="184"/>
-      <c r="B5" s="183"/>
-      <c r="C5" s="194" t="s">
+      <c r="A5" s="188"/>
+      <c r="B5" s="187"/>
+      <c r="C5" s="198" t="s">
         <v>190</v>
       </c>
-      <c r="D5" s="193" t="s">
+      <c r="D5" s="197" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="7.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="184"/>
-      <c r="B6" s="183"/>
-      <c r="C6" s="194"/>
-      <c r="D6" s="193"/>
+      <c r="A6" s="188"/>
+      <c r="B6" s="187"/>
+      <c r="C6" s="198"/>
+      <c r="D6" s="197"/>
     </row>
     <row r="7" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="184"/>
-      <c r="B7" s="183"/>
+      <c r="A7" s="188"/>
+      <c r="B7" s="187"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="184"/>
-      <c r="B8" s="183"/>
+      <c r="A8" s="188"/>
+      <c r="B8" s="187"/>
       <c r="C8" s="58"/>
       <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="184"/>
-      <c r="B9" s="183"/>
+      <c r="A9" s="188"/>
+      <c r="B9" s="187"/>
       <c r="C9" s="71"/>
       <c r="D9" s="49"/>
     </row>
     <row r="10" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="186" t="s">
+      <c r="A10" s="190" t="s">
         <v>146</v>
       </c>
-      <c r="B10" s="183" t="s">
+      <c r="B10" s="187" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="196"/>
-      <c r="D10" s="193" t="s">
+      <c r="C10" s="200"/>
+      <c r="D10" s="197" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="186"/>
-      <c r="B11" s="183"/>
-      <c r="C11" s="196"/>
-      <c r="D11" s="193"/>
+      <c r="A11" s="190"/>
+      <c r="B11" s="187"/>
+      <c r="C11" s="200"/>
+      <c r="D11" s="197"/>
     </row>
     <row r="12" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="186"/>
-      <c r="B12" s="183"/>
-      <c r="C12" s="196"/>
-      <c r="D12" s="193"/>
+      <c r="A12" s="190"/>
+      <c r="B12" s="187"/>
+      <c r="C12" s="200"/>
+      <c r="D12" s="197"/>
     </row>
     <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="169" t="s">
+      <c r="A13" s="173" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="178" t="s">
+      <c r="B13" s="182" t="s">
         <v>185</v>
       </c>
-      <c r="C13" s="195"/>
-      <c r="D13" s="193" t="s">
+      <c r="C13" s="199"/>
+      <c r="D13" s="197" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="169"/>
-      <c r="B14" s="178"/>
-      <c r="C14" s="195"/>
-      <c r="D14" s="193"/>
+      <c r="A14" s="173"/>
+      <c r="B14" s="182"/>
+      <c r="C14" s="199"/>
+      <c r="D14" s="197"/>
     </row>
     <row r="15" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="169"/>
-      <c r="B15" s="178"/>
-      <c r="C15" s="195"/>
+      <c r="A15" s="173"/>
+      <c r="B15" s="182"/>
+      <c r="C15" s="199"/>
       <c r="D15" s="49"/>
     </row>
     <row r="16" spans="1:4" ht="27.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="169"/>
-      <c r="B16" s="178"/>
-      <c r="C16" s="195"/>
+      <c r="A16" s="173"/>
+      <c r="B16" s="182"/>
+      <c r="C16" s="199"/>
       <c r="D16" s="49"/>
     </row>
     <row r="17" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="169"/>
-      <c r="B17" s="178"/>
-      <c r="C17" s="195"/>
+      <c r="A17" s="173"/>
+      <c r="B17" s="182"/>
+      <c r="C17" s="199"/>
       <c r="D17" s="49"/>
     </row>
     <row r="18" spans="1:4" ht="41.65" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="169"/>
-      <c r="B18" s="178"/>
-      <c r="C18" s="195"/>
+      <c r="A18" s="173"/>
+      <c r="B18" s="182"/>
+      <c r="C18" s="199"/>
       <c r="D18" s="49"/>
     </row>
     <row r="19" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="169"/>
-      <c r="B19" s="178"/>
-      <c r="C19" s="195"/>
+      <c r="A19" s="173"/>
+      <c r="B19" s="182"/>
+      <c r="C19" s="199"/>
       <c r="D19" s="49"/>
     </row>
     <row r="20" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="169"/>
-      <c r="B20" s="178"/>
-      <c r="C20" s="195"/>
+      <c r="A20" s="173"/>
+      <c r="B20" s="182"/>
+      <c r="C20" s="199"/>
       <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="169"/>
-      <c r="B21" s="178"/>
-      <c r="C21" s="195"/>
+      <c r="A21" s="173"/>
+      <c r="B21" s="182"/>
+      <c r="C21" s="199"/>
       <c r="D21" s="49"/>
     </row>
     <row r="22" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="169"/>
-      <c r="B22" s="178"/>
-      <c r="C22" s="195"/>
+      <c r="A22" s="173"/>
+      <c r="B22" s="182"/>
+      <c r="C22" s="199"/>
       <c r="D22" s="49"/>
     </row>
     <row r="23" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="169"/>
-      <c r="B23" s="178"/>
-      <c r="C23" s="195"/>
+      <c r="A23" s="173"/>
+      <c r="B23" s="182"/>
+      <c r="C23" s="199"/>
       <c r="D23" s="58" t="s">
         <v>221</v>
       </c>
@@ -31389,10 +31473,10 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="187" t="s">
+      <c r="A32" s="191" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="190" t="s">
+      <c r="B32" s="194" t="s">
         <v>185</v>
       </c>
       <c r="C32" s="91" t="s">
@@ -31403,26 +31487,26 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="188"/>
-      <c r="B33" s="191"/>
+      <c r="A33" s="192"/>
+      <c r="B33" s="195"/>
       <c r="C33" s="78"/>
       <c r="D33" s="75"/>
     </row>
     <row r="34" spans="1:4" ht="9.6" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="188"/>
-      <c r="B34" s="191"/>
+      <c r="A34" s="192"/>
+      <c r="B34" s="195"/>
       <c r="C34" s="78"/>
       <c r="D34" s="75"/>
     </row>
     <row r="35" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="188"/>
-      <c r="B35" s="191"/>
+      <c r="A35" s="192"/>
+      <c r="B35" s="195"/>
       <c r="C35" s="78"/>
       <c r="D35" s="75"/>
     </row>
     <row r="36" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="189"/>
-      <c r="B36" s="192"/>
+      <c r="A36" s="193"/>
+      <c r="B36" s="196"/>
       <c r="C36" s="78" t="s">
         <v>223</v>
       </c>
@@ -31451,10 +31535,10 @@
       <c r="D38" s="44"/>
     </row>
     <row r="39" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="185" t="s">
+      <c r="A39" s="189" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="183" t="s">
+      <c r="B39" s="187" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="76" t="s">
@@ -31465,8 +31549,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="185"/>
-      <c r="B40" s="183"/>
+      <c r="A40" s="189"/>
+      <c r="B40" s="187"/>
       <c r="C40" s="69" t="s">
         <v>190</v>
       </c>
@@ -31475,84 +31559,84 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="184" t="s">
+      <c r="A41" s="188" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="183" t="s">
+      <c r="B41" s="187" t="s">
         <v>185</v>
       </c>
-      <c r="C41" s="196" t="s">
+      <c r="C41" s="200" t="s">
         <v>194</v>
       </c>
-      <c r="D41" s="169" t="s">
+      <c r="D41" s="173" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="184"/>
-      <c r="B42" s="183"/>
-      <c r="C42" s="196"/>
-      <c r="D42" s="169"/>
+      <c r="A42" s="188"/>
+      <c r="B42" s="187"/>
+      <c r="C42" s="200"/>
+      <c r="D42" s="173"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="184"/>
-      <c r="B43" s="183"/>
-      <c r="C43" s="196" t="s">
+      <c r="A43" s="188"/>
+      <c r="B43" s="187"/>
+      <c r="C43" s="200" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="179" t="s">
+      <c r="D43" s="183" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="184"/>
-      <c r="B44" s="183"/>
-      <c r="C44" s="196"/>
-      <c r="D44" s="179"/>
+      <c r="A44" s="188"/>
+      <c r="B44" s="187"/>
+      <c r="C44" s="200"/>
+      <c r="D44" s="183"/>
     </row>
     <row r="45" spans="1:4" ht="24.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="177" t="s">
+      <c r="A45" s="181" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="178" t="s">
+      <c r="B45" s="182" t="s">
         <v>185</v>
       </c>
-      <c r="C45" s="200"/>
+      <c r="C45" s="204"/>
       <c r="D45" s="90" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="177"/>
-      <c r="B46" s="178"/>
-      <c r="C46" s="201"/>
-      <c r="D46" s="197" t="s">
+      <c r="A46" s="181"/>
+      <c r="B46" s="182"/>
+      <c r="C46" s="205"/>
+      <c r="D46" s="201" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="177"/>
-      <c r="B47" s="178"/>
-      <c r="C47" s="201"/>
-      <c r="D47" s="198"/>
+      <c r="A47" s="181"/>
+      <c r="B47" s="182"/>
+      <c r="C47" s="205"/>
+      <c r="D47" s="202"/>
     </row>
     <row r="48" spans="1:4" ht="13.9" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="177"/>
-      <c r="B48" s="178"/>
-      <c r="C48" s="202"/>
-      <c r="D48" s="198"/>
+      <c r="A48" s="181"/>
+      <c r="B48" s="182"/>
+      <c r="C48" s="206"/>
+      <c r="D48" s="202"/>
     </row>
     <row r="49" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="177"/>
-      <c r="B49" s="178"/>
-      <c r="C49" s="172"/>
-      <c r="D49" s="198"/>
+      <c r="A49" s="181"/>
+      <c r="B49" s="182"/>
+      <c r="C49" s="176"/>
+      <c r="D49" s="202"/>
     </row>
     <row r="50" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="177"/>
-      <c r="B50" s="178"/>
-      <c r="C50" s="172"/>
-      <c r="D50" s="199"/>
+      <c r="A50" s="181"/>
+      <c r="B50" s="182"/>
+      <c r="C50" s="176"/>
+      <c r="D50" s="203"/>
     </row>
     <row r="51" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="39" t="s">
@@ -31575,10 +31659,10 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="178" t="s">
+      <c r="A53" s="182" t="s">
         <v>84</v>
       </c>
-      <c r="B53" s="178" t="s">
+      <c r="B53" s="182" t="s">
         <v>185</v>
       </c>
       <c r="C53" s="78" t="s">
@@ -31589,8 +31673,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="178"/>
-      <c r="B54" s="178"/>
+      <c r="A54" s="182"/>
+      <c r="B54" s="182"/>
       <c r="C54" s="78" t="s">
         <v>190</v>
       </c>
@@ -31599,8 +31683,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="178"/>
-      <c r="B55" s="178"/>
+      <c r="A55" s="182"/>
+      <c r="B55" s="182"/>
       <c r="C55" s="78" t="s">
         <v>205</v>
       </c>
@@ -31609,9 +31693,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="34.35" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="178"/>
-      <c r="B56" s="178"/>
-      <c r="C56" s="203" t="s">
+      <c r="A56" s="182"/>
+      <c r="B56" s="182"/>
+      <c r="C56" s="207" t="s">
         <v>208</v>
       </c>
       <c r="D56" s="79" t="s">
@@ -31619,16 +31703,16 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="178"/>
-      <c r="B57" s="178"/>
-      <c r="C57" s="203"/>
+      <c r="A57" s="182"/>
+      <c r="B57" s="182"/>
+      <c r="C57" s="207"/>
       <c r="D57" s="47" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="178"/>
-      <c r="B58" s="178"/>
+      <c r="A58" s="182"/>
+      <c r="B58" s="182"/>
       <c r="C58" s="78" t="s">
         <v>209</v>
       </c>
@@ -31637,8 +31721,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="178"/>
-      <c r="B59" s="178"/>
+      <c r="A59" s="182"/>
+      <c r="B59" s="182"/>
       <c r="C59" s="78" t="s">
         <v>210</v>
       </c>
@@ -31647,9 +31731,9 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="178"/>
-      <c r="B60" s="178"/>
-      <c r="C60" s="203" t="s">
+      <c r="A60" s="182"/>
+      <c r="B60" s="182"/>
+      <c r="C60" s="207" t="s">
         <v>207</v>
       </c>
       <c r="D60" s="46" t="s">
@@ -31657,25 +31741,25 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="178"/>
-      <c r="B61" s="178"/>
-      <c r="C61" s="203"/>
+      <c r="A61" s="182"/>
+      <c r="B61" s="182"/>
+      <c r="C61" s="207"/>
       <c r="D61" s="46" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="178"/>
-      <c r="B62" s="178"/>
-      <c r="C62" s="203"/>
+      <c r="A62" s="182"/>
+      <c r="B62" s="182"/>
+      <c r="C62" s="207"/>
       <c r="D62" s="79" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="178"/>
-      <c r="B63" s="178"/>
-      <c r="C63" s="196" t="s">
+      <c r="A63" s="182"/>
+      <c r="B63" s="182"/>
+      <c r="C63" s="200" t="s">
         <v>206</v>
       </c>
       <c r="D63" s="45" t="s">
@@ -31683,30 +31767,30 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="14.45" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="178"/>
-      <c r="B64" s="178"/>
-      <c r="C64" s="196"/>
-      <c r="D64" s="179" t="s">
+      <c r="A64" s="182"/>
+      <c r="B64" s="182"/>
+      <c r="C64" s="200"/>
+      <c r="D64" s="183" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="12.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="178"/>
-      <c r="B65" s="178"/>
-      <c r="C65" s="196"/>
-      <c r="D65" s="179"/>
+      <c r="A65" s="182"/>
+      <c r="B65" s="182"/>
+      <c r="C65" s="200"/>
+      <c r="D65" s="183"/>
     </row>
     <row r="66" spans="1:4" ht="13.15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="178"/>
-      <c r="B66" s="178"/>
-      <c r="C66" s="196"/>
-      <c r="D66" s="179"/>
+      <c r="A66" s="182"/>
+      <c r="B66" s="182"/>
+      <c r="C66" s="200"/>
+      <c r="D66" s="183"/>
     </row>
     <row r="67" spans="1:4" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="178"/>
-      <c r="B67" s="178"/>
-      <c r="C67" s="196"/>
-      <c r="D67" s="179"/>
+      <c r="A67" s="182"/>
+      <c r="B67" s="182"/>
+      <c r="C67" s="200"/>
+      <c r="D67" s="183"/>
     </row>
     <row r="68" spans="1:4" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="39"/>
@@ -31803,18 +31887,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D220"/>
+  <dimension ref="A1:D247"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A214" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B249" sqref="B249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" customWidth="1"/>
+    <col min="1" max="1" width="62.42578125" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" style="157" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="65" customWidth="1"/>
+    <col min="4" max="4" width="107.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -31831,19 +31915,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="103" t="s">
         <v>433</v>
       </c>
-      <c r="B2" s="103"/>
+      <c r="B2" s="155"/>
       <c r="C2" s="103"/>
       <c r="D2" s="104"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="226" t="s">
+      <c r="A3" s="230" t="s">
         <v>434</v>
       </c>
-      <c r="B3" s="226" t="s">
+      <c r="B3" s="230" t="s">
         <v>435</v>
       </c>
       <c r="C3" s="101" t="s">
@@ -31854,8 +31938,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="227"/>
-      <c r="B4" s="227"/>
+      <c r="A4" s="231"/>
+      <c r="B4" s="231"/>
       <c r="C4" s="100" t="s">
         <v>438</v>
       </c>
@@ -31864,76 +31948,76 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="228"/>
-      <c r="B5" s="228"/>
+      <c r="A5" s="232"/>
+      <c r="B5" s="232"/>
       <c r="C5" s="100" t="s">
         <v>438</v>
       </c>
-      <c r="D5" s="147" t="s">
+      <c r="D5" s="144" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="144" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="143" t="s">
         <v>482</v>
       </c>
-      <c r="B6" s="145" t="s">
+      <c r="B6" s="153" t="s">
         <v>432</v>
       </c>
-      <c r="C6" s="142" t="s">
+      <c r="C6" s="141" t="s">
         <v>480</v>
       </c>
-      <c r="D6" s="143" t="s">
+      <c r="D6" s="142" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="226" t="s">
+      <c r="A7" s="230" t="s">
         <v>485</v>
       </c>
-      <c r="B7" s="226" t="s">
+      <c r="B7" s="230" t="s">
         <v>435</v>
       </c>
-      <c r="C7" s="142" t="s">
+      <c r="C7" s="141" t="s">
         <v>486</v>
       </c>
-      <c r="D7" s="143" t="s">
+      <c r="D7" s="142" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="227"/>
-      <c r="B8" s="227"/>
-      <c r="C8" s="142" t="s">
+      <c r="A8" s="231"/>
+      <c r="B8" s="231"/>
+      <c r="C8" s="141" t="s">
         <v>486</v>
       </c>
-      <c r="D8" s="143" t="s">
+      <c r="D8" s="142" t="s">
         <v>487</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="228"/>
-      <c r="B9" s="228"/>
-      <c r="C9" s="142" t="s">
+      <c r="A9" s="232"/>
+      <c r="B9" s="232"/>
+      <c r="C9" s="141" t="s">
         <v>489</v>
       </c>
-      <c r="D9" s="143" t="s">
+      <c r="D9" s="142" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="126" t="s">
         <v>247</v>
       </c>
-      <c r="B10" s="103"/>
+      <c r="B10" s="155"/>
       <c r="C10" s="127"/>
       <c r="D10" s="127"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="208" t="s">
+      <c r="A11" s="212" t="s">
         <v>248</v>
       </c>
-      <c r="B11" s="206" t="s">
+      <c r="B11" s="210" t="s">
         <v>432</v>
       </c>
       <c r="C11" s="128" t="s">
@@ -31944,8 +32028,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="211"/>
-      <c r="B12" s="207"/>
+      <c r="A12" s="215"/>
+      <c r="B12" s="211"/>
       <c r="C12" s="128" t="s">
         <v>451</v>
       </c>
@@ -31954,10 +32038,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="206" t="s">
+      <c r="A13" s="210" t="s">
         <v>280</v>
       </c>
-      <c r="B13" s="148" t="s">
+      <c r="B13" s="149" t="s">
         <v>432</v>
       </c>
       <c r="C13" s="95" t="s">
@@ -31968,8 +32052,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="210"/>
-      <c r="B14" s="149"/>
+      <c r="A14" s="214"/>
+      <c r="B14" s="151"/>
       <c r="C14" s="106" t="s">
         <v>300</v>
       </c>
@@ -31978,8 +32062,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="210"/>
-      <c r="B15" s="149"/>
+      <c r="A15" s="214"/>
+      <c r="B15" s="151"/>
       <c r="C15" s="128" t="s">
         <v>281</v>
       </c>
@@ -31988,8 +32072,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="210"/>
-      <c r="B16" s="149"/>
+      <c r="A16" s="214"/>
+      <c r="B16" s="151"/>
       <c r="C16" s="128" t="s">
         <v>21</v>
       </c>
@@ -31998,7 +32082,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="210"/>
+      <c r="A17" s="214"/>
       <c r="B17" s="150"/>
       <c r="C17" s="128" t="s">
         <v>449</v>
@@ -32008,8 +32092,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="207"/>
-      <c r="B18" s="146"/>
+      <c r="A18" s="211"/>
+      <c r="B18" s="151"/>
       <c r="C18" s="128" t="s">
         <v>436</v>
       </c>
@@ -32018,10 +32102,10 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="133" t="s">
+      <c r="A19" s="132" t="s">
         <v>453</v>
       </c>
-      <c r="B19" s="132" t="s">
+      <c r="B19" s="149" t="s">
         <v>432</v>
       </c>
       <c r="C19" s="128" t="s">
@@ -32032,10 +32116,10 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="208" t="s">
+      <c r="A20" s="212" t="s">
         <v>454</v>
       </c>
-      <c r="B20" s="206" t="s">
+      <c r="B20" s="210" t="s">
         <v>432</v>
       </c>
       <c r="C20" s="128" t="s">
@@ -32046,8 +32130,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="211"/>
-      <c r="B21" s="207"/>
+      <c r="A21" s="215"/>
+      <c r="B21" s="211"/>
       <c r="C21" s="128"/>
       <c r="D21" s="106" t="s">
         <v>479</v>
@@ -32057,15 +32141,15 @@
       <c r="A22" s="103" t="s">
         <v>336</v>
       </c>
-      <c r="B22" s="103"/>
+      <c r="B22" s="155"/>
       <c r="C22" s="103"/>
       <c r="D22" s="104"/>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="231" t="s">
+      <c r="A23" s="235" t="s">
         <v>337</v>
       </c>
-      <c r="B23" s="232" t="s">
+      <c r="B23" s="236" t="s">
         <v>432</v>
       </c>
       <c r="C23" s="100" t="s">
@@ -32076,8 +32160,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="231"/>
-      <c r="B24" s="232"/>
+      <c r="A24" s="235"/>
+      <c r="B24" s="236"/>
       <c r="C24" s="100" t="s">
         <v>342</v>
       </c>
@@ -32086,8 +32170,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="231"/>
-      <c r="B25" s="232"/>
+      <c r="A25" s="235"/>
+      <c r="B25" s="236"/>
       <c r="C25" s="100" t="s">
         <v>338</v>
       </c>
@@ -32099,15 +32183,15 @@
       <c r="A26" s="103" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="103"/>
+      <c r="B26" s="155"/>
       <c r="C26" s="103"/>
       <c r="D26" s="104"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="208" t="s">
+      <c r="A27" s="212" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="206" t="s">
+      <c r="B27" s="210" t="s">
         <v>432</v>
       </c>
       <c r="C27" s="106"/>
@@ -32116,8 +32200,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="209"/>
-      <c r="B28" s="210"/>
+      <c r="A28" s="213"/>
+      <c r="B28" s="214"/>
       <c r="C28" s="70" t="s">
         <v>234</v>
       </c>
@@ -32126,9 +32210,9 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="209"/>
-      <c r="B29" s="210"/>
-      <c r="C29" s="141" t="s">
+      <c r="A29" s="213"/>
+      <c r="B29" s="214"/>
+      <c r="C29" s="140" t="s">
         <v>445</v>
       </c>
       <c r="D29" s="107" t="s">
@@ -32136,19 +32220,19 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="209"/>
-      <c r="B30" s="210"/>
-      <c r="C30" s="140" t="s">
+      <c r="A30" s="213"/>
+      <c r="B30" s="214"/>
+      <c r="C30" s="139" t="s">
         <v>480</v>
       </c>
-      <c r="D30" s="136" t="s">
+      <c r="D30" s="135" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="209"/>
-      <c r="B31" s="210"/>
-      <c r="C31" s="153" t="s">
+      <c r="A31" s="213"/>
+      <c r="B31" s="214"/>
+      <c r="C31" s="147" t="s">
         <v>491</v>
       </c>
       <c r="D31" s="58" t="s">
@@ -32156,9 +32240,9 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="209"/>
-      <c r="B32" s="210"/>
-      <c r="C32" s="153" t="s">
+      <c r="A32" s="213"/>
+      <c r="B32" s="214"/>
+      <c r="C32" s="147" t="s">
         <v>480</v>
       </c>
       <c r="D32" s="58" t="s">
@@ -32166,10 +32250,10 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="208" t="s">
+      <c r="A33" s="212" t="s">
         <v>74</v>
       </c>
-      <c r="B33" s="206" t="s">
+      <c r="B33" s="210" t="s">
         <v>432</v>
       </c>
       <c r="C33" s="70" t="s">
@@ -32180,8 +32264,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="209"/>
-      <c r="B34" s="210"/>
+      <c r="A34" s="213"/>
+      <c r="B34" s="214"/>
       <c r="C34" s="131" t="s">
         <v>467</v>
       </c>
@@ -32190,9 +32274,9 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="211"/>
-      <c r="B35" s="207"/>
-      <c r="C35" s="137" t="s">
+      <c r="A35" s="215"/>
+      <c r="B35" s="211"/>
+      <c r="C35" s="136" t="s">
         <v>457</v>
       </c>
       <c r="D35" s="129" t="s">
@@ -32203,7 +32287,7 @@
       <c r="A36" s="108" t="s">
         <v>253</v>
       </c>
-      <c r="B36" s="70" t="s">
+      <c r="B36" s="152" t="s">
         <v>432</v>
       </c>
       <c r="C36" s="70" t="s">
@@ -32217,7 +32301,7 @@
       <c r="A37" s="108" t="s">
         <v>372</v>
       </c>
-      <c r="B37" s="70" t="s">
+      <c r="B37" s="152" t="s">
         <v>432</v>
       </c>
       <c r="C37" s="70" t="s">
@@ -32231,7 +32315,7 @@
       <c r="A38" s="108" t="s">
         <v>402</v>
       </c>
-      <c r="B38" s="70" t="s">
+      <c r="B38" s="152" t="s">
         <v>432</v>
       </c>
       <c r="C38" s="70"/>
@@ -32240,10 +32324,10 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="222" t="s">
+      <c r="A39" s="226" t="s">
         <v>270</v>
       </c>
-      <c r="B39" s="223" t="s">
+      <c r="B39" s="227" t="s">
         <v>432</v>
       </c>
       <c r="C39" s="106"/>
@@ -32252,8 +32336,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="222"/>
-      <c r="B40" s="223"/>
+      <c r="A40" s="226"/>
+      <c r="B40" s="227"/>
       <c r="C40" s="106" t="s">
         <v>494</v>
       </c>
@@ -32262,16 +32346,16 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="222"/>
-      <c r="B41" s="223"/>
+      <c r="A41" s="226"/>
+      <c r="B41" s="227"/>
       <c r="C41" s="106"/>
       <c r="D41" s="106" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="222"/>
-      <c r="B42" s="223"/>
+      <c r="A42" s="226"/>
+      <c r="B42" s="227"/>
       <c r="C42" s="110" t="s">
         <v>320</v>
       </c>
@@ -32280,8 +32364,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="222"/>
-      <c r="B43" s="223"/>
+      <c r="A43" s="226"/>
+      <c r="B43" s="227"/>
       <c r="C43" s="111" t="s">
         <v>399</v>
       </c>
@@ -32293,7 +32377,7 @@
       <c r="A44" s="108" t="s">
         <v>285</v>
       </c>
-      <c r="B44" s="70" t="s">
+      <c r="B44" s="152" t="s">
         <v>432</v>
       </c>
       <c r="C44" s="111" t="s">
@@ -32302,10 +32386,10 @@
       <c r="D44" s="106"/>
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="229" t="s">
+      <c r="A45" s="233" t="s">
         <v>165</v>
       </c>
-      <c r="B45" s="206" t="s">
+      <c r="B45" s="210" t="s">
         <v>432</v>
       </c>
       <c r="C45" s="106"/>
@@ -32314,8 +32398,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="230"/>
-      <c r="B46" s="210"/>
+      <c r="A46" s="234"/>
+      <c r="B46" s="214"/>
       <c r="C46" s="111" t="s">
         <v>356</v>
       </c>
@@ -32324,8 +32408,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="230"/>
-      <c r="B47" s="210"/>
+      <c r="A47" s="234"/>
+      <c r="B47" s="214"/>
       <c r="C47" s="111" t="s">
         <v>354</v>
       </c>
@@ -32334,8 +32418,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="230"/>
-      <c r="B48" s="210"/>
+      <c r="A48" s="234"/>
+      <c r="B48" s="214"/>
       <c r="C48" s="114" t="s">
         <v>362</v>
       </c>
@@ -32344,8 +32428,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="230"/>
-      <c r="B49" s="210"/>
+      <c r="A49" s="234"/>
+      <c r="B49" s="214"/>
       <c r="C49" s="111" t="s">
         <v>354</v>
       </c>
@@ -32354,8 +32438,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="230"/>
-      <c r="B50" s="210"/>
+      <c r="A50" s="234"/>
+      <c r="B50" s="214"/>
       <c r="C50" s="111" t="s">
         <v>366</v>
       </c>
@@ -32364,8 +32448,8 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="230"/>
-      <c r="B51" s="210"/>
+      <c r="A51" s="234"/>
+      <c r="B51" s="214"/>
       <c r="C51" s="111" t="s">
         <v>354</v>
       </c>
@@ -32374,8 +32458,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="230"/>
-      <c r="B52" s="210"/>
+      <c r="A52" s="234"/>
+      <c r="B52" s="214"/>
       <c r="C52" s="130" t="s">
         <v>461</v>
       </c>
@@ -32384,8 +32468,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="230"/>
-      <c r="B53" s="210"/>
+      <c r="A53" s="234"/>
+      <c r="B53" s="214"/>
       <c r="C53" s="130" t="s">
         <v>456</v>
       </c>
@@ -32394,8 +32478,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="230"/>
-      <c r="B54" s="210"/>
+      <c r="A54" s="234"/>
+      <c r="B54" s="214"/>
       <c r="C54" s="130" t="s">
         <v>354</v>
       </c>
@@ -32404,8 +32488,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="230"/>
-      <c r="B55" s="210"/>
+      <c r="A55" s="234"/>
+      <c r="B55" s="214"/>
       <c r="C55" s="130" t="s">
         <v>456</v>
       </c>
@@ -32414,29 +32498,29 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="230"/>
-      <c r="B56" s="210"/>
-      <c r="C56" s="151" t="s">
+      <c r="A56" s="234"/>
+      <c r="B56" s="214"/>
+      <c r="C56" s="145" t="s">
         <v>354</v>
       </c>
-      <c r="D56" s="136" t="s">
+      <c r="D56" s="135" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="230"/>
-      <c r="B57" s="210"/>
-      <c r="C57" s="151" t="s">
+      <c r="A57" s="234"/>
+      <c r="B57" s="214"/>
+      <c r="C57" s="145" t="s">
         <v>480</v>
       </c>
-      <c r="D57" s="136" t="s">
+      <c r="D57" s="135" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="230"/>
-      <c r="B58" s="210"/>
-      <c r="C58" s="153" t="s">
+      <c r="A58" s="234"/>
+      <c r="B58" s="214"/>
+      <c r="C58" s="147" t="s">
         <v>491</v>
       </c>
       <c r="D58" s="58" t="s">
@@ -32444,9 +32528,9 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="230"/>
-      <c r="B59" s="210"/>
-      <c r="C59" s="153" t="s">
+      <c r="A59" s="234"/>
+      <c r="B59" s="214"/>
+      <c r="C59" s="147" t="s">
         <v>480</v>
       </c>
       <c r="D59" s="58" t="s">
@@ -32457,7 +32541,7 @@
       <c r="A60" s="115" t="s">
         <v>326</v>
       </c>
-      <c r="B60" s="70" t="s">
+      <c r="B60" s="152" t="s">
         <v>432</v>
       </c>
       <c r="C60" s="111" t="s">
@@ -32471,7 +32555,7 @@
       <c r="A61" s="115" t="s">
         <v>346</v>
       </c>
-      <c r="B61" s="70" t="s">
+      <c r="B61" s="152" t="s">
         <v>432</v>
       </c>
       <c r="C61" s="111" t="s">
@@ -32480,10 +32564,10 @@
       <c r="D61" s="112"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="204" t="s">
+      <c r="A62" s="208" t="s">
         <v>364</v>
       </c>
-      <c r="B62" s="206" t="s">
+      <c r="B62" s="210" t="s">
         <v>432</v>
       </c>
       <c r="C62" s="111" t="s">
@@ -32492,8 +32576,8 @@
       <c r="D62" s="112"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="205"/>
-      <c r="B63" s="207"/>
+      <c r="A63" s="209"/>
+      <c r="B63" s="211"/>
       <c r="C63" s="111" t="s">
         <v>399</v>
       </c>
@@ -32505,15 +32589,15 @@
       <c r="A64" s="103" t="s">
         <v>28</v>
       </c>
-      <c r="B64" s="103"/>
+      <c r="B64" s="155"/>
       <c r="C64" s="103"/>
       <c r="D64" s="103"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="204" t="s">
+      <c r="A65" s="208" t="s">
         <v>236</v>
       </c>
-      <c r="B65" s="206" t="s">
+      <c r="B65" s="210" t="s">
         <v>432</v>
       </c>
       <c r="C65" s="106"/>
@@ -32522,24 +32606,24 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="212"/>
-      <c r="B66" s="210"/>
+      <c r="A66" s="216"/>
+      <c r="B66" s="214"/>
       <c r="C66" s="106"/>
       <c r="D66" s="106" t="s">
         <v>443</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="212"/>
-      <c r="B67" s="210"/>
+      <c r="A67" s="216"/>
+      <c r="B67" s="214"/>
       <c r="C67" s="106"/>
       <c r="D67" s="106" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="212"/>
-      <c r="B68" s="210"/>
+      <c r="A68" s="216"/>
+      <c r="B68" s="214"/>
       <c r="C68" s="106" t="s">
         <v>295</v>
       </c>
@@ -32548,8 +32632,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="212"/>
-      <c r="B69" s="210"/>
+      <c r="A69" s="216"/>
+      <c r="B69" s="214"/>
       <c r="C69" s="106" t="s">
         <v>323</v>
       </c>
@@ -32558,8 +32642,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="212"/>
-      <c r="B70" s="210"/>
+      <c r="A70" s="216"/>
+      <c r="B70" s="214"/>
       <c r="C70" s="106" t="s">
         <v>368</v>
       </c>
@@ -32568,8 +32652,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="212"/>
-      <c r="B71" s="210"/>
+      <c r="A71" s="216"/>
+      <c r="B71" s="214"/>
       <c r="C71" s="61" t="s">
         <v>472</v>
       </c>
@@ -32578,8 +32662,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="212"/>
-      <c r="B72" s="210"/>
+      <c r="A72" s="216"/>
+      <c r="B72" s="214"/>
       <c r="C72" s="58" t="s">
         <v>37</v>
       </c>
@@ -32588,9 +32672,9 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="212"/>
-      <c r="B73" s="210"/>
-      <c r="C73" s="138" t="s">
+      <c r="A73" s="216"/>
+      <c r="B73" s="214"/>
+      <c r="C73" s="137" t="s">
         <v>354</v>
       </c>
       <c r="D73" s="58" t="s">
@@ -32598,9 +32682,9 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="212"/>
-      <c r="B74" s="210"/>
-      <c r="C74" s="138" t="s">
+      <c r="A74" s="216"/>
+      <c r="B74" s="214"/>
+      <c r="C74" s="137" t="s">
         <v>456</v>
       </c>
       <c r="D74" s="58" t="s">
@@ -32608,19 +32692,19 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="212"/>
-      <c r="B75" s="210"/>
-      <c r="C75" s="138" t="s">
+      <c r="A75" s="216"/>
+      <c r="B75" s="214"/>
+      <c r="C75" s="137" t="s">
         <v>480</v>
       </c>
-      <c r="D75" s="136" t="s">
+      <c r="D75" s="135" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="212"/>
-      <c r="B76" s="210"/>
-      <c r="C76" s="152" t="s">
+      <c r="A76" s="216"/>
+      <c r="B76" s="214"/>
+      <c r="C76" s="146" t="s">
         <v>491</v>
       </c>
       <c r="D76" s="58" t="s">
@@ -32628,9 +32712,9 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="212"/>
-      <c r="B77" s="210"/>
-      <c r="C77" s="152" t="s">
+      <c r="A77" s="216"/>
+      <c r="B77" s="214"/>
+      <c r="C77" s="146" t="s">
         <v>480</v>
       </c>
       <c r="D77" s="58" t="s">
@@ -32638,10 +32722,10 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="213" t="s">
+      <c r="A78" s="217" t="s">
         <v>27</v>
       </c>
-      <c r="B78" s="206" t="s">
+      <c r="B78" s="210" t="s">
         <v>432</v>
       </c>
       <c r="C78" s="106" t="s">
@@ -32652,16 +32736,16 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="214"/>
-      <c r="B79" s="210"/>
+      <c r="A79" s="218"/>
+      <c r="B79" s="214"/>
       <c r="C79" s="106"/>
       <c r="D79" s="106" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A80" s="214"/>
-      <c r="B80" s="210"/>
+      <c r="A80" s="218"/>
+      <c r="B80" s="214"/>
       <c r="C80" s="116" t="s">
         <v>324</v>
       </c>
@@ -32670,8 +32754,8 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="214"/>
-      <c r="B81" s="210"/>
+      <c r="A81" s="218"/>
+      <c r="B81" s="214"/>
       <c r="C81" s="116" t="s">
         <v>494</v>
       </c>
@@ -32680,8 +32764,8 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="214"/>
-      <c r="B82" s="210"/>
+      <c r="A82" s="218"/>
+      <c r="B82" s="214"/>
       <c r="C82" s="116" t="s">
         <v>354</v>
       </c>
@@ -32690,8 +32774,8 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="214"/>
-      <c r="B83" s="210"/>
+      <c r="A83" s="218"/>
+      <c r="B83" s="214"/>
       <c r="C83" s="116" t="s">
         <v>362</v>
       </c>
@@ -32700,8 +32784,8 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="214"/>
-      <c r="B84" s="210"/>
+      <c r="A84" s="218"/>
+      <c r="B84" s="214"/>
       <c r="C84" s="116" t="s">
         <v>366</v>
       </c>
@@ -32710,8 +32794,8 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="214"/>
-      <c r="B85" s="210"/>
+      <c r="A85" s="218"/>
+      <c r="B85" s="214"/>
       <c r="C85" s="116" t="s">
         <v>376</v>
       </c>
@@ -32720,8 +32804,8 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="214"/>
-      <c r="B86" s="210"/>
+      <c r="A86" s="218"/>
+      <c r="B86" s="214"/>
       <c r="C86" s="108" t="s">
         <v>354</v>
       </c>
@@ -32730,9 +32814,9 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="214"/>
-      <c r="B87" s="210"/>
-      <c r="C87" s="138" t="s">
+      <c r="A87" s="218"/>
+      <c r="B87" s="214"/>
+      <c r="C87" s="137" t="s">
         <v>461</v>
       </c>
       <c r="D87" s="58" t="s">
@@ -32740,9 +32824,9 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="214"/>
-      <c r="B88" s="210"/>
-      <c r="C88" s="138" t="s">
+      <c r="A88" s="218"/>
+      <c r="B88" s="214"/>
+      <c r="C88" s="137" t="s">
         <v>456</v>
       </c>
       <c r="D88" s="58" t="s">
@@ -32750,9 +32834,9 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="214"/>
-      <c r="B89" s="210"/>
-      <c r="C89" s="138" t="s">
+      <c r="A89" s="218"/>
+      <c r="B89" s="214"/>
+      <c r="C89" s="137" t="s">
         <v>354</v>
       </c>
       <c r="D89" s="58" t="s">
@@ -32760,9 +32844,9 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="214"/>
-      <c r="B90" s="210"/>
-      <c r="C90" s="138" t="s">
+      <c r="A90" s="218"/>
+      <c r="B90" s="214"/>
+      <c r="C90" s="137" t="s">
         <v>456</v>
       </c>
       <c r="D90" s="58" t="s">
@@ -32770,9 +32854,9 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="214"/>
-      <c r="B91" s="210"/>
-      <c r="C91" s="138" t="s">
+      <c r="A91" s="218"/>
+      <c r="B91" s="214"/>
+      <c r="C91" s="137" t="s">
         <v>368</v>
       </c>
       <c r="D91" s="58" t="s">
@@ -32780,29 +32864,29 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="214"/>
-      <c r="B92" s="210"/>
-      <c r="C92" s="138" t="s">
+      <c r="A92" s="218"/>
+      <c r="B92" s="214"/>
+      <c r="C92" s="137" t="s">
         <v>354</v>
       </c>
-      <c r="D92" s="136" t="s">
+      <c r="D92" s="135" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="214"/>
-      <c r="B93" s="210"/>
-      <c r="C93" s="138" t="s">
+      <c r="A93" s="218"/>
+      <c r="B93" s="214"/>
+      <c r="C93" s="137" t="s">
         <v>480</v>
       </c>
-      <c r="D93" s="136" t="s">
+      <c r="D93" s="135" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="214"/>
-      <c r="B94" s="210"/>
-      <c r="C94" s="152" t="s">
+      <c r="A94" s="218"/>
+      <c r="B94" s="214"/>
+      <c r="C94" s="146" t="s">
         <v>491</v>
       </c>
       <c r="D94" s="58" t="s">
@@ -32810,9 +32894,9 @@
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="215"/>
-      <c r="B95" s="207"/>
-      <c r="C95" s="152" t="s">
+      <c r="A95" s="219"/>
+      <c r="B95" s="211"/>
+      <c r="C95" s="146" t="s">
         <v>480</v>
       </c>
       <c r="D95" s="58" t="s">
@@ -32820,13 +32904,13 @@
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="208" t="s">
+      <c r="A96" s="212" t="s">
         <v>222</v>
       </c>
-      <c r="B96" s="206" t="s">
+      <c r="B96" s="210" t="s">
         <v>432</v>
       </c>
-      <c r="C96" s="224" t="s">
+      <c r="C96" s="228" t="s">
         <v>238</v>
       </c>
       <c r="D96" s="96" t="s">
@@ -32834,17 +32918,17 @@
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="209"/>
-      <c r="B97" s="210"/>
-      <c r="C97" s="225"/>
+      <c r="A97" s="213"/>
+      <c r="B97" s="214"/>
+      <c r="C97" s="229"/>
       <c r="D97" s="112" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="209"/>
-      <c r="B98" s="210"/>
-      <c r="C98" s="221" t="s">
+      <c r="A98" s="213"/>
+      <c r="B98" s="214"/>
+      <c r="C98" s="225" t="s">
         <v>239</v>
       </c>
       <c r="D98" s="106" t="s">
@@ -32852,16 +32936,16 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A99" s="209"/>
-      <c r="B99" s="210"/>
-      <c r="C99" s="221"/>
+      <c r="A99" s="213"/>
+      <c r="B99" s="214"/>
+      <c r="C99" s="225"/>
       <c r="D99" s="118" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="209"/>
-      <c r="B100" s="210"/>
+      <c r="A100" s="213"/>
+      <c r="B100" s="214"/>
       <c r="C100" s="111" t="s">
         <v>302</v>
       </c>
@@ -32870,8 +32954,8 @@
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="209"/>
-      <c r="B101" s="210"/>
+      <c r="A101" s="213"/>
+      <c r="B101" s="214"/>
       <c r="C101" s="111">
         <v>2.1</v>
       </c>
@@ -32880,8 +32964,8 @@
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="209"/>
-      <c r="B102" s="210"/>
+      <c r="A102" s="213"/>
+      <c r="B102" s="214"/>
       <c r="C102" s="111" t="s">
         <v>238</v>
       </c>
@@ -32890,8 +32974,8 @@
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="209"/>
-      <c r="B103" s="210"/>
+      <c r="A103" s="213"/>
+      <c r="B103" s="214"/>
       <c r="C103" s="111" t="s">
         <v>238</v>
       </c>
@@ -32900,8 +32984,8 @@
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="209"/>
-      <c r="B104" s="210"/>
+      <c r="A104" s="213"/>
+      <c r="B104" s="214"/>
       <c r="C104" s="111" t="s">
         <v>238</v>
       </c>
@@ -32910,8 +32994,8 @@
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="209"/>
-      <c r="B105" s="210"/>
+      <c r="A105" s="213"/>
+      <c r="B105" s="214"/>
       <c r="C105" s="119" t="s">
         <v>373</v>
       </c>
@@ -32920,8 +33004,8 @@
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="209"/>
-      <c r="B106" s="210"/>
+      <c r="A106" s="213"/>
+      <c r="B106" s="214"/>
       <c r="C106" s="111">
         <v>2.1</v>
       </c>
@@ -32930,8 +33014,8 @@
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="209"/>
-      <c r="B107" s="210"/>
+      <c r="A107" s="213"/>
+      <c r="B107" s="214"/>
       <c r="C107" s="111" t="s">
         <v>238</v>
       </c>
@@ -32940,8 +33024,8 @@
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="209"/>
-      <c r="B108" s="210"/>
+      <c r="A108" s="213"/>
+      <c r="B108" s="214"/>
       <c r="C108" s="111" t="s">
         <v>238</v>
       </c>
@@ -32950,8 +33034,8 @@
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="209"/>
-      <c r="B109" s="210"/>
+      <c r="A109" s="213"/>
+      <c r="B109" s="214"/>
       <c r="C109" s="111">
         <v>2.1</v>
       </c>
@@ -32960,10 +33044,10 @@
       </c>
     </row>
     <row r="110" spans="1:4" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="213" t="s">
+      <c r="A110" s="217" t="s">
         <v>291</v>
       </c>
-      <c r="B110" s="206" t="s">
+      <c r="B110" s="210" t="s">
         <v>432</v>
       </c>
       <c r="C110" s="106" t="s">
@@ -32974,8 +33058,8 @@
       </c>
     </row>
     <row r="111" spans="1:4" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="214"/>
-      <c r="B111" s="210"/>
+      <c r="A111" s="218"/>
+      <c r="B111" s="214"/>
       <c r="C111" s="106" t="s">
         <v>494</v>
       </c>
@@ -32984,8 +33068,8 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A112" s="214"/>
-      <c r="B112" s="210"/>
+      <c r="A112" s="218"/>
+      <c r="B112" s="214"/>
       <c r="C112" s="118" t="s">
         <v>276</v>
       </c>
@@ -32994,8 +33078,8 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="215"/>
-      <c r="B113" s="207"/>
+      <c r="A113" s="219"/>
+      <c r="B113" s="211"/>
       <c r="C113" s="106" t="s">
         <v>345</v>
       </c>
@@ -33004,10 +33088,10 @@
       </c>
     </row>
     <row r="114" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="204" t="s">
+      <c r="A114" s="208" t="s">
         <v>365</v>
       </c>
-      <c r="B114" s="206" t="s">
+      <c r="B114" s="210" t="s">
         <v>432</v>
       </c>
       <c r="C114" s="111" t="s">
@@ -33016,8 +33100,8 @@
       <c r="D114" s="106"/>
     </row>
     <row r="115" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="212"/>
-      <c r="B115" s="210"/>
+      <c r="A115" s="216"/>
+      <c r="B115" s="214"/>
       <c r="C115" s="111" t="s">
         <v>373</v>
       </c>
@@ -33026,8 +33110,8 @@
       </c>
     </row>
     <row r="116" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="212"/>
-      <c r="B116" s="210"/>
+      <c r="A116" s="216"/>
+      <c r="B116" s="214"/>
       <c r="C116" s="111">
         <v>2.1</v>
       </c>
@@ -33036,8 +33120,8 @@
       </c>
     </row>
     <row r="117" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="212"/>
-      <c r="B117" s="210"/>
+      <c r="A117" s="216"/>
+      <c r="B117" s="214"/>
       <c r="C117" s="111" t="s">
         <v>239</v>
       </c>
@@ -33046,8 +33130,8 @@
       </c>
     </row>
     <row r="118" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="212"/>
-      <c r="B118" s="210"/>
+      <c r="A118" s="216"/>
+      <c r="B118" s="214"/>
       <c r="C118" s="111" t="s">
         <v>238</v>
       </c>
@@ -33059,7 +33143,7 @@
       <c r="A119" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="B119" s="103"/>
+      <c r="B119" s="155"/>
       <c r="C119" s="103"/>
       <c r="D119" s="104"/>
     </row>
@@ -33076,10 +33160,10 @@
       <c r="D120" s="112"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="208" t="s">
+      <c r="A121" s="212" t="s">
         <v>256</v>
       </c>
-      <c r="B121" s="206" t="s">
+      <c r="B121" s="210" t="s">
         <v>432</v>
       </c>
       <c r="C121" s="106"/>
@@ -33088,24 +33172,24 @@
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="209"/>
-      <c r="B122" s="210"/>
+      <c r="A122" s="213"/>
+      <c r="B122" s="214"/>
       <c r="C122" s="106"/>
       <c r="D122" s="106" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="209"/>
-      <c r="B123" s="210"/>
+      <c r="A123" s="213"/>
+      <c r="B123" s="214"/>
       <c r="C123" s="106"/>
       <c r="D123" s="112" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="209"/>
-      <c r="B124" s="210"/>
+      <c r="A124" s="213"/>
+      <c r="B124" s="214"/>
       <c r="C124" s="106" t="s">
         <v>419</v>
       </c>
@@ -33114,8 +33198,8 @@
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="209"/>
-      <c r="B125" s="210"/>
+      <c r="A125" s="213"/>
+      <c r="B125" s="214"/>
       <c r="C125" s="106" t="s">
         <v>424</v>
       </c>
@@ -33124,8 +33208,8 @@
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="209"/>
-      <c r="B126" s="210"/>
+      <c r="A126" s="213"/>
+      <c r="B126" s="214"/>
       <c r="C126" s="58" t="s">
         <v>474</v>
       </c>
@@ -33134,8 +33218,8 @@
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="209"/>
-      <c r="B127" s="210"/>
+      <c r="A127" s="213"/>
+      <c r="B127" s="214"/>
       <c r="C127" s="58" t="s">
         <v>480</v>
       </c>
@@ -33144,10 +33228,10 @@
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="222" t="s">
+      <c r="A128" s="226" t="s">
         <v>329</v>
       </c>
-      <c r="B128" s="223" t="s">
+      <c r="B128" s="227" t="s">
         <v>432</v>
       </c>
       <c r="C128" s="80" t="s">
@@ -33158,8 +33242,8 @@
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A129" s="222"/>
-      <c r="B129" s="223"/>
+      <c r="A129" s="226"/>
+      <c r="B129" s="227"/>
       <c r="C129" s="106" t="s">
         <v>406</v>
       </c>
@@ -33168,43 +33252,43 @@
       </c>
     </row>
     <row r="130" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A130" s="222"/>
-      <c r="B130" s="223"/>
+      <c r="A130" s="226"/>
+      <c r="B130" s="227"/>
       <c r="C130" s="121" t="s">
         <v>409</v>
       </c>
-      <c r="D130" s="204" t="s">
+      <c r="D130" s="208" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A131" s="222"/>
-      <c r="B131" s="223"/>
+      <c r="A131" s="226"/>
+      <c r="B131" s="227"/>
       <c r="C131" s="121" t="s">
         <v>410</v>
       </c>
-      <c r="D131" s="212"/>
+      <c r="D131" s="216"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="222"/>
-      <c r="B132" s="223"/>
+      <c r="A132" s="226"/>
+      <c r="B132" s="227"/>
       <c r="C132" s="121" t="s">
         <v>411</v>
       </c>
-      <c r="D132" s="212"/>
+      <c r="D132" s="216"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="222"/>
-      <c r="B133" s="223"/>
+      <c r="A133" s="226"/>
+      <c r="B133" s="227"/>
       <c r="C133" s="121" t="s">
         <v>412</v>
       </c>
-      <c r="D133" s="212"/>
+      <c r="D133" s="216"/>
     </row>
     <row r="134" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A134" s="222"/>
-      <c r="B134" s="223"/>
-      <c r="C134" s="139" t="s">
+      <c r="A134" s="226"/>
+      <c r="B134" s="227"/>
+      <c r="C134" s="138" t="s">
         <v>475</v>
       </c>
       <c r="D134" s="67" t="s">
@@ -33226,10 +33310,10 @@
       </c>
     </row>
     <row r="136" spans="1:4" ht="30.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="216" t="s">
+      <c r="A136" s="220" t="s">
         <v>32</v>
       </c>
-      <c r="B136" s="206" t="s">
+      <c r="B136" s="210" t="s">
         <v>432</v>
       </c>
       <c r="C136" s="106" t="s">
@@ -33240,8 +33324,8 @@
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A137" s="217"/>
-      <c r="B137" s="210"/>
+      <c r="A137" s="221"/>
+      <c r="B137" s="214"/>
       <c r="C137" s="106" t="s">
         <v>265</v>
       </c>
@@ -33250,8 +33334,8 @@
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="217"/>
-      <c r="B138" s="210"/>
+      <c r="A138" s="221"/>
+      <c r="B138" s="214"/>
       <c r="C138" s="106" t="s">
         <v>264</v>
       </c>
@@ -33260,8 +33344,8 @@
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="217"/>
-      <c r="B139" s="210"/>
+      <c r="A139" s="221"/>
+      <c r="B139" s="214"/>
       <c r="C139" s="112" t="s">
         <v>272</v>
       </c>
@@ -33270,8 +33354,8 @@
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="217"/>
-      <c r="B140" s="210"/>
+      <c r="A140" s="221"/>
+      <c r="B140" s="214"/>
       <c r="C140" s="106" t="s">
         <v>277</v>
       </c>
@@ -33280,8 +33364,8 @@
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="217"/>
-      <c r="B141" s="210"/>
+      <c r="A141" s="221"/>
+      <c r="B141" s="214"/>
       <c r="C141" s="106" t="s">
         <v>278</v>
       </c>
@@ -33290,8 +33374,8 @@
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="217"/>
-      <c r="B142" s="210"/>
+      <c r="A142" s="221"/>
+      <c r="B142" s="214"/>
       <c r="C142" s="112" t="s">
         <v>283</v>
       </c>
@@ -33300,8 +33384,8 @@
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="217"/>
-      <c r="B143" s="210"/>
+      <c r="A143" s="221"/>
+      <c r="B143" s="214"/>
       <c r="C143" s="112" t="s">
         <v>297</v>
       </c>
@@ -33310,8 +33394,8 @@
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="217"/>
-      <c r="B144" s="210"/>
+      <c r="A144" s="221"/>
+      <c r="B144" s="214"/>
       <c r="C144" s="112" t="s">
         <v>284</v>
       </c>
@@ -33320,8 +33404,8 @@
       </c>
     </row>
     <row r="145" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A145" s="217"/>
-      <c r="B145" s="210"/>
+      <c r="A145" s="221"/>
+      <c r="B145" s="214"/>
       <c r="C145" s="122" t="s">
         <v>243</v>
       </c>
@@ -33330,8 +33414,8 @@
       </c>
     </row>
     <row r="146" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A146" s="217"/>
-      <c r="B146" s="210"/>
+      <c r="A146" s="221"/>
+      <c r="B146" s="214"/>
       <c r="C146" s="116" t="s">
         <v>306</v>
       </c>
@@ -33340,8 +33424,8 @@
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="217"/>
-      <c r="B147" s="210"/>
+      <c r="A147" s="221"/>
+      <c r="B147" s="214"/>
       <c r="C147" s="106" t="s">
         <v>307</v>
       </c>
@@ -33350,8 +33434,8 @@
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="217"/>
-      <c r="B148" s="210"/>
+      <c r="A148" s="221"/>
+      <c r="B148" s="214"/>
       <c r="C148" s="112" t="s">
         <v>308</v>
       </c>
@@ -33360,8 +33444,8 @@
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="217"/>
-      <c r="B149" s="210"/>
+      <c r="A149" s="221"/>
+      <c r="B149" s="214"/>
       <c r="C149" s="112" t="s">
         <v>310</v>
       </c>
@@ -33370,8 +33454,8 @@
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="217"/>
-      <c r="B150" s="210"/>
+      <c r="A150" s="221"/>
+      <c r="B150" s="214"/>
       <c r="C150" s="112" t="s">
         <v>263</v>
       </c>
@@ -33380,8 +33464,8 @@
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="217"/>
-      <c r="B151" s="210"/>
+      <c r="A151" s="221"/>
+      <c r="B151" s="214"/>
       <c r="C151" s="106" t="s">
         <v>313</v>
       </c>
@@ -33390,8 +33474,8 @@
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="217"/>
-      <c r="B152" s="210"/>
+      <c r="A152" s="221"/>
+      <c r="B152" s="214"/>
       <c r="C152" s="112" t="s">
         <v>278</v>
       </c>
@@ -33400,8 +33484,8 @@
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="217"/>
-      <c r="B153" s="210"/>
+      <c r="A153" s="221"/>
+      <c r="B153" s="214"/>
       <c r="C153" s="112" t="s">
         <v>314</v>
       </c>
@@ -33410,16 +33494,16 @@
       </c>
     </row>
     <row r="154" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A154" s="217"/>
-      <c r="B154" s="210"/>
+      <c r="A154" s="221"/>
+      <c r="B154" s="214"/>
       <c r="C154" s="106"/>
       <c r="D154" s="97" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="217"/>
-      <c r="B155" s="210"/>
+      <c r="A155" s="221"/>
+      <c r="B155" s="214"/>
       <c r="C155" s="112" t="s">
         <v>317</v>
       </c>
@@ -33428,8 +33512,8 @@
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="217"/>
-      <c r="B156" s="210"/>
+      <c r="A156" s="221"/>
+      <c r="B156" s="214"/>
       <c r="C156" s="112" t="s">
         <v>263</v>
       </c>
@@ -33438,8 +33522,8 @@
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="217"/>
-      <c r="B157" s="210"/>
+      <c r="A157" s="221"/>
+      <c r="B157" s="214"/>
       <c r="C157" s="112" t="s">
         <v>334</v>
       </c>
@@ -33448,8 +33532,8 @@
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="217"/>
-      <c r="B158" s="210"/>
+      <c r="A158" s="221"/>
+      <c r="B158" s="214"/>
       <c r="C158" s="112" t="s">
         <v>335</v>
       </c>
@@ -33458,8 +33542,8 @@
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="217"/>
-      <c r="B159" s="210"/>
+      <c r="A159" s="221"/>
+      <c r="B159" s="214"/>
       <c r="C159" s="112" t="s">
         <v>319</v>
       </c>
@@ -33468,8 +33552,8 @@
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="217"/>
-      <c r="B160" s="210"/>
+      <c r="A160" s="221"/>
+      <c r="B160" s="214"/>
       <c r="C160" s="117" t="s">
         <v>340</v>
       </c>
@@ -33478,8 +33562,8 @@
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A161" s="217"/>
-      <c r="B161" s="210"/>
+      <c r="A161" s="221"/>
+      <c r="B161" s="214"/>
       <c r="C161" s="112" t="s">
         <v>333</v>
       </c>
@@ -33488,8 +33572,8 @@
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="217"/>
-      <c r="B162" s="210"/>
+      <c r="A162" s="221"/>
+      <c r="B162" s="214"/>
       <c r="C162" s="112" t="s">
         <v>348</v>
       </c>
@@ -33498,8 +33582,8 @@
       </c>
     </row>
     <row r="163" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A163" s="217"/>
-      <c r="B163" s="210"/>
+      <c r="A163" s="221"/>
+      <c r="B163" s="214"/>
       <c r="C163" s="101" t="s">
         <v>351</v>
       </c>
@@ -33508,8 +33592,8 @@
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="217"/>
-      <c r="B164" s="210"/>
+      <c r="A164" s="221"/>
+      <c r="B164" s="214"/>
       <c r="C164" s="112" t="s">
         <v>352</v>
       </c>
@@ -33518,8 +33602,8 @@
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="217"/>
-      <c r="B165" s="210"/>
+      <c r="A165" s="221"/>
+      <c r="B165" s="214"/>
       <c r="C165" s="112" t="s">
         <v>353</v>
       </c>
@@ -33528,8 +33612,8 @@
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="217"/>
-      <c r="B166" s="210"/>
+      <c r="A166" s="221"/>
+      <c r="B166" s="214"/>
       <c r="C166" s="112" t="s">
         <v>359</v>
       </c>
@@ -33538,8 +33622,8 @@
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="217"/>
-      <c r="B167" s="210"/>
+      <c r="A167" s="221"/>
+      <c r="B167" s="214"/>
       <c r="C167" s="112" t="s">
         <v>361</v>
       </c>
@@ -33548,8 +33632,8 @@
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="217"/>
-      <c r="B168" s="210"/>
+      <c r="A168" s="221"/>
+      <c r="B168" s="214"/>
       <c r="C168" s="112" t="s">
         <v>367</v>
       </c>
@@ -33558,8 +33642,8 @@
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="217"/>
-      <c r="B169" s="210"/>
+      <c r="A169" s="221"/>
+      <c r="B169" s="214"/>
       <c r="C169" s="112" t="s">
         <v>359</v>
       </c>
@@ -33568,8 +33652,8 @@
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="217"/>
-      <c r="B170" s="210"/>
+      <c r="A170" s="221"/>
+      <c r="B170" s="214"/>
       <c r="C170" s="117" t="s">
         <v>380</v>
       </c>
@@ -33578,8 +33662,8 @@
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="217"/>
-      <c r="B171" s="210"/>
+      <c r="A171" s="221"/>
+      <c r="B171" s="214"/>
       <c r="C171" s="106" t="s">
         <v>384</v>
       </c>
@@ -33588,8 +33672,8 @@
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="217"/>
-      <c r="B172" s="210"/>
+      <c r="A172" s="221"/>
+      <c r="B172" s="214"/>
       <c r="C172" s="106" t="s">
         <v>387</v>
       </c>
@@ -33598,8 +33682,8 @@
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="217"/>
-      <c r="B173" s="210"/>
+      <c r="A173" s="221"/>
+      <c r="B173" s="214"/>
       <c r="C173" s="106" t="s">
         <v>388</v>
       </c>
@@ -33608,8 +33692,8 @@
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="217"/>
-      <c r="B174" s="210"/>
+      <c r="A174" s="221"/>
+      <c r="B174" s="214"/>
       <c r="C174" s="106" t="s">
         <v>389</v>
       </c>
@@ -33618,8 +33702,8 @@
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="217"/>
-      <c r="B175" s="210"/>
+      <c r="A175" s="221"/>
+      <c r="B175" s="214"/>
       <c r="C175" s="106" t="s">
         <v>390</v>
       </c>
@@ -33628,8 +33712,8 @@
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="217"/>
-      <c r="B176" s="210"/>
+      <c r="A176" s="221"/>
+      <c r="B176" s="214"/>
       <c r="C176" s="106" t="s">
         <v>391</v>
       </c>
@@ -33638,8 +33722,8 @@
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A177" s="217"/>
-      <c r="B177" s="210"/>
+      <c r="A177" s="221"/>
+      <c r="B177" s="214"/>
       <c r="C177" s="106" t="s">
         <v>394</v>
       </c>
@@ -33648,8 +33732,8 @@
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="217"/>
-      <c r="B178" s="210"/>
+      <c r="A178" s="221"/>
+      <c r="B178" s="214"/>
       <c r="C178" s="106" t="s">
         <v>404</v>
       </c>
@@ -33658,8 +33742,8 @@
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="217"/>
-      <c r="B179" s="210"/>
+      <c r="A179" s="221"/>
+      <c r="B179" s="214"/>
       <c r="C179" s="106" t="s">
         <v>405</v>
       </c>
@@ -33668,8 +33752,8 @@
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="217"/>
-      <c r="B180" s="210"/>
+      <c r="A180" s="221"/>
+      <c r="B180" s="214"/>
       <c r="C180" s="106" t="s">
         <v>422</v>
       </c>
@@ -33678,8 +33762,8 @@
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="217"/>
-      <c r="B181" s="210"/>
+      <c r="A181" s="221"/>
+      <c r="B181" s="214"/>
       <c r="C181" s="106" t="s">
         <v>423</v>
       </c>
@@ -33688,8 +33772,8 @@
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="217"/>
-      <c r="B182" s="210"/>
+      <c r="A182" s="221"/>
+      <c r="B182" s="214"/>
       <c r="C182" s="106" t="s">
         <v>426</v>
       </c>
@@ -33698,8 +33782,8 @@
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="217"/>
-      <c r="B183" s="210"/>
+      <c r="A183" s="221"/>
+      <c r="B183" s="214"/>
       <c r="C183" s="58" t="s">
         <v>477</v>
       </c>
@@ -33708,8 +33792,8 @@
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="217"/>
-      <c r="B184" s="210"/>
+      <c r="A184" s="221"/>
+      <c r="B184" s="214"/>
       <c r="C184" s="106" t="s">
         <v>422</v>
       </c>
@@ -33718,8 +33802,8 @@
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A185" s="217"/>
-      <c r="B185" s="210"/>
+      <c r="A185" s="221"/>
+      <c r="B185" s="214"/>
       <c r="C185" s="106" t="s">
         <v>476</v>
       </c>
@@ -33728,8 +33812,8 @@
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="218"/>
-      <c r="B186" s="207"/>
+      <c r="A186" s="222"/>
+      <c r="B186" s="211"/>
       <c r="C186" s="112" t="s">
         <v>333</v>
       </c>
@@ -33738,10 +33822,10 @@
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="216" t="s">
+      <c r="A187" s="220" t="s">
         <v>416</v>
       </c>
-      <c r="B187" s="206" t="s">
+      <c r="B187" s="210" t="s">
         <v>432</v>
       </c>
       <c r="C187" s="106" t="s">
@@ -33752,8 +33836,8 @@
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="217"/>
-      <c r="B188" s="210"/>
+      <c r="A188" s="221"/>
+      <c r="B188" s="214"/>
       <c r="C188" s="58" t="s">
         <v>478</v>
       </c>
@@ -33762,8 +33846,8 @@
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="218"/>
-      <c r="B189" s="207"/>
+      <c r="A189" s="222"/>
+      <c r="B189" s="211"/>
       <c r="C189" s="58" t="s">
         <v>483</v>
       </c>
@@ -33775,7 +33859,7 @@
       <c r="A190" s="108" t="s">
         <v>304</v>
       </c>
-      <c r="B190" s="70" t="s">
+      <c r="B190" s="152" t="s">
         <v>432</v>
       </c>
       <c r="C190" s="106" t="s">
@@ -33789,7 +33873,7 @@
       <c r="A191" s="108" t="s">
         <v>305</v>
       </c>
-      <c r="B191" s="70" t="s">
+      <c r="B191" s="152" t="s">
         <v>432</v>
       </c>
       <c r="C191" s="106" t="s">
@@ -33803,15 +33887,15 @@
       <c r="A192" s="103" t="s">
         <v>40</v>
       </c>
-      <c r="B192" s="103"/>
+      <c r="B192" s="155"/>
       <c r="C192" s="103"/>
       <c r="D192" s="104"/>
     </row>
     <row r="193" spans="1:4" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="208" t="s">
+      <c r="A193" s="212" t="s">
         <v>84</v>
       </c>
-      <c r="B193" s="206" t="s">
+      <c r="B193" s="210" t="s">
         <v>432</v>
       </c>
       <c r="C193" s="106"/>
@@ -33820,8 +33904,8 @@
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="209"/>
-      <c r="B194" s="210"/>
+      <c r="A194" s="213"/>
+      <c r="B194" s="214"/>
       <c r="C194" s="70" t="s">
         <v>245</v>
       </c>
@@ -33830,8 +33914,8 @@
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="209"/>
-      <c r="B195" s="210"/>
+      <c r="A195" s="213"/>
+      <c r="B195" s="214"/>
       <c r="C195" s="70">
         <v>10.1</v>
       </c>
@@ -33840,8 +33924,8 @@
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="209"/>
-      <c r="B196" s="210"/>
+      <c r="A196" s="213"/>
+      <c r="B196" s="214"/>
       <c r="C196" s="70">
         <v>10.199999999999999</v>
       </c>
@@ -33850,8 +33934,8 @@
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="209"/>
-      <c r="B197" s="210"/>
+      <c r="A197" s="213"/>
+      <c r="B197" s="214"/>
       <c r="C197" s="98" t="s">
         <v>288</v>
       </c>
@@ -33860,8 +33944,8 @@
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="209"/>
-      <c r="B198" s="210"/>
+      <c r="A198" s="213"/>
+      <c r="B198" s="214"/>
       <c r="C198" s="98" t="s">
         <v>370</v>
       </c>
@@ -33870,8 +33954,8 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="209"/>
-      <c r="B199" s="210"/>
+      <c r="A199" s="213"/>
+      <c r="B199" s="214"/>
       <c r="C199" s="98" t="s">
         <v>117</v>
       </c>
@@ -33880,8 +33964,8 @@
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="209"/>
-      <c r="B200" s="210"/>
+      <c r="A200" s="213"/>
+      <c r="B200" s="214"/>
       <c r="C200" s="98" t="s">
         <v>417</v>
       </c>
@@ -33890,8 +33974,8 @@
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A201" s="209"/>
-      <c r="B201" s="210"/>
+      <c r="A201" s="213"/>
+      <c r="B201" s="214"/>
       <c r="C201" s="98" t="s">
         <v>17</v>
       </c>
@@ -33900,20 +33984,20 @@
       </c>
     </row>
     <row r="202" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A202" s="211"/>
-      <c r="B202" s="207"/>
+      <c r="A202" s="215"/>
+      <c r="B202" s="211"/>
       <c r="C202" s="98" t="s">
         <v>460</v>
       </c>
-      <c r="D202" s="135" t="s">
+      <c r="D202" s="134" t="s">
         <v>459</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="208" t="s">
+      <c r="A203" s="212" t="s">
         <v>246</v>
       </c>
-      <c r="B203" s="206" t="s">
+      <c r="B203" s="210" t="s">
         <v>432</v>
       </c>
       <c r="C203" s="98"/>
@@ -33922,8 +34006,8 @@
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="209"/>
-      <c r="B204" s="210"/>
+      <c r="A204" s="213"/>
+      <c r="B204" s="214"/>
       <c r="C204" s="125" t="s">
         <v>428</v>
       </c>
@@ -33935,10 +34019,10 @@
       <c r="A205" s="109" t="s">
         <v>257</v>
       </c>
-      <c r="B205" s="70" t="s">
+      <c r="B205" s="152" t="s">
         <v>432</v>
       </c>
-      <c r="C205" s="134" t="s">
+      <c r="C205" s="133" t="s">
         <v>249</v>
       </c>
       <c r="D205" s="112" t="s">
@@ -33949,15 +34033,15 @@
       <c r="A206" s="127" t="s">
         <v>56</v>
       </c>
-      <c r="B206" s="127"/>
+      <c r="B206" s="156"/>
       <c r="C206" s="127"/>
       <c r="D206" s="127"/>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="208" t="s">
+      <c r="A207" s="212" t="s">
         <v>58</v>
       </c>
-      <c r="B207" s="206" t="s">
+      <c r="B207" s="210" t="s">
         <v>266</v>
       </c>
       <c r="C207" s="128" t="s">
@@ -33968,8 +34052,8 @@
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="209"/>
-      <c r="B208" s="210"/>
+      <c r="A208" s="213"/>
+      <c r="B208" s="214"/>
       <c r="C208" s="128" t="s">
         <v>260</v>
       </c>
@@ -33978,18 +34062,18 @@
       </c>
     </row>
     <row r="209" spans="1:4" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="211"/>
-      <c r="B209" s="207"/>
+      <c r="A209" s="215"/>
+      <c r="B209" s="211"/>
       <c r="C209" s="106"/>
       <c r="D209" s="106" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="210" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A210" s="219" t="s">
+      <c r="A210" s="223" t="s">
         <v>59</v>
       </c>
-      <c r="B210" s="206" t="s">
+      <c r="B210" s="210" t="s">
         <v>266</v>
       </c>
       <c r="C210" s="118" t="s">
@@ -34000,18 +34084,18 @@
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="220"/>
-      <c r="B211" s="207"/>
+      <c r="A211" s="224"/>
+      <c r="B211" s="211"/>
       <c r="C211" s="118"/>
       <c r="D211" s="106" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="212" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A212" s="219" t="s">
+      <c r="A212" s="223" t="s">
         <v>286</v>
       </c>
-      <c r="B212" s="206" t="s">
+      <c r="B212" s="210" t="s">
         <v>266</v>
       </c>
       <c r="C212" s="118"/>
@@ -34020,18 +34104,18 @@
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" s="220"/>
-      <c r="B213" s="207"/>
+      <c r="A213" s="224"/>
+      <c r="B213" s="211"/>
       <c r="C213" s="106"/>
       <c r="D213" s="106" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="214" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A214" s="219" t="s">
+      <c r="A214" s="223" t="s">
         <v>60</v>
       </c>
-      <c r="B214" s="206" t="s">
+      <c r="B214" s="210" t="s">
         <v>266</v>
       </c>
       <c r="C214" s="118" t="s">
@@ -34042,8 +34126,8 @@
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" s="220"/>
-      <c r="B215" s="207"/>
+      <c r="A215" s="224"/>
+      <c r="B215" s="211"/>
       <c r="C215" s="106"/>
       <c r="D215" s="106" t="s">
         <v>408</v>
@@ -34053,13 +34137,13 @@
       <c r="A216" s="127" t="s">
         <v>268</v>
       </c>
-      <c r="B216" s="127"/>
+      <c r="B216" s="156"/>
       <c r="C216" s="127"/>
       <c r="D216" s="127"/>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A217" s="106"/>
-      <c r="B217" s="70" t="s">
+      <c r="B217" s="152" t="s">
         <v>432</v>
       </c>
       <c r="C217" s="106" t="s">
@@ -34073,13 +34157,13 @@
       <c r="A218" s="127" t="s">
         <v>274</v>
       </c>
-      <c r="B218" s="127"/>
+      <c r="B218" s="156"/>
       <c r="C218" s="127"/>
       <c r="D218" s="127"/>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A219" s="106"/>
-      <c r="B219" s="70" t="s">
+      <c r="B219" s="152" t="s">
         <v>432</v>
       </c>
       <c r="C219" s="106" t="s">
@@ -34091,12 +34175,378 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A220" s="106"/>
-      <c r="B220" s="70"/>
+      <c r="B220" s="152"/>
       <c r="C220" s="106" t="s">
         <v>396</v>
       </c>
       <c r="D220" s="112" t="s">
         <v>397</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" s="103" t="s">
+        <v>497</v>
+      </c>
+      <c r="B221" s="155"/>
+      <c r="C221" s="103"/>
+      <c r="D221" s="104"/>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" s="58" t="s">
+        <v>498</v>
+      </c>
+      <c r="B222" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C222" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D222" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" s="58" t="s">
+        <v>499</v>
+      </c>
+      <c r="B223" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C223" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D223" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" s="58" t="s">
+        <v>500</v>
+      </c>
+      <c r="B224" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C224" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D224" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225" s="58" t="s">
+        <v>501</v>
+      </c>
+      <c r="B225" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C225" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D225" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" s="58" t="s">
+        <v>502</v>
+      </c>
+      <c r="B226" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C226" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D226" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" s="58" t="s">
+        <v>86</v>
+      </c>
+      <c r="B227" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C227" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D227" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="B228" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C228" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D228" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="B229" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C229" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D229" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="B230" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C230" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D230" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" s="58" t="s">
+        <v>165</v>
+      </c>
+      <c r="B231" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C231" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D231" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" s="58" t="s">
+        <v>503</v>
+      </c>
+      <c r="B232" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C232" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D232" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" s="58" t="s">
+        <v>504</v>
+      </c>
+      <c r="B233" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C233" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D233" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" s="58" t="s">
+        <v>505</v>
+      </c>
+      <c r="B234" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C234" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D234" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" s="58" t="s">
+        <v>506</v>
+      </c>
+      <c r="B235" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C235" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D235" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236" s="58" t="s">
+        <v>402</v>
+      </c>
+      <c r="B236" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C236" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D236" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A237" s="103" t="s">
+        <v>507</v>
+      </c>
+      <c r="B237" s="155"/>
+      <c r="C237" s="103"/>
+      <c r="D237" s="104"/>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A238" s="58" t="s">
+        <v>508</v>
+      </c>
+      <c r="B238" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C238" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D238" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A239" s="58" t="s">
+        <v>509</v>
+      </c>
+      <c r="B239" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C239" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D239" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240" s="58" t="s">
+        <v>510</v>
+      </c>
+      <c r="B240" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C240" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D240" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" s="58" t="s">
+        <v>511</v>
+      </c>
+      <c r="B241" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C241" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D241" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" s="58" t="s">
+        <v>512</v>
+      </c>
+      <c r="B242" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C242" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D242" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" s="58" t="s">
+        <v>513</v>
+      </c>
+      <c r="B243" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C243" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D243" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244" s="58" t="s">
+        <v>514</v>
+      </c>
+      <c r="B244" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C244" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D244" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245" s="58" t="s">
+        <v>515</v>
+      </c>
+      <c r="B245" s="148" t="s">
+        <v>432</v>
+      </c>
+      <c r="C245" s="58" t="s">
+        <v>30</v>
+      </c>
+      <c r="D245" s="58" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A246" s="58" t="s">
+        <v>516</v>
+      </c>
+      <c r="B246" s="154" t="s">
+        <v>432</v>
+      </c>
+      <c r="C246" s="58" t="s">
+        <v>517</v>
+      </c>
+      <c r="D246" s="58" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A247" s="58" t="s">
+        <v>516</v>
+      </c>
+      <c r="B247" s="154" t="s">
+        <v>432</v>
+      </c>
+      <c r="C247" s="58" t="s">
+        <v>519</v>
+      </c>
+      <c r="D247" s="58" t="s">
+        <v>520</v>
       </c>
     </row>
   </sheetData>

</xml_diff>